<commit_message>
New IO-Existing Member Scripts
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -5,19 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrown\TDECUWorkspace\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrown\IOExistingMember\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22425" windowHeight="7125" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22425" windowHeight="7125" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
-    <sheet name="ProdSelection" sheetId="4" r:id="rId2"/>
-    <sheet name="CCData" sheetId="5" r:id="rId3"/>
-    <sheet name="LoanData" sheetId="6" r:id="rId4"/>
-    <sheet name="Data" sheetId="2" r:id="rId5"/>
-    <sheet name="DNA_Upgrade" sheetId="3" r:id="rId6"/>
+    <sheet name="ProdData" sheetId="6" r:id="rId2"/>
+    <sheet name="Data" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="142">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -136,51 +133,6 @@
     <t>Term</t>
   </si>
   <si>
-    <t>C24213_VerifySingleCheckStopPayment</t>
-  </si>
-  <si>
-    <t>AccountNumber</t>
-  </si>
-  <si>
-    <t>Payee</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>CheckNumber</t>
-  </si>
-  <si>
-    <t>EndCheckNumber</t>
-  </si>
-  <si>
-    <t>PayeeName</t>
-  </si>
-  <si>
-    <t>Test Payee</t>
-  </si>
-  <si>
-    <t>2,3</t>
-  </si>
-  <si>
-    <t>Test Note</t>
-  </si>
-  <si>
-    <t>C24214_VerifyMultiCheckStopPayment_DNA</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>456789148</t>
-  </si>
-  <si>
-    <t>2364</t>
-  </si>
-  <si>
-    <t>2365</t>
-  </si>
-  <si>
     <t>C24105_VerifyCreditCardSelection</t>
   </si>
   <si>
@@ -196,12 +148,6 @@
     <t>Confirm-EM-0001</t>
   </si>
   <si>
-    <t>ProductHeader</t>
-  </si>
-  <si>
-    <t>ProductMessage</t>
-  </si>
-  <si>
     <t>Let’s get started!</t>
   </si>
   <si>
@@ -214,9 +160,6 @@
     <t>Credit Cards</t>
   </si>
   <si>
-    <t>Vehicle Loans and Refinance Options (Auto, Boat, Motorcycle, RV/ Camper)</t>
-  </si>
-  <si>
     <t>Personal Loans</t>
   </si>
   <si>
@@ -226,33 +169,6 @@
     <t>Additional Ways to Save</t>
   </si>
   <si>
-    <t>G2Section1</t>
-  </si>
-  <si>
-    <t>G2Section2</t>
-  </si>
-  <si>
-    <t>G1Section3</t>
-  </si>
-  <si>
-    <t>G1Section2</t>
-  </si>
-  <si>
-    <t>G1Section1</t>
-  </si>
-  <si>
-    <t>Group1</t>
-  </si>
-  <si>
-    <t>Group2</t>
-  </si>
-  <si>
-    <t>G2Section3</t>
-  </si>
-  <si>
-    <t>G2Section4</t>
-  </si>
-  <si>
     <t>Certificates of Deposit (CDs)</t>
   </si>
   <si>
@@ -268,54 +184,21 @@
     <t>C24104_VerifyProductExpandSections</t>
   </si>
   <si>
-    <t>ClassicMin</t>
-  </si>
-  <si>
     <t>Minimum credit limit of $500</t>
   </si>
   <si>
     <t>Minimum credit limit of $2,000</t>
   </si>
   <si>
-    <t>OtherMin</t>
-  </si>
-  <si>
-    <t>CCInfoMessage</t>
-  </si>
-  <si>
     <t>Please select the credit card product you would are requesting below:</t>
   </si>
   <si>
-    <t>ClassicName</t>
-  </si>
-  <si>
-    <t>BuceesName</t>
-  </si>
-  <si>
-    <t>PlatinumName</t>
-  </si>
-  <si>
-    <t>OnyxName</t>
-  </si>
-  <si>
-    <t>TypeLabel</t>
-  </si>
-  <si>
     <t>*Which credit card type?</t>
   </si>
   <si>
     <t>*Credit Limit Requested:</t>
   </si>
   <si>
-    <t>LimitLabel</t>
-  </si>
-  <si>
-    <t>ClassicLimit</t>
-  </si>
-  <si>
-    <t>OtherLimit</t>
-  </si>
-  <si>
     <t>Minimum $500.00</t>
   </si>
   <si>
@@ -337,36 +220,6 @@
     <t>C24106_VerifyVehicleLoanSelection</t>
   </si>
   <si>
-    <t>AutoLoanTitle</t>
-  </si>
-  <si>
-    <t>RefAutoTtile</t>
-  </si>
-  <si>
-    <t>CycleTitle</t>
-  </si>
-  <si>
-    <t>RefCycleTitle</t>
-  </si>
-  <si>
-    <t>BoatTitle</t>
-  </si>
-  <si>
-    <t>RefBoatTitle</t>
-  </si>
-  <si>
-    <t>RVTitle</t>
-  </si>
-  <si>
-    <t>RefRVTitle</t>
-  </si>
-  <si>
-    <t>JetSkiTitle</t>
-  </si>
-  <si>
-    <t>ATVTitle</t>
-  </si>
-  <si>
     <t>Auto Loan (New or Used)</t>
   </si>
   <si>
@@ -397,17 +250,215 @@
     <t>ATV/UTV Loans (New or Used)</t>
   </si>
   <si>
-    <t>Check out the latest rates here</t>
-  </si>
-  <si>
-    <t>Rates</t>
+    <t>Minimum $1,000.00</t>
+  </si>
+  <si>
+    <t>Minimum $5,000.00</t>
+  </si>
+  <si>
+    <t>Includes Jet Ski®</t>
+  </si>
+  <si>
+    <t>Check out the latest rates</t>
+  </si>
+  <si>
+    <t>C24107_VerifyPersonalLoanSelection</t>
+  </si>
+  <si>
+    <t>My Way Loan: $4,000</t>
+  </si>
+  <si>
+    <t>My Way Loan: $6,000</t>
+  </si>
+  <si>
+    <t>My Way Loan: $7,000</t>
+  </si>
+  <si>
+    <t>Personal Loan</t>
+  </si>
+  <si>
+    <t>Home Advantage Personal Loan</t>
+  </si>
+  <si>
+    <t>Cash $tash™ Line of Credit</t>
+  </si>
+  <si>
+    <t>Certificate of Deposit Secured Loan</t>
+  </si>
+  <si>
+    <t>Share Secured Loan</t>
+  </si>
+  <si>
+    <t>month term</t>
+  </si>
+  <si>
+    <t>8.99% APR3</t>
+  </si>
+  <si>
+    <t>No collateral required</t>
+  </si>
+  <si>
+    <t>ProdTitle1</t>
+  </si>
+  <si>
+    <t>ProdTitle2</t>
+  </si>
+  <si>
+    <t>ProdTitle3</t>
+  </si>
+  <si>
+    <t>ProdTitle4</t>
+  </si>
+  <si>
+    <t>ProdTitle5</t>
+  </si>
+  <si>
+    <t>ProdTitle6</t>
+  </si>
+  <si>
+    <t>ProdTitle7</t>
+  </si>
+  <si>
+    <t>ProdTitle8</t>
+  </si>
+  <si>
+    <t>ProdTitle9</t>
+  </si>
+  <si>
+    <t>ProdTitle10</t>
+  </si>
+  <si>
+    <t>ProdDesc1</t>
+  </si>
+  <si>
+    <t>ProdDesc2</t>
+  </si>
+  <si>
+    <t>ProdDesc3</t>
+  </si>
+  <si>
+    <t>ProdMin1</t>
+  </si>
+  <si>
+    <t>ProdMin2</t>
+  </si>
+  <si>
+    <t>ProdMin3</t>
+  </si>
+  <si>
+    <t>ProdMin4</t>
+  </si>
+  <si>
+    <t>ProdMin5</t>
+  </si>
+  <si>
+    <t>ProdDesc4</t>
+  </si>
+  <si>
+    <t>ProdDesc5</t>
+  </si>
+  <si>
+    <t>ProdText1</t>
+  </si>
+  <si>
+    <t>ProdText2</t>
+  </si>
+  <si>
+    <t>ProdText3</t>
+  </si>
+  <si>
+    <t>Minimum $4,000.00</t>
+  </si>
+  <si>
+    <t>Minimum $6,000.00</t>
+  </si>
+  <si>
+    <t>Minimum $7,000.00</t>
+  </si>
+  <si>
+    <t>Minimum loan amount of $1,000</t>
+  </si>
+  <si>
+    <t>ProdDesc6</t>
+  </si>
+  <si>
+    <t>ProdDesc7</t>
+  </si>
+  <si>
+    <t>Cash $tash&amp;trade; Line of Credit</t>
+  </si>
+  <si>
+    <t>Borrow 100% of your current share savings account balance</t>
+  </si>
+  <si>
+    <t>Terms as long as 10 years</t>
+  </si>
+  <si>
+    <t>A safe, fixed-term investment with great rates</t>
+  </si>
+  <si>
+    <t>$1,000 minimum deposit required</t>
+  </si>
+  <si>
+    <t>Search for a CD</t>
+  </si>
+  <si>
+    <t>Complete the fields below to find a CD that fits your needs!</t>
+  </si>
+  <si>
+    <t>C24108_VerifyCDSelection</t>
+  </si>
+  <si>
+    <t>C24109_VerifyCheckingMMSelection</t>
+  </si>
+  <si>
+    <t>Classic Checking</t>
+  </si>
+  <si>
+    <t>Money Market</t>
+  </si>
+  <si>
+    <t>High Yield Checking</t>
+  </si>
+  <si>
+    <t>No monthly fee</t>
+  </si>
+  <si>
+    <t>No minimum balance requirement</t>
+  </si>
+  <si>
+    <t>High-yield investment account with a competitive rate</t>
+  </si>
+  <si>
+    <t>$2,500 minimum deposit required</t>
+  </si>
+  <si>
+    <t>Minimum balance must be maintained to avoid $10 monthly service charge</t>
+  </si>
+  <si>
+    <t>Vehicle Loans and Refinance Options</t>
+  </si>
+  <si>
+    <t>(Auto, Boat, Motorcycle, RV/ Camper)</t>
+  </si>
+  <si>
+    <t>Overdraft Protection Plan</t>
+  </si>
+  <si>
+    <t>Our Overdraft Protection Plan is the service on your checking account which allows funds to be pulled from the savings account in the event funds are not available and an overdraft occurs. This feature is used before Courtesy Pay and subject to Regulation D limitations.</t>
+  </si>
+  <si>
+    <t>Opt into Courtesy Pay</t>
+  </si>
+  <si>
+    <t>Courtesy Pay overdraft protection allows TDECU to overdraw your checking account in order to pay a transaction up to a predetermined limit. Our standard overdraft practice covers checks and other transactions using your account number as well as automatic bill payments that may overdraw your account. However, we will not authorize and pay overdrafts for ATM transactions or one-time debit card transactions unless you opt-in by clicking the provided box. We pay overdrafts at our discretion, which means we do not guarantee we will always authorize and pay any type of transaction. If we do not authorize and pay an overdraft, your transaction will be declined.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,13 +478,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -460,7 +504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -471,7 +515,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -790,7 +835,7 @@
   <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
+      <selection activeCell="B8" sqref="B8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +870,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
@@ -840,7 +885,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -855,7 +900,7 @@
     </row>
     <row r="4" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
@@ -870,7 +915,7 @@
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
@@ -884,22 +929,49 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="1"/>
     </row>
@@ -1275,231 +1347,22 @@
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B3" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K2" t="s">
-        <v>95</v>
-      </c>
-      <c r="L2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L2" sqref="L2"/>
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,82 +1377,358 @@
     <col min="8" max="8" width="21.5703125" customWidth="1"/>
     <col min="9" max="9" width="26.85546875" customWidth="1"/>
     <col min="10" max="11" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="9.140625" style="6"/>
+    <col min="17" max="17" width="22.7109375" customWidth="1"/>
+    <col min="18" max="18" width="22.7109375" style="6" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" customWidth="1"/>
+    <col min="22" max="22" width="18.42578125" style="6" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="V1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>77</v>
+      </c>
+      <c r="R5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" t="s">
+        <v>119</v>
+      </c>
+      <c r="L6" t="s">
+        <v>113</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>87</v>
+      </c>
+      <c r="R6" t="s">
+        <v>89</v>
+      </c>
+      <c r="S6" t="s">
+        <v>88</v>
+      </c>
+      <c r="T6" t="s">
+        <v>116</v>
+      </c>
+      <c r="U6" t="s">
+        <v>77</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="L7">
+        <v>500</v>
+      </c>
+      <c r="M7" s="9">
+        <v>1000</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>122</v>
+      </c>
+      <c r="R7" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J2" t="s">
-        <v>120</v>
-      </c>
-      <c r="K2" t="s">
-        <v>121</v>
-      </c>
-      <c r="L2" t="s">
-        <v>122</v>
+      <c r="X7" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>131</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="T8" t="s">
+        <v>134</v>
+      </c>
+      <c r="U8" t="s">
+        <v>135</v>
+      </c>
+      <c r="X8" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1598,7 +1737,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W30"/>
   <sheetViews>
@@ -1699,14 +1838,14 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="6" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="G2" s="2">
         <v>98826</v>
@@ -1721,7 +1860,7 @@
         <v>31</v>
       </c>
       <c r="K2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="L2" s="7">
         <v>42005</v>
@@ -1873,82 +2012,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
IO Existing Member added/updated scripts
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrown\IOExistingMember\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrown\TDECUWorkspace\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="215">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -64,15 +64,9 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>SuffixName</t>
-  </si>
-  <si>
     <t>StreetAddress</t>
   </si>
   <si>
-    <t>ZipCode</t>
-  </si>
-  <si>
     <t>SSN</t>
   </si>
   <si>
@@ -88,51 +82,12 @@
     <t>IssueDate</t>
   </si>
   <si>
-    <t>ExpiryDate</t>
-  </si>
-  <si>
-    <t>MotherName</t>
-  </si>
-  <si>
-    <t>CurrentEmployer</t>
-  </si>
-  <si>
-    <t>Occupation</t>
-  </si>
-  <si>
-    <t>PhoneNumber</t>
-  </si>
-  <si>
-    <t>PhoneType</t>
-  </si>
-  <si>
-    <t>PrimaryEmail</t>
-  </si>
-  <si>
-    <t>8008391154</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>HowDidYouHear</t>
-  </si>
-  <si>
-    <t>Internet</t>
-  </si>
-  <si>
     <t>Photo Non-Drivers License</t>
   </si>
   <si>
     <t>MemberNumber</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Term</t>
-  </si>
-  <si>
     <t>C24105_VerifyCreditCardSelection</t>
   </si>
   <si>
@@ -145,9 +100,6 @@
     <t>27897 Napeequa Dr</t>
   </si>
   <si>
-    <t>Confirm-EM-0001</t>
-  </si>
-  <si>
     <t>Let’s get started!</t>
   </si>
   <si>
@@ -313,21 +265,6 @@
     <t>ProdTitle5</t>
   </si>
   <si>
-    <t>ProdTitle6</t>
-  </si>
-  <si>
-    <t>ProdTitle7</t>
-  </si>
-  <si>
-    <t>ProdTitle8</t>
-  </si>
-  <si>
-    <t>ProdTitle9</t>
-  </si>
-  <si>
-    <t>ProdTitle10</t>
-  </si>
-  <si>
     <t>ProdDesc1</t>
   </si>
   <si>
@@ -452,6 +389,288 @@
   </si>
   <si>
     <t>Courtesy Pay overdraft protection allows TDECU to overdraw your checking account in order to pay a transaction up to a predetermined limit. Our standard overdraft practice covers checks and other transactions using your account number as well as automatic bill payments that may overdraw your account. However, we will not authorize and pay overdrafts for ATM transactions or one-time debit card transactions unless you opt-in by clicking the provided box. We pay overdrafts at our discretion, which means we do not guarantee we will always authorize and pay any type of transaction. If we do not authorize and pay an overdraft, your transaction will be declined.</t>
+  </si>
+  <si>
+    <t>ProdField1</t>
+  </si>
+  <si>
+    <t>ProdField2</t>
+  </si>
+  <si>
+    <t>ProdField3</t>
+  </si>
+  <si>
+    <t>ProdField4</t>
+  </si>
+  <si>
+    <t>NameSuffix</t>
+  </si>
+  <si>
+    <t>CityStateZip</t>
+  </si>
+  <si>
+    <t>ExpDate</t>
+  </si>
+  <si>
+    <t>HouseType</t>
+  </si>
+  <si>
+    <t>HousePaymt</t>
+  </si>
+  <si>
+    <t>HouseYr</t>
+  </si>
+  <si>
+    <t>HouseMon</t>
+  </si>
+  <si>
+    <t>EmpStatus</t>
+  </si>
+  <si>
+    <t>CurrEmp</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>EmpYr</t>
+  </si>
+  <si>
+    <t>EmpMon</t>
+  </si>
+  <si>
+    <t>ProdField5</t>
+  </si>
+  <si>
+    <t>ProdField6</t>
+  </si>
+  <si>
+    <t>ProdField7</t>
+  </si>
+  <si>
+    <t>ErrorMsg1</t>
+  </si>
+  <si>
+    <t>ErrorMsg2</t>
+  </si>
+  <si>
+    <t>ProdInfo6</t>
+  </si>
+  <si>
+    <t>ProdInfo7</t>
+  </si>
+  <si>
+    <t>ProdInfo8</t>
+  </si>
+  <si>
+    <t>ProdInfo9</t>
+  </si>
+  <si>
+    <t>ProdInfo10</t>
+  </si>
+  <si>
+    <t>ProdText4</t>
+  </si>
+  <si>
+    <t>OtherTxt1</t>
+  </si>
+  <si>
+    <t>OtherTxt2</t>
+  </si>
+  <si>
+    <t>OtherTxt3</t>
+  </si>
+  <si>
+    <t>OtherTxt4</t>
+  </si>
+  <si>
+    <t>OtherTxt5</t>
+  </si>
+  <si>
+    <t>OtherTxt6</t>
+  </si>
+  <si>
+    <t>OtherTxt7</t>
+  </si>
+  <si>
+    <t>OtherTxt8</t>
+  </si>
+  <si>
+    <t>OtherTxt9</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Continue</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>01012010</t>
+  </si>
+  <si>
+    <t>01012025</t>
+  </si>
+  <si>
+    <t>1700</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>University of Washington</t>
+  </si>
+  <si>
+    <t>Save 10¢ per gallon when you buy fuel at participating Buc-ee’s locations</t>
+  </si>
+  <si>
+    <t>No annual fee</t>
+  </si>
+  <si>
+    <t>0% Introductory APR</t>
+  </si>
+  <si>
+    <t>Up to 2% annual rebate on your first $500,000 in net purchases</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>8229386</t>
+  </si>
+  <si>
+    <t>456127890</t>
+  </si>
+  <si>
+    <t>01011980</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Onyx MasterCard ®</t>
+  </si>
+  <si>
+    <t>67890</t>
+  </si>
+  <si>
+    <t>02062010</t>
+  </si>
+  <si>
+    <t>02062025</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Software Testing Co</t>
+  </si>
+  <si>
+    <t>6000</t>
+  </si>
+  <si>
+    <t>8229319</t>
+  </si>
+  <si>
+    <t>023465789</t>
+  </si>
+  <si>
+    <t>02061980</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Club Account</t>
+  </si>
+  <si>
+    <t>Buc-ee's MasterCard ®</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>$500.00</t>
+  </si>
+  <si>
+    <t>Please enter an amount for 12 Month Share Certificate between $1,000.00 and $100,000.00</t>
+  </si>
+  <si>
+    <t>C24110_VerifySavingsSelection</t>
+  </si>
+  <si>
+    <t>Additional savings account available to all Members</t>
+  </si>
+  <si>
+    <t>C24111_VerifyProdSelectButtons</t>
+  </si>
+  <si>
+    <t>C24251_VerifyAddServiceSelection</t>
+  </si>
+  <si>
+    <t>E-Documents</t>
+  </si>
+  <si>
+    <t>E-Documents provide you with secure online access to your account statement and other important documents.</t>
+  </si>
+  <si>
+    <t>C24256_VerifyCheckingAccountsOrder</t>
+  </si>
+  <si>
+    <t>C24260_VerifyBackButton</t>
+  </si>
+  <si>
+    <t>C24309_VerifyMoneyMarketSelection</t>
+  </si>
+  <si>
+    <t>Please select a funding method.</t>
+  </si>
+  <si>
+    <t>C24314_VerifyCheckingAccountSelection1</t>
+  </si>
+  <si>
+    <t>Please enter an amount for Classic Checking between $1.00 and $2,500.00</t>
+  </si>
+  <si>
+    <t>Please enter an amount for High Yield Checking between $0.00 and $2,500.00</t>
+  </si>
+  <si>
+    <t>C24314_VerifyCheckingAccountSelection2</t>
+  </si>
+  <si>
+    <t>Online/Mobile Banking</t>
+  </si>
+  <si>
+    <t>12 Month Share Certificate (Estimated Maturity Date:</t>
+  </si>
+  <si>
+    <t>24 Month Share Certificate (Estimated Maturity Date:</t>
   </si>
 </sst>
 </file>
@@ -504,7 +723,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -517,6 +736,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -870,7 +1092,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
@@ -885,7 +1107,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -900,7 +1122,7 @@
     </row>
     <row r="4" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
@@ -915,7 +1137,7 @@
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
@@ -930,7 +1152,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>8</v>
@@ -945,7 +1167,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
@@ -961,7 +1183,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>8</v>
@@ -1358,377 +1580,877 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:AM16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y8" sqref="Y8"/>
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
-    <col min="10" max="11" width="22.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24" style="6" customWidth="1"/>
+    <col min="6" max="6" width="24" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" style="6" customWidth="1"/>
+    <col min="10" max="11" width="22.140625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="6"/>
+    <col min="13" max="13" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="9.140625" style="6"/>
-    <col min="17" max="17" width="22.7109375" customWidth="1"/>
-    <col min="18" max="18" width="22.7109375" style="6" customWidth="1"/>
+    <col min="17" max="18" width="22.7109375" style="6" customWidth="1"/>
     <col min="19" max="19" width="11.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5703125" customWidth="1"/>
-    <col min="21" max="21" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" style="6" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" style="6" customWidth="1"/>
     <col min="22" max="22" width="18.42578125" style="6" customWidth="1"/>
     <col min="23" max="23" width="14.140625" style="6" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="8">
+        <v>2000</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="V4" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB4" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC4" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD4" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE4" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF4" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="AG4" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="AH4" s="8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="6">
+        <v>5000</v>
+      </c>
+      <c r="O5" s="6">
+        <v>6000</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="X5" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y5" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z5" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA5" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB5" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC5" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="AD5" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="AE5" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="AF5" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG5" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="M6" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="N6" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="O6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="T6" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="U6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="V6" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="W6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="X6" s="6">
+        <v>2000</v>
+      </c>
+      <c r="Y6" s="6">
+        <v>6000</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA6" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB6" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC6" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD6" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE6" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF6" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="AG6" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="AH6" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="AI6" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="AJ6" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="AK6" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="AL6" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AM6" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="B7" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="J7" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J5" t="s">
-        <v>72</v>
-      </c>
-      <c r="K5" t="s">
-        <v>73</v>
-      </c>
-      <c r="L5" t="s">
-        <v>74</v>
-      </c>
-      <c r="M5" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>77</v>
-      </c>
-      <c r="R5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H6" t="s">
-        <v>85</v>
-      </c>
-      <c r="I6" t="s">
-        <v>86</v>
-      </c>
-      <c r="J6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L6" t="s">
-        <v>113</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>87</v>
-      </c>
-      <c r="R6" t="s">
-        <v>89</v>
-      </c>
-      <c r="S6" t="s">
-        <v>88</v>
-      </c>
-      <c r="T6" t="s">
-        <v>116</v>
-      </c>
-      <c r="U6" t="s">
-        <v>77</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="W6" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="L7">
+      <c r="K7" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="L7" s="6">
         <v>500</v>
       </c>
       <c r="M7" s="9">
         <v>1000</v>
       </c>
-      <c r="Q7" t="s">
-        <v>122</v>
+      <c r="N7" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="O7" s="6">
+        <v>5000</v>
+      </c>
+      <c r="P7" s="6">
+        <v>12000</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="X7" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8" t="s">
-        <v>138</v>
-      </c>
-      <c r="F8" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>131</v>
+        <v>102</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="U7" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="V7" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="W7" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC7" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="AD7" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="AE7" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF7" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="AG7" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="AH7" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="AI7" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="AJ7" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="AK7" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="T8" t="s">
-        <v>134</v>
-      </c>
-      <c r="U8" t="s">
-        <v>135</v>
-      </c>
-      <c r="X8" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>141</v>
+        <v>112</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="U8" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="X8" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y8" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="L13" s="6">
+        <v>2000</v>
+      </c>
+      <c r="M13" s="6">
+        <v>5000</v>
+      </c>
+      <c r="N13" s="6">
+        <v>10000</v>
+      </c>
+      <c r="O13" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="L14" s="6">
+        <v>1000</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="S14" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="T14" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="U14" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="V14" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="W14" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="X14" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y14" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA14" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB14" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC14" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD14" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE14" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB15" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC15" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="AD15" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="AE15" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="AF15" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="L16" s="6">
+        <v>5000</v>
+      </c>
+      <c r="M16" s="6">
+        <v>6000</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="T16" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="U16" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="V16" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="W16" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="X16" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y16" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z16" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA16" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB16" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC16" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD16" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE16" s="6" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -1739,11 +2461,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W30"/>
+  <dimension ref="A1:AF30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X1" sqref="X1"/>
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G2" sqref="G2:AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,128 +2487,129 @@
     <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="N1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="R1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="2">
-        <v>98826</v>
-      </c>
-      <c r="H2" s="2">
-        <v>456127890</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1011980</v>
-      </c>
-      <c r="J2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="7">
-        <v>42005</v>
-      </c>
-      <c r="M2" s="7">
-        <v>45658</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" t="s">
-        <v>30</v>
-      </c>
-      <c r="U2" s="2">
-        <v>8229386</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="Q2" s="2"/>
+      <c r="U2" s="2"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1894,7 +2617,7 @@
       <c r="I4" s="2"/>
       <c r="U4" s="2"/>
     </row>
-    <row r="5" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1904,7 +2627,7 @@
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1913,39 +2636,39 @@
       <c r="I6" s="2"/>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>

</xml_diff>

<commit_message>
IO-Existing Member updated/added scripts
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="264">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -454,21 +454,6 @@
     <t>ErrorMsg2</t>
   </si>
   <si>
-    <t>ProdInfo6</t>
-  </si>
-  <si>
-    <t>ProdInfo7</t>
-  </si>
-  <si>
-    <t>ProdInfo8</t>
-  </si>
-  <si>
-    <t>ProdInfo9</t>
-  </si>
-  <si>
-    <t>ProdInfo10</t>
-  </si>
-  <si>
     <t>ProdText4</t>
   </si>
   <si>
@@ -499,12 +484,6 @@
     <t>OtherTxt9</t>
   </si>
   <si>
-    <t>Back</t>
-  </si>
-  <si>
-    <t>Continue</t>
-  </si>
-  <si>
     <t>12345</t>
   </si>
   <si>
@@ -671,6 +650,174 @@
   </si>
   <si>
     <t>24 Month Share Certificate (Estimated Maturity Date:</t>
+  </si>
+  <si>
+    <t>C24150_VerifyCreditCardInfo</t>
+  </si>
+  <si>
+    <t>$1,500.00</t>
+  </si>
+  <si>
+    <t>C24153_VerifyCreditCardLimit</t>
+  </si>
+  <si>
+    <t>ProdInfo1</t>
+  </si>
+  <si>
+    <t>ProdInfo2</t>
+  </si>
+  <si>
+    <t>ProdInfo3</t>
+  </si>
+  <si>
+    <t>ProdInfo4</t>
+  </si>
+  <si>
+    <t>ProdInfo5</t>
+  </si>
+  <si>
+    <t>Please enter a value between $500 and $1,999</t>
+  </si>
+  <si>
+    <t>Please enter a value between $2,000 and $100,000</t>
+  </si>
+  <si>
+    <t>C24154_VerifyCCMinMax</t>
+  </si>
+  <si>
+    <t>Please enter an Amount.</t>
+  </si>
+  <si>
+    <t>$99,999.00</t>
+  </si>
+  <si>
+    <t>C24155_VerifyVehicleLoanInfo</t>
+  </si>
+  <si>
+    <t>Please provide information for the vehicle loan that you are requesting below:</t>
+  </si>
+  <si>
+    <t>*Which type of Vehicle Loan are you requesting?</t>
+  </si>
+  <si>
+    <t>*What loan amount are you requesting?</t>
+  </si>
+  <si>
+    <t>*What was the Purchase Price of the vehicle?</t>
+  </si>
+  <si>
+    <t>Make:</t>
+  </si>
+  <si>
+    <t>Model:</t>
+  </si>
+  <si>
+    <t>Year:</t>
+  </si>
+  <si>
+    <t>Mileage:</t>
+  </si>
+  <si>
+    <t>What is the Vehicle Identification Number (VIN)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Back </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Continue </t>
+  </si>
+  <si>
+    <t>Please enter a value between $1,000 and $100,000</t>
+  </si>
+  <si>
+    <t>$10,550.00</t>
+  </si>
+  <si>
+    <t>$21,568.00</t>
+  </si>
+  <si>
+    <t>Harley Davidson</t>
+  </si>
+  <si>
+    <t>Fat Boy</t>
+  </si>
+  <si>
+    <t>6546df54sdfwef41</t>
+  </si>
+  <si>
+    <t>7256</t>
+  </si>
+  <si>
+    <t>$700.00</t>
+  </si>
+  <si>
+    <t>$2,500.00</t>
+  </si>
+  <si>
+    <t>C24156_VerifyVehicleLoanLimit</t>
+  </si>
+  <si>
+    <t>$6,500.00</t>
+  </si>
+  <si>
+    <t>$12,222.00</t>
+  </si>
+  <si>
+    <t>C24157_VerifyVehicleLoanMinMax</t>
+  </si>
+  <si>
+    <t>Please enter a value between $1,000 and $150,000</t>
+  </si>
+  <si>
+    <t>$6,789.00</t>
+  </si>
+  <si>
+    <t>Please enter a value between $5,000 and $100,000</t>
+  </si>
+  <si>
+    <t>Please enter a value between $1,000 and $125,000</t>
+  </si>
+  <si>
+    <t>Please enter a value between $5,000 and $150,000</t>
+  </si>
+  <si>
+    <t>Please enter a value between $1,000 and $1,000,000</t>
+  </si>
+  <si>
+    <t>C24313_VerifyCheckingOptions</t>
+  </si>
+  <si>
+    <t>Debit Card</t>
+  </si>
+  <si>
+    <t>Courtesty Pay Opt-In</t>
+  </si>
+  <si>
+    <t>C24257_VerifyFreedomLoanNotDisplayed</t>
+  </si>
+  <si>
+    <t>Freedom</t>
+  </si>
+  <si>
+    <t>C24158_VerifyVehicleLoanReqFields</t>
+  </si>
+  <si>
+    <t>Please select a product type.</t>
+  </si>
+  <si>
+    <t>Please select an item from the drop down list.</t>
+  </si>
+  <si>
+    <t>Please enter a vehicle VIN</t>
+  </si>
+  <si>
+    <t>lksdjf9092kf0d</t>
+  </si>
+  <si>
+    <t>C24158_VerifyVehicleLoanReqFields2</t>
+  </si>
+  <si>
+    <t>C24176_VerifyValidVehicleInfo</t>
   </si>
 </sst>
 </file>
@@ -1054,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B27" sqref="B27:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,7 +1346,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
@@ -1214,7 +1361,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>8</v>
@@ -1228,7 +1375,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>8</v>
@@ -1242,7 +1389,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>8</v>
@@ -1255,9 +1402,9 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>205</v>
+        <v>255</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>8</v>
@@ -1272,7 +1419,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>8</v>
@@ -1285,9 +1432,9 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>208</v>
+        <v>252</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>8</v>
@@ -1302,7 +1449,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>8</v>
@@ -1315,67 +1462,188 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>208</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>218</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>221</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>245</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>257</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>263</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="F32" s="1"/>
     </row>
@@ -1509,20 +1777,20 @@
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="4"/>
-      <c r="E65" s="2"/>
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="4"/>
-      <c r="E66" s="2"/>
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="4"/>
+      <c r="E67" s="2"/>
       <c r="F67" s="1"/>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="4"/>
+      <c r="E68" s="2"/>
       <c r="F68" s="1"/>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
@@ -1531,20 +1799,20 @@
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="4"/>
-      <c r="E70" s="2"/>
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
-      <c r="E71" s="2"/>
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
+      <c r="E72" s="2"/>
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
+      <c r="E73" s="2"/>
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
@@ -1557,12 +1825,10 @@
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
-      <c r="E76" s="2"/>
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
-      <c r="E77" s="2"/>
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
@@ -1572,10 +1838,12 @@
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="4"/>
+      <c r="E79" s="2"/>
       <c r="F79" s="1"/>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" s="4"/>
+      <c r="E80" s="2"/>
       <c r="F80" s="1"/>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
@@ -1592,12 +1860,10 @@
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" s="4"/>
-      <c r="E84" s="2"/>
       <c r="F84" s="1"/>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="4"/>
-      <c r="E85" s="2"/>
       <c r="F85" s="1"/>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
@@ -1622,10 +1888,12 @@
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" s="4"/>
+      <c r="E90" s="2"/>
       <c r="F90" s="1"/>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91" s="4"/>
+      <c r="E91" s="2"/>
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.25">
@@ -1651,6 +1919,14 @@
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="4"/>
       <c r="F97" s="1"/>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B98" s="4"/>
+      <c r="F98" s="1"/>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B99" s="4"/>
+      <c r="F99" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1665,23 +1941,34 @@
     <hyperlink ref="B10" r:id="rId9"/>
     <hyperlink ref="B11" r:id="rId10"/>
     <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
+    <hyperlink ref="B14" r:id="rId12"/>
+    <hyperlink ref="B16" r:id="rId13"/>
+    <hyperlink ref="B17" r:id="rId14"/>
+    <hyperlink ref="B18" r:id="rId15"/>
+    <hyperlink ref="B19" r:id="rId16"/>
+    <hyperlink ref="B20" r:id="rId17"/>
+    <hyperlink ref="B21" r:id="rId18"/>
+    <hyperlink ref="B22" r:id="rId19"/>
+    <hyperlink ref="B23" r:id="rId20"/>
+    <hyperlink ref="B24" r:id="rId21"/>
+    <hyperlink ref="B15" r:id="rId22"/>
+    <hyperlink ref="B13" r:id="rId23"/>
+    <hyperlink ref="B25" r:id="rId24"/>
+    <hyperlink ref="B26" r:id="rId25"/>
+    <hyperlink ref="B27" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM16"/>
+  <dimension ref="A1:AM27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9:A16"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,7 +1983,7 @@
     <col min="8" max="8" width="21.5703125" style="6" customWidth="1"/>
     <col min="9" max="9" width="26.85546875" style="6" customWidth="1"/>
     <col min="10" max="11" width="22.140625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="6"/>
+    <col min="12" max="12" width="13.42578125" style="6" customWidth="1"/>
     <col min="13" max="13" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="9.140625" style="6"/>
     <col min="17" max="18" width="22.7109375" style="6" customWidth="1"/>
@@ -1728,19 +2015,19 @@
         <v>78</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>142</v>
+        <v>211</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>143</v>
+        <v>212</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>144</v>
+        <v>213</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>145</v>
+        <v>214</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>146</v>
+        <v>215</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>82</v>
@@ -1788,7 +2075,7 @@
         <v>91</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="AB1" s="3" t="s">
         <v>19</v>
@@ -1800,31 +2087,31 @@
         <v>14</v>
       </c>
       <c r="AE1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1862,10 +2149,10 @@
         <v>34</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>157</v>
+        <v>231</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>158</v>
+        <v>232</v>
       </c>
       <c r="X2" s="6" t="s">
         <v>24</v>
@@ -1899,19 +2186,19 @@
         <v>18</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>41</v>
@@ -1923,13 +2210,13 @@
         <v>2000</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="R4" s="6" t="s">
         <v>36</v>
@@ -1938,13 +2225,13 @@
         <v>37</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="X4" s="6" t="s">
         <v>38</v>
@@ -1956,28 +2243,28 @@
         <v>40</v>
       </c>
       <c r="AA4" s="11" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AB4" s="12" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="AC4" s="12" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="AD4" s="12" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="AG4" s="8" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="AH4" s="8" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
@@ -2036,46 +2323,46 @@
         <v>18</v>
       </c>
       <c r="T5" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="X5" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y5" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z5" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA5" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB5" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="U5" s="11" t="s">
+      <c r="AC5" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="V5" s="11" t="s">
+      <c r="AD5" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="W5" s="11" t="s">
+      <c r="AE5" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF5" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="X5" s="11" t="s">
+      <c r="AG5" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="Y5" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="Z5" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA5" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="AB5" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="AC5" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="AD5" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="AE5" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="AF5" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="AG5" s="11" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
@@ -2110,7 +2397,7 @@
         <v>98</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>92</v>
@@ -2158,43 +2445,43 @@
         <v>18</v>
       </c>
       <c r="AA6" s="11" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="AB6" s="12" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="AC6" s="12" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="AD6" s="12" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="AE6" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="AF6" s="11" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="AG6" s="11" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="AH6" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="AI6" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="AJ6" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="AK6" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI6" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="AJ6" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="AK6" s="11" t="s">
-        <v>170</v>
-      </c>
       <c r="AL6" s="11" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="AM6" s="11" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
@@ -2202,31 +2489,31 @@
         <v>105</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>48</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="L7" s="6">
         <v>500</v>
@@ -2235,7 +2522,7 @@
         <v>1000</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="O7" s="6">
         <v>5000</v>
@@ -2253,16 +2540,16 @@
         <v>18</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="W7" s="11" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="X7" s="6" t="s">
         <v>103</v>
@@ -2271,34 +2558,34 @@
         <v>104</v>
       </c>
       <c r="AB7" s="12" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="AC7" s="12" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="AD7" s="12" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="AE7" s="11" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="AF7" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="AG7" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="AG7" s="11" t="s">
-        <v>182</v>
-      </c>
       <c r="AH7" s="11" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="AI7" s="11" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="AJ7" s="11" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="AK7" s="11" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
@@ -2344,34 +2631,34 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>109</v>
@@ -2385,169 +2672,530 @@
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="L13" s="6">
-        <v>2000</v>
-      </c>
-      <c r="M13" s="6">
-        <v>5000</v>
-      </c>
-      <c r="N13" s="6">
-        <v>10000</v>
-      </c>
-      <c r="O13" s="6">
-        <v>500</v>
+        <v>255</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>108</v>
+        <v>198</v>
       </c>
       <c r="L14" s="6">
-        <v>1000</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="R14" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="S14" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="T14" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="U14" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="V14" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="W14" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="X14" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="Y14" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="Z14" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA14" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="AB14" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="AC14" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="AD14" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="AE14" s="11" t="s">
-        <v>207</v>
+        <v>2000</v>
+      </c>
+      <c r="M14" s="6">
+        <v>5000</v>
+      </c>
+      <c r="N14" s="6">
+        <v>10000</v>
+      </c>
+      <c r="O14" s="6">
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AB15" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="AC15" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="AD15" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="AE15" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="AF15" s="6" t="s">
-        <v>210</v>
+        <v>252</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>54</v>
+        <v>199</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="L16" s="6">
-        <v>5000</v>
-      </c>
-      <c r="M16" s="6">
-        <v>6000</v>
+        <v>1000</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>18</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="T16" s="11" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="U16" s="11" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="V16" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="W16" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="X16" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y16" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="W16" s="11" t="s">
+      <c r="Z16" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="AA16" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB16" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="X16" s="11" t="s">
+      <c r="AC16" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="Y16" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="Z16" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA16" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="AB16" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="AC16" s="12" t="s">
-        <v>172</v>
-      </c>
       <c r="AD16" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="AE16" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="AE16" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB17" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="AC17" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="AD17" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="AE17" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="AF17" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="L18" s="6">
+        <v>5000</v>
+      </c>
+      <c r="M18" s="6">
+        <v>6000</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R18" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="S18" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="T18" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="U18" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="V18" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="W18" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="X18" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y18" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z18" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="AA18" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB18" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="AC18" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD18" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="AE18" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="L19" s="6">
+        <v>1500</v>
+      </c>
+      <c r="M19" s="11" t="s">
         <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="6">
+        <v>4</v>
+      </c>
+      <c r="H20" s="6">
+        <v>700</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="J20" s="6">
+        <v>2500</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="X20" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y20" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="6">
+        <v>99999</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="I21" s="6">
+        <v>1999.99</v>
+      </c>
+      <c r="J21" s="6">
+        <v>333333.33</v>
+      </c>
+      <c r="X21" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y21" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L22" s="6">
+        <v>5</v>
+      </c>
+      <c r="M22" s="6">
+        <v>10550</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="O22" s="6">
+        <v>21568</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="T22" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="U22" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="V22" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="W22" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="X22" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y22" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="Z22" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="AA22" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="AE22" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF22" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="AG22" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH22" s="6">
+        <v>2017</v>
+      </c>
+      <c r="AI22" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="AJ22" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="6">
+        <v>6500</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="I23" s="6">
+        <v>12222</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="K23" s="6">
+        <v>7</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="X23" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="Y23" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="6">
+        <v>999.99</v>
+      </c>
+      <c r="H24" s="6">
+        <v>100000.01</v>
+      </c>
+      <c r="I24" s="6">
+        <v>125000.01</v>
+      </c>
+      <c r="J24" s="6">
+        <v>4999.99</v>
+      </c>
+      <c r="K24" s="6">
+        <v>150000.01</v>
+      </c>
+      <c r="L24" s="6">
+        <v>1000000.99</v>
+      </c>
+      <c r="M24" s="6">
+        <v>6789</v>
+      </c>
+      <c r="N24" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="X24" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="Y24" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="Z24" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA24" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AB24" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AC24" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="6">
+        <v>5000</v>
+      </c>
+      <c r="H25" s="6">
+        <v>10000</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="X25" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y25" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Z25" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="6">
+        <v>6321.17</v>
+      </c>
+      <c r="H26" s="6">
+        <v>9841.5</v>
+      </c>
+      <c r="X26" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y26" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2562,7 +3210,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G2" sqref="G2:AF2"/>
+      <selection pane="topRight" activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated/Added IO-Existing Member scripts
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrown\TDECUWorkspace\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97389A16-E70C-453D-9B83-C5CB1B49DCA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="507">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1428,12 +1427,132 @@
   </si>
   <si>
     <t>Please select an answer for question 4.</t>
+  </si>
+  <si>
+    <t>8244863</t>
+  </si>
+  <si>
+    <t>111223333</t>
+  </si>
+  <si>
+    <t>04041984</t>
+  </si>
+  <si>
+    <t>C24030_VerifySaveProgressOption</t>
+  </si>
+  <si>
+    <t>04042010</t>
+  </si>
+  <si>
+    <t>04042025</t>
+  </si>
+  <si>
+    <t>Austin Airport</t>
+  </si>
+  <si>
+    <t>Storm Relief</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>email@hotmail.com</t>
+  </si>
+  <si>
+    <t>8244872</t>
+  </si>
+  <si>
+    <t>410258963</t>
+  </si>
+  <si>
+    <t>12251987</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>C24031_VerifyValidLoginToSave</t>
+  </si>
+  <si>
+    <t>testgmail.com</t>
+  </si>
+  <si>
+    <t>test@gmail</t>
+  </si>
+  <si>
+    <t>Please enter a valid email address.</t>
+  </si>
+  <si>
+    <t>Please enter some text.</t>
+  </si>
+  <si>
+    <t>Short#1</t>
+  </si>
+  <si>
+    <t>NUMBER5?</t>
+  </si>
+  <si>
+    <t>234+lower</t>
+  </si>
+  <si>
+    <t>UP(PER)!</t>
+  </si>
+  <si>
+    <t>p@ssword</t>
+  </si>
+  <si>
+    <t>$678_90*</t>
+  </si>
+  <si>
+    <t>ZYXabcWVU</t>
+  </si>
+  <si>
+    <t>Please create a stronger password. Passwords must be at least 8 characters long and include three of the following: uppercase letter, lowercase letter, a number or a special character. Allowable special characters include the following: !@#$%^&amp;*()_&gt;</t>
+  </si>
+  <si>
+    <t>C24052_VerifyAccountFundingOption</t>
+  </si>
+  <si>
+    <t>Transfer Funds</t>
+  </si>
+  <si>
+    <t>Electronic Check</t>
+  </si>
+  <si>
+    <t>Debit/Credit Card</t>
+  </si>
+  <si>
+    <t>C24054_VerifyCDFunding</t>
+  </si>
+  <si>
+    <t>18 Month Share Certificate (Estimated Maturity Date:</t>
+  </si>
+  <si>
+    <t>Please enter an amount for 18 Month Share Certificate between $1,000.00 and $100,000.00</t>
+  </si>
+  <si>
+    <t>C24055_VerifyCheckingFunding</t>
+  </si>
+  <si>
+    <t>Please enter a value between $1 and $2,500</t>
+  </si>
+  <si>
+    <t>C24056_VerifyMoneyMarketFunding</t>
+  </si>
+  <si>
+    <t>C24057_VerifyClubFunding</t>
+  </si>
+  <si>
+    <t>Please enter an amount for Club Account between $1.00 and $2,500.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1810,11 +1929,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F98"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="B65" sqref="B65:D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2703,97 +2822,174 @@
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="4"/>
+      <c r="A59" t="s">
+        <v>470</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="4"/>
+      <c r="A60" t="s">
+        <v>482</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="4"/>
+      <c r="A61" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="4"/>
+      <c r="A62" t="s">
+        <v>499</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="4"/>
+      <c r="A63" t="s">
+        <v>502</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="4"/>
+      <c r="A64" t="s">
+        <v>504</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B65" s="4"/>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>505</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B66" s="4"/>
       <c r="E66" s="2"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B67" s="4"/>
       <c r="E67" s="2"/>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B68" s="4"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B69" s="4"/>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B70" s="4"/>
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
       <c r="E71" s="2"/>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
       <c r="E72" s="2"/>
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B74" s="4"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" s="4"/>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
       <c r="E77" s="2"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B78" s="4"/>
       <c r="E78" s="2"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B79" s="4"/>
       <c r="E79" s="2"/>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B80" s="4"/>
       <c r="F80" s="1"/>
     </row>
@@ -2877,82 +3073,91 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B15" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B13" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="B52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="B54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="B58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="B12" r:id="rId11"/>
+    <hyperlink ref="B14" r:id="rId12"/>
+    <hyperlink ref="B16" r:id="rId13"/>
+    <hyperlink ref="B17" r:id="rId14"/>
+    <hyperlink ref="B18" r:id="rId15"/>
+    <hyperlink ref="B19" r:id="rId16"/>
+    <hyperlink ref="B20" r:id="rId17"/>
+    <hyperlink ref="B21" r:id="rId18"/>
+    <hyperlink ref="B22" r:id="rId19"/>
+    <hyperlink ref="B23" r:id="rId20"/>
+    <hyperlink ref="B24" r:id="rId21"/>
+    <hyperlink ref="B15" r:id="rId22"/>
+    <hyperlink ref="B13" r:id="rId23"/>
+    <hyperlink ref="B25" r:id="rId24"/>
+    <hyperlink ref="B26" r:id="rId25"/>
+    <hyperlink ref="B27" r:id="rId26"/>
+    <hyperlink ref="B28" r:id="rId27"/>
+    <hyperlink ref="B29" r:id="rId28"/>
+    <hyperlink ref="B30" r:id="rId29"/>
+    <hyperlink ref="B31" r:id="rId30"/>
+    <hyperlink ref="B32" r:id="rId31"/>
+    <hyperlink ref="B33" r:id="rId32"/>
+    <hyperlink ref="B34" r:id="rId33"/>
+    <hyperlink ref="B35" r:id="rId34"/>
+    <hyperlink ref="B36" r:id="rId35"/>
+    <hyperlink ref="B37" r:id="rId36"/>
+    <hyperlink ref="B38" r:id="rId37"/>
+    <hyperlink ref="B39" r:id="rId38"/>
+    <hyperlink ref="B40" r:id="rId39"/>
+    <hyperlink ref="B41" r:id="rId40"/>
+    <hyperlink ref="B42" r:id="rId41"/>
+    <hyperlink ref="B43" r:id="rId42"/>
+    <hyperlink ref="B44" r:id="rId43"/>
+    <hyperlink ref="B45" r:id="rId44"/>
+    <hyperlink ref="B46" r:id="rId45"/>
+    <hyperlink ref="B47" r:id="rId46"/>
+    <hyperlink ref="B48" r:id="rId47"/>
+    <hyperlink ref="B49" r:id="rId48"/>
+    <hyperlink ref="B50" r:id="rId49"/>
+    <hyperlink ref="B51" r:id="rId50"/>
+    <hyperlink ref="B52" r:id="rId51"/>
+    <hyperlink ref="B53" r:id="rId52"/>
+    <hyperlink ref="B54" r:id="rId53"/>
+    <hyperlink ref="B55" r:id="rId54"/>
+    <hyperlink ref="B56" r:id="rId55"/>
+    <hyperlink ref="B57" r:id="rId56"/>
+    <hyperlink ref="B58" r:id="rId57"/>
+    <hyperlink ref="B59" r:id="rId58"/>
+    <hyperlink ref="B60" r:id="rId59"/>
+    <hyperlink ref="B61" r:id="rId60"/>
+    <hyperlink ref="B62" r:id="rId61"/>
+    <hyperlink ref="B63" r:id="rId62"/>
+    <hyperlink ref="B64" r:id="rId63"/>
+    <hyperlink ref="B65" r:id="rId64"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId58"/>
+  <pageSetup orientation="portrait" r:id="rId65"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AM58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A19" sqref="A19"/>
+      <selection pane="topRight" activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="41" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27" style="6" customWidth="1"/>
     <col min="5" max="5" width="24" style="6" customWidth="1"/>
     <col min="6" max="6" width="24" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" style="6" customWidth="1"/>
@@ -3487,6 +3692,9 @@
       <c r="H7" s="11" t="s">
         <v>188</v>
       </c>
+      <c r="I7" s="11" t="s">
+        <v>481</v>
+      </c>
       <c r="J7" s="11" t="s">
         <v>48</v>
       </c>
@@ -3534,6 +3742,12 @@
       </c>
       <c r="Y7" s="6" t="s">
         <v>104</v>
+      </c>
+      <c r="Z7" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="AA7" s="11" t="s">
+        <v>480</v>
       </c>
       <c r="AB7" s="12" t="s">
         <v>177</v>
@@ -5597,13 +5811,291 @@
         <v>466</v>
       </c>
       <c r="AB58" s="12" t="s">
-        <v>328</v>
+        <v>467</v>
       </c>
       <c r="AC58" s="12" t="s">
-        <v>329</v>
+        <v>468</v>
       </c>
       <c r="AD58" s="12" t="s">
-        <v>166</v>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="G59" s="6">
+        <v>2500</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="Q59" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R59" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="S59" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="T59" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="U59" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="V59" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="W59" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="X59" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="Y59" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z59" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA59" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB59" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="AC59" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD59" s="12" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="J60" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="L60" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="M60" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="N60" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="O60" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="P60" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="Q60" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="R60" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="S60" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="AB60" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="AC60" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="AD60" s="12" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="G61" s="6">
+        <v>1000</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q61" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB61" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="AC61" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD61" s="12" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>481</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L62" s="6">
+        <v>999.99</v>
+      </c>
+      <c r="M62" s="6">
+        <v>200000</v>
+      </c>
+      <c r="N62" s="6">
+        <v>50000</v>
+      </c>
+      <c r="AB62" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="AC62" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="AD62" s="12" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L63" s="6">
+        <v>2501</v>
+      </c>
+      <c r="M63" s="6">
+        <v>0</v>
+      </c>
+      <c r="N63" s="6">
+        <v>1000</v>
+      </c>
+      <c r="AB63" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="AC63" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD63" s="12" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="AB64" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="AC64" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="AD64" s="12" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L65" s="6">
+        <v>3000</v>
+      </c>
+      <c r="M65" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="N65" s="6">
+        <v>2500</v>
+      </c>
+      <c r="AB65" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="AC65" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD65" s="12" t="s">
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -5613,7 +6105,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF30"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
12/2/19 Created existing member scripts
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="518">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1547,6 +1547,39 @@
   </si>
   <si>
     <t>Please enter an amount for Club Account between $1.00 and $2,500.00</t>
+  </si>
+  <si>
+    <t>C24058_VerifyTransferFundsMethod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I would like to transfer funds from: </t>
+  </si>
+  <si>
+    <t>8244863 CK - 611 Classic Checking</t>
+  </si>
+  <si>
+    <t>8244863 SAV - 603 Main Share</t>
+  </si>
+  <si>
+    <t>C24063_VerifyMaxFundingAmount</t>
+  </si>
+  <si>
+    <t>3 Month Share Certificate (Estimated Maturity Date:</t>
+  </si>
+  <si>
+    <t>The maximum funding amount is $100,000.00. Please adjust your amount and try again.</t>
+  </si>
+  <si>
+    <t>8244872 CK - 801 Classic Checking</t>
+  </si>
+  <si>
+    <t>C24269_VerifyCDFundingAmount</t>
+  </si>
+  <si>
+    <t>13 Month Share Certificate (Estimated Maturity Date:</t>
+  </si>
+  <si>
+    <t>13 Month Share Certificate</t>
   </si>
 </sst>
 </file>
@@ -1932,8 +1965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65:D65"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68:D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2927,17 +2960,50 @@
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B66" s="4"/>
+      <c r="A66" t="s">
+        <v>507</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E66" s="2"/>
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="4"/>
+      <c r="A67" t="s">
+        <v>511</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E67" s="2"/>
       <c r="F67" s="1"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B68" s="4"/>
+      <c r="A68" t="s">
+        <v>515</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F68" s="1"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -3137,19 +3203,22 @@
     <hyperlink ref="B63" r:id="rId62"/>
     <hyperlink ref="B64" r:id="rId63"/>
     <hyperlink ref="B65" r:id="rId64"/>
+    <hyperlink ref="B66" r:id="rId65"/>
+    <hyperlink ref="B67" r:id="rId66"/>
+    <hyperlink ref="B68" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId65"/>
+  <pageSetup orientation="portrait" r:id="rId68"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM65"/>
+  <dimension ref="A1:AM68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H65" sqref="H65"/>
+      <selection pane="topRight" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6096,6 +6165,102 @@
       </c>
       <c r="AD65" s="12" t="s">
         <v>479</v>
+      </c>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="L66" s="6">
+        <v>10</v>
+      </c>
+      <c r="AB66" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="AC66" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="AD66" s="12" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="67" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="L67" s="6">
+        <v>99999</v>
+      </c>
+      <c r="M67" s="6">
+        <v>2000</v>
+      </c>
+      <c r="AB67" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="AC67" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD67" s="12" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="G68" s="6">
+        <v>1500</v>
+      </c>
+      <c r="H68" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="AB68" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="AC68" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="AD68" s="12" t="s">
+        <v>469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated IO Existing Member scripts
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="512">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -157,18 +157,6 @@
     <t>Minimum $2,000.00</t>
   </si>
   <si>
-    <t>Classic MasterCard &amp;reg;</t>
-  </si>
-  <si>
-    <t>Buc-ee's MasterCard &amp;reg;</t>
-  </si>
-  <si>
-    <t>Onyx MasterCard &amp;reg;</t>
-  </si>
-  <si>
-    <t>Platinum MasterCard &amp;reg;</t>
-  </si>
-  <si>
     <t>C24106_VerifyVehicleLoanSelection</t>
   </si>
   <si>
@@ -322,9 +310,6 @@
     <t>ProdDesc7</t>
   </si>
   <si>
-    <t>Cash $tash&amp;trade; Line of Credit</t>
-  </si>
-  <si>
     <t>Borrow 100% of your current share savings account balance</t>
   </si>
   <si>
@@ -367,9 +352,6 @@
     <t>High-yield investment account with a competitive rate</t>
   </si>
   <si>
-    <t>$2,500 minimum deposit required</t>
-  </si>
-  <si>
     <t>Minimum balance must be maintained to avoid $10 monthly service charge</t>
   </si>
   <si>
@@ -520,9 +502,6 @@
     <t>5000</t>
   </si>
   <si>
-    <t>8229386</t>
-  </si>
-  <si>
     <t>456127890</t>
   </si>
   <si>
@@ -559,15 +538,6 @@
     <t>6000</t>
   </si>
   <si>
-    <t>8229319</t>
-  </si>
-  <si>
-    <t>023465789</t>
-  </si>
-  <si>
-    <t>02061980</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -598,9 +568,6 @@
     <t>$500.00</t>
   </si>
   <si>
-    <t>Please enter an amount for 12 Month Share Certificate between $1,000.00 and $100,000.00</t>
-  </si>
-  <si>
     <t>C24110_VerifySavingsSelection</t>
   </si>
   <si>
@@ -643,12 +610,6 @@
     <t>C24314_VerifyCheckingAccountSelection2</t>
   </si>
   <si>
-    <t>Online/Mobile Banking</t>
-  </si>
-  <si>
-    <t>12 Month Share Certificate (Estimated Maturity Date:</t>
-  </si>
-  <si>
     <t>24 Month Share Certificate (Estimated Maturity Date:</t>
   </si>
   <si>
@@ -790,9 +751,6 @@
     <t>Debit Card</t>
   </si>
   <si>
-    <t>Courtesty Pay Opt-In</t>
-  </si>
-  <si>
     <t>C24257_VerifyFreedomLoanNotDisplayed</t>
   </si>
   <si>
@@ -1012,12 +970,6 @@
     <t>income</t>
   </si>
   <si>
-    <t>8229312</t>
-  </si>
-  <si>
-    <t>168151171</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -1183,18 +1135,6 @@
     <t>C24285_VerifyPersonalInfoRO</t>
   </si>
   <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>Applicant</t>
-  </si>
-  <si>
-    <t>1221 SW 4th Ave</t>
-  </si>
-  <si>
-    <t>Portland, OR 97204-1900</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -1213,9 +1153,6 @@
     <t>C24070_VerifyMemberVerification</t>
   </si>
   <si>
-    <t>456-12-7890</t>
-  </si>
-  <si>
     <t>01/01/1980</t>
   </si>
   <si>
@@ -1288,12 +1225,6 @@
     <t>$36,541.00</t>
   </si>
   <si>
-    <t>023-46-5789</t>
-  </si>
-  <si>
-    <t>02/06/1980</t>
-  </si>
-  <si>
     <t>06/21/2011</t>
   </si>
   <si>
@@ -1558,9 +1489,6 @@
     <t>8244863 CK - 611 Classic Checking</t>
   </si>
   <si>
-    <t>8244863 SAV - 603 Main Share</t>
-  </si>
-  <si>
     <t>C24063_VerifyMaxFundingAmount</t>
   </si>
   <si>
@@ -1570,16 +1498,70 @@
     <t>The maximum funding amount is $100,000.00. Please adjust your amount and try again.</t>
   </si>
   <si>
-    <t>8244872 CK - 801 Classic Checking</t>
-  </si>
-  <si>
     <t>C24269_VerifyCDFundingAmount</t>
   </si>
   <si>
-    <t>13 Month Share Certificate (Estimated Maturity Date:</t>
-  </si>
-  <si>
-    <t>13 Month Share Certificate</t>
+    <t>Classic MasterCard ®</t>
+  </si>
+  <si>
+    <t> Buc-ee's MasterCard ®</t>
+  </si>
+  <si>
+    <t>Platinum MasterCard ®</t>
+  </si>
+  <si>
+    <t>$2,500 deposit required</t>
+  </si>
+  <si>
+    <t>Additional funds may be deposited once account is opened</t>
+  </si>
+  <si>
+    <t>12 Month Promotional Share Certificate (Estimated Maturity Date:</t>
+  </si>
+  <si>
+    <t>Please enter an amount for 12 Month Promotional Share Certificate between $1,000.00 and $100,000.00</t>
+  </si>
+  <si>
+    <t>8244893</t>
+  </si>
+  <si>
+    <t>125229991</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>887 Holly Branch Dr</t>
+  </si>
+  <si>
+    <t>Gatlinburg, TN 37738-3921</t>
+  </si>
+  <si>
+    <t>125-22-9991</t>
+  </si>
+  <si>
+    <t>111-22-3333</t>
+  </si>
+  <si>
+    <t>410-25-8963</t>
+  </si>
+  <si>
+    <t>04/04/1984</t>
+  </si>
+  <si>
+    <t>12/25/1987</t>
+  </si>
+  <si>
+    <t>60 Month Share Certificate (Estimated Maturity Date:</t>
+  </si>
+  <si>
+    <t>8244893 CK - 726 High Yield Checking</t>
+  </si>
+  <si>
+    <t>8244893 SAV - 718 Main Share</t>
   </si>
 </sst>
 </file>
@@ -1632,7 +1614,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1648,6 +1630,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2046,7 +2029,7 @@
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
@@ -2061,7 +2044,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>8</v>
@@ -2076,7 +2059,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
@@ -2092,7 +2075,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>8</v>
@@ -2108,7 +2091,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
@@ -2123,7 +2106,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>8</v>
@@ -2137,7 +2120,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>8</v>
@@ -2151,7 +2134,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>8</v>
@@ -2166,7 +2149,7 @@
     </row>
     <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>8</v>
@@ -2181,7 +2164,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>8</v>
@@ -2196,7 +2179,7 @@
     </row>
     <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>8</v>
@@ -2211,7 +2194,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>8</v>
@@ -2226,7 +2209,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>8</v>
@@ -2241,7 +2224,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>8</v>
@@ -2256,7 +2239,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>8</v>
@@ -2271,7 +2254,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>8</v>
@@ -2286,7 +2269,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>8</v>
@@ -2301,7 +2284,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>8</v>
@@ -2316,7 +2299,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>8</v>
@@ -2331,7 +2314,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>8</v>
@@ -2346,7 +2329,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>8</v>
@@ -2361,7 +2344,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>8</v>
@@ -2376,7 +2359,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>8</v>
@@ -2391,7 +2374,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>8</v>
@@ -2406,7 +2389,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>8</v>
@@ -2421,7 +2404,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>8</v>
@@ -2436,7 +2419,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>8</v>
@@ -2451,7 +2434,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>8</v>
@@ -2466,7 +2449,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>8</v>
@@ -2481,7 +2464,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>8</v>
@@ -2496,7 +2479,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>8</v>
@@ -2511,7 +2494,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>8</v>
@@ -2526,7 +2509,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>8</v>
@@ -2541,7 +2524,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>8</v>
@@ -2556,7 +2539,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>8</v>
@@ -2571,7 +2554,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>8</v>
@@ -2586,7 +2569,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>8</v>
@@ -2601,7 +2584,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>8</v>
@@ -2616,7 +2599,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>8</v>
@@ -2631,7 +2614,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>8</v>
@@ -2646,7 +2629,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>8</v>
@@ -2661,7 +2644,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>8</v>
@@ -2676,7 +2659,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>8</v>
@@ -2691,7 +2674,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>397</v>
+        <v>376</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>8</v>
@@ -2706,7 +2689,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>8</v>
@@ -2721,7 +2704,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>406</v>
+        <v>385</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>8</v>
@@ -2736,7 +2719,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>407</v>
+        <v>386</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>8</v>
@@ -2751,7 +2734,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>8</v>
@@ -2766,7 +2749,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>426</v>
+        <v>403</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>8</v>
@@ -2781,7 +2764,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>427</v>
+        <v>404</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>8</v>
@@ -2796,7 +2779,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>8</v>
@@ -2811,7 +2794,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>454</v>
+        <v>431</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>8</v>
@@ -2826,7 +2809,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>457</v>
+        <v>434</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>8</v>
@@ -2841,7 +2824,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>461</v>
+        <v>438</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>8</v>
@@ -2856,7 +2839,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>470</v>
+        <v>447</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>8</v>
@@ -2871,7 +2854,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>482</v>
+        <v>459</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>8</v>
@@ -2886,7 +2869,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>495</v>
+        <v>472</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>8</v>
@@ -2901,7 +2884,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>499</v>
+        <v>476</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>8</v>
@@ -2916,7 +2899,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>502</v>
+        <v>479</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>8</v>
@@ -2931,7 +2914,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>504</v>
+        <v>481</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>8</v>
@@ -2946,7 +2929,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>505</v>
+        <v>482</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>8</v>
@@ -2961,7 +2944,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>507</v>
+        <v>484</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>8</v>
@@ -2977,7 +2960,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>511</v>
+        <v>487</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>8</v>
@@ -2993,7 +2976,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>515</v>
+        <v>490</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>8</v>
@@ -3216,9 +3199,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D68" sqref="D68"/>
+      <selection pane="topRight" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3252,82 +3235,82 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="V1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="T1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="AA1" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="AB1" s="3" t="s">
         <v>19</v>
@@ -3339,31 +3322,31 @@
         <v>14</v>
       </c>
       <c r="AE1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AK1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3377,10 +3360,10 @@
         <v>27</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>28</v>
@@ -3401,10 +3384,10 @@
         <v>34</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="X2" s="6" t="s">
         <v>24</v>
@@ -3423,34 +3406,34 @@
         <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>43</v>
+        <v>491</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>44</v>
+        <v>492</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>46</v>
+        <v>493</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>41</v>
@@ -3462,13 +3445,13 @@
         <v>2000</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="R4" s="6" t="s">
         <v>36</v>
@@ -3477,13 +3460,13 @@
         <v>37</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="X4" s="6" t="s">
         <v>38</v>
@@ -3495,69 +3478,69 @@
         <v>40</v>
       </c>
       <c r="AA4" s="11" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="AB4" s="12" t="s">
-        <v>164</v>
+        <v>444</v>
       </c>
       <c r="AC4" s="12" t="s">
-        <v>165</v>
+        <v>445</v>
       </c>
       <c r="AD4" s="12" t="s">
-        <v>166</v>
+        <v>446</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="AG4" s="8" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="AH4" s="8" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="N5" s="6">
         <v>5000</v>
@@ -3566,126 +3549,123 @@
         <v>6000</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>18</v>
       </c>
       <c r="T5" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="X5" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y5" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z5" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA5" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="AB5" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="AC5" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="AD5" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="AE5" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF5" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="U5" s="11" t="s">
+      <c r="AG5" s="11" t="s">
         <v>171</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="W5" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="X5" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="Y5" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="Z5" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="AA5" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="AB5" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="AC5" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="AD5" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="AE5" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="AF5" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="AG5" s="11" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="K6" s="6" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>41</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="T6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="W6" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="U6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="W6" s="6" t="s">
-        <v>100</v>
       </c>
       <c r="X6" s="6">
         <v>2000</v>
@@ -3697,78 +3677,78 @@
         <v>18</v>
       </c>
       <c r="AA6" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB6" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="AC6" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="AD6" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="AE6" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="AF6" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG6" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="AH6" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI6" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ6" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AB6" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="AC6" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="AD6" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="AE6" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="AF6" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="AG6" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="AH6" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="AI6" s="11" t="s">
+      <c r="AK6" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="AJ6" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="AK6" s="11" t="s">
-        <v>163</v>
-      </c>
       <c r="AL6" s="11" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="AM6" s="11" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>481</v>
+        <v>458</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>206</v>
+        <v>496</v>
       </c>
       <c r="L7" s="6">
         <v>500</v>
@@ -3777,7 +3757,7 @@
         <v>1000</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="O7" s="6">
         <v>5000</v>
@@ -3786,162 +3766,165 @@
         <v>12000</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="S7" s="6" t="s">
         <v>18</v>
       </c>
       <c r="T7" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="U7" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="V7" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="W7" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z7" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="AA7" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="AC7" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="AD7" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="AE7" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="AF7" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="AG7" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="AH7" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI7" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ7" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="U7" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="V7" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="W7" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z7" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="AA7" s="11" t="s">
-        <v>480</v>
-      </c>
-      <c r="AB7" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="AC7" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="AD7" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="AE7" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="AF7" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="AG7" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="AH7" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="AI7" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="AJ7" s="11" t="s">
-        <v>180</v>
-      </c>
       <c r="AK7" s="11" t="s">
-        <v>190</v>
+        <v>497</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="R8" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="S8" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="T8" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="U8" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="R8" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="S8" s="6" t="s">
+      <c r="X8" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="T8" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="U8" s="6" t="s">
+      <c r="Y8" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="X8" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y8" s="6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q9" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="L14" s="6">
         <v>2000</v>
@@ -3958,27 +3941,27 @@
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>117</v>
+        <v>240</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>254</v>
+        <v>111</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L16" s="6">
         <v>1000</v>
@@ -3987,86 +3970,86 @@
         <v>18</v>
       </c>
       <c r="R16" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="T16" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="U16" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="V16" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="W16" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="X16" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="S16" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="T16" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="U16" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="V16" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="W16" s="11" t="s">
+      <c r="Y16" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="X16" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="Y16" s="11" t="s">
-        <v>163</v>
-      </c>
       <c r="Z16" s="11" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="AA16" s="11" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="AB16" s="12" t="s">
-        <v>164</v>
+        <v>444</v>
       </c>
       <c r="AC16" s="12" t="s">
-        <v>165</v>
+        <v>445</v>
       </c>
       <c r="AD16" s="12" t="s">
-        <v>166</v>
+        <v>446</v>
       </c>
       <c r="AE16" s="11" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AB17" s="12" t="s">
-        <v>177</v>
+        <v>454</v>
       </c>
       <c r="AC17" s="12" t="s">
-        <v>178</v>
+        <v>455</v>
       </c>
       <c r="AD17" s="12" t="s">
-        <v>179</v>
+        <v>456</v>
       </c>
       <c r="AE17" s="6" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="AF17" s="6" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>204</v>
+      <c r="A18" s="13" t="s">
+        <v>193</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="L18" s="6">
         <v>5000</v>
@@ -4078,83 +4061,83 @@
         <v>18</v>
       </c>
       <c r="R18" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="S18" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="T18" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="U18" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="V18" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="W18" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="X18" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="S18" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="T18" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="U18" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="V18" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="W18" s="11" t="s">
+      <c r="Y18" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="X18" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="Y18" s="11" t="s">
-        <v>163</v>
-      </c>
       <c r="Z18" s="11" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="AA18" s="11" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="AB18" s="12" t="s">
-        <v>164</v>
+        <v>498</v>
       </c>
       <c r="AC18" s="12" t="s">
-        <v>165</v>
+        <v>499</v>
       </c>
       <c r="AD18" s="12" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="AE18" s="6" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>43</v>
+        <v>491</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>44</v>
+        <v>492</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>46</v>
+        <v>493</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="L19" s="6">
         <v>1500</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="G20" s="6">
         <v>4</v>
@@ -4163,36 +4146,36 @@
         <v>700</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="J20" s="6">
         <v>2500</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="L20" s="6" t="s">
         <v>42</v>
       </c>
       <c r="X20" s="6" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="Y20" s="6" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>44</v>
+        <v>492</v>
       </c>
       <c r="G21" s="6">
         <v>99999</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="I21" s="6">
         <v>1999.99</v>
@@ -4201,45 +4184,45 @@
         <v>333333.33</v>
       </c>
       <c r="X21" s="6" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="Y21" s="6" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="F22" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J22" s="6" t="s">
+      <c r="K22" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="L22" s="6">
         <v>5</v>
@@ -4248,116 +4231,116 @@
         <v>10550</v>
       </c>
       <c r="N22" s="11" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="O22" s="6">
         <v>21568</v>
       </c>
       <c r="P22" s="11" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="Q22" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="T22" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="U22" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="V22" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="W22" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="X22" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y22" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z22" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA22" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="AE22" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF22" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="R22" s="6" t="s">
+      <c r="AG22" s="6" t="s">
         <v>224</v>
-      </c>
-      <c r="S22" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="T22" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="V22" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="W22" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="X22" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="Y22" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="Z22" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="AA22" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="AE22" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="AF22" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="AG22" s="6" t="s">
-        <v>237</v>
       </c>
       <c r="AH22" s="6">
         <v>2017</v>
       </c>
       <c r="AI22" s="11" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="AJ22" s="6" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G23" s="6">
         <v>6500</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="I23" s="6">
         <v>12222</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="K23" s="6">
         <v>7</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="X23" s="6" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="Y23" s="6" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G24" s="6">
         <v>999.99</v>
@@ -4381,36 +4364,36 @@
         <v>6789</v>
       </c>
       <c r="N24" s="11" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="X24" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y24" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="Z24" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="AA24" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE24" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="Y24" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="Z24" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="AA24" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="AE24" s="6" t="s">
-        <v>246</v>
-      </c>
       <c r="AF24" s="6" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G25" s="6">
         <v>5000</v>
@@ -4419,27 +4402,27 @@
         <v>10000</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="X25" s="6" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="Y25" s="6" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="Z25" s="6" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G26" s="6">
         <v>6321.17</v>
@@ -4448,18 +4431,18 @@
         <v>9841.5</v>
       </c>
       <c r="X26" s="6" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="Y26" s="6" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G27" s="6">
         <v>2000</v>
@@ -4471,163 +4454,163 @@
         <v>1000</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="L27" s="11" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="M27" s="11" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="N27" s="6">
         <v>13256.22</v>
       </c>
       <c r="O27" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q27" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="R27" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="S27" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="T27" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="U27" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="V27" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="X27" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="Y27" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z27" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="AA27" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="AE27" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="AF27" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="AG27" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="AH27" s="11" t="s">
         <v>265</v>
-      </c>
-      <c r="Q27" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="R27" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="S27" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="T27" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="U27" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="V27" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="X27" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="Y27" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z27" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="AA27" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="AE27" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="AF27" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="AG27" s="11" t="s">
-        <v>278</v>
-      </c>
-      <c r="AH27" s="11" t="s">
-        <v>279</v>
       </c>
       <c r="AI27" s="6">
         <v>16872.560000000001</v>
       </c>
       <c r="AJ27" s="11" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="G28" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="H28" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="I28" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="L28" s="6">
         <v>5000</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="Q28" s="6" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="R28" s="6" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="S28" s="6" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="T28" s="10" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M29" s="6">
         <v>13000</v>
       </c>
       <c r="N29" s="11" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="G30" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="H30" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="L30" s="6">
         <v>5</v>
@@ -4636,42 +4619,42 @@
         <v>25147</v>
       </c>
       <c r="N30" s="11" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="X30" s="6" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="Y30" s="6" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="Z30" s="6" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="AA30" s="6" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="AE30" s="6" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="AF30" s="6" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="AG30" s="6" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="AH30" s="6" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="G31" s="6">
         <v>800</v>
@@ -4680,76 +4663,76 @@
         <v>1000.11</v>
       </c>
       <c r="X31" s="6" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="Y31" s="6" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="Z31" s="6" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="G32" s="6">
         <v>3000</v>
       </c>
       <c r="X32" s="6" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="AB32" s="12" t="s">
-        <v>177</v>
+        <v>454</v>
       </c>
       <c r="AC32" s="12" t="s">
-        <v>178</v>
+        <v>455</v>
       </c>
       <c r="AD32" s="12" t="s">
-        <v>179</v>
+        <v>456</v>
       </c>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="G33" s="6">
         <v>4000</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="AB33" s="12" t="s">
-        <v>164</v>
+        <v>444</v>
       </c>
       <c r="AC33" s="12" t="s">
-        <v>165</v>
+        <v>445</v>
       </c>
       <c r="AD33" s="12" t="s">
-        <v>166</v>
+        <v>446</v>
       </c>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="G34" s="6">
         <v>6000</v>
@@ -4758,54 +4741,54 @@
         <v>-1</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="J34" s="11" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="K34" s="11" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="L34" s="11" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="M34" s="6">
         <v>1252</v>
       </c>
       <c r="N34" s="11" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="X34" s="6" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="Y34" s="6" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="AB34" s="12" t="s">
-        <v>177</v>
+        <v>454</v>
       </c>
       <c r="AC34" s="12" t="s">
-        <v>178</v>
+        <v>455</v>
       </c>
       <c r="AD34" s="12" t="s">
-        <v>179</v>
+        <v>456</v>
       </c>
       <c r="AE34" s="6" t="s">
         <v>18</v>
       </c>
       <c r="AF34" s="11" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="AG34" s="11" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="AH34" s="11" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="G35" s="6">
         <v>7000</v>
@@ -4814,34 +4797,34 @@
         <v>101</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="K35" s="11" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="L35" s="11" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="M35" s="11" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="X35" s="6" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="Y35" s="6" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="AB35" s="12" t="s">
-        <v>164</v>
+        <v>444</v>
       </c>
       <c r="AC35" s="12" t="s">
-        <v>165</v>
+        <v>445</v>
       </c>
       <c r="AD35" s="12" t="s">
-        <v>166</v>
+        <v>446</v>
       </c>
       <c r="AF35" s="11"/>
       <c r="AG35" s="11"/>
@@ -4849,28 +4832,28 @@
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="G36" s="6">
         <v>15000</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="AB36" s="12" t="s">
-        <v>177</v>
+        <v>454</v>
       </c>
       <c r="AC36" s="12" t="s">
-        <v>178</v>
+        <v>455</v>
       </c>
       <c r="AD36" s="12" t="s">
-        <v>179</v>
+        <v>456</v>
       </c>
       <c r="AF36" s="11"/>
       <c r="AG36" s="11"/>
@@ -4878,7 +4861,7 @@
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="G37" s="6">
         <v>35000</v>
@@ -4887,66 +4870,66 @@
         <v>2222</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="Q37" s="11" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="R37" s="11" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="S37" s="11" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="T37" s="11" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="U37" s="11" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="V37" s="6">
         <v>5500</v>
       </c>
       <c r="W37" s="11" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="X37" s="11" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="Y37" s="11" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="AB37" s="12" t="s">
-        <v>164</v>
+        <v>444</v>
       </c>
       <c r="AC37" s="12" t="s">
-        <v>165</v>
+        <v>445</v>
       </c>
       <c r="AD37" s="12" t="s">
-        <v>166</v>
+        <v>446</v>
       </c>
       <c r="AE37" s="6" t="s">
         <v>18</v>
       </c>
       <c r="AF37" s="11" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="AG37" s="11" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="AH37" s="11" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="G38" s="6">
         <v>1000</v>
@@ -4955,39 +4938,39 @@
         <v>100</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="J38" s="11" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="K38" s="11" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="L38" s="11" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="M38" s="11" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="X38" s="6" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="Y38" s="6" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="AB38" s="12" t="s">
-        <v>328</v>
+        <v>498</v>
       </c>
       <c r="AC38" s="12" t="s">
-        <v>329</v>
+        <v>499</v>
       </c>
       <c r="AD38" s="12" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="G39" s="6">
         <v>250000</v>
@@ -4996,45 +4979,45 @@
         <v>4000</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="K39" s="11" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="L39" s="11" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="X39" s="6" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="AB39" s="12" t="s">
-        <v>164</v>
+        <v>454</v>
       </c>
       <c r="AC39" s="12" t="s">
-        <v>165</v>
+        <v>455</v>
       </c>
       <c r="AD39" s="12" t="s">
-        <v>166</v>
+        <v>456</v>
       </c>
       <c r="AE39" s="6" t="s">
         <v>18</v>
       </c>
       <c r="AF39" s="11" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="AG39" s="12" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="AH39" s="12" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="G40" s="6">
         <v>500</v>
@@ -5043,54 +5026,54 @@
         <v>452.67</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="Q40" s="6" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="R40" s="6">
         <v>7000</v>
       </c>
       <c r="S40" s="11" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="T40" s="11" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="U40" s="11" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="X40" s="11" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="AB40" s="12" t="s">
-        <v>177</v>
+        <v>444</v>
       </c>
       <c r="AC40" s="12" t="s">
-        <v>178</v>
+        <v>445</v>
       </c>
       <c r="AD40" s="12" t="s">
-        <v>179</v>
+        <v>446</v>
       </c>
       <c r="AE40" s="6" t="s">
         <v>18</v>
       </c>
       <c r="AF40" s="11" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AG40" s="11" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="AH40" s="11" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="G41" s="6">
         <v>5000</v>
@@ -5099,69 +5082,69 @@
         <v>1954.23</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="K41" s="6">
         <v>4444.4399999999996</v>
       </c>
       <c r="L41" s="11" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="Q41" s="11" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="R41" s="11" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="S41" s="11" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="T41" s="11" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="V41" s="6">
         <v>3333.33</v>
       </c>
       <c r="W41" s="11" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="X41" s="11" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="Y41" s="11" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="AB41" s="12" t="s">
-        <v>164</v>
+        <v>498</v>
       </c>
       <c r="AC41" s="12" t="s">
-        <v>165</v>
+        <v>499</v>
       </c>
       <c r="AD41" s="12" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="AE41" s="6" t="s">
         <v>18</v>
       </c>
       <c r="AF41" s="11" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="AG41" s="11" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="AH41" s="11" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="G42" s="6">
         <v>123456.78</v>
@@ -5170,283 +5153,283 @@
         <v>200</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="J42" s="11" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="K42" s="11" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="L42" s="11" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="M42" s="11" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="X42" s="6" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="Y42" s="6" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="AB42" s="12" t="s">
-        <v>328</v>
+        <v>454</v>
       </c>
       <c r="AC42" s="12" t="s">
-        <v>329</v>
+        <v>455</v>
       </c>
       <c r="AD42" s="12" t="s">
-        <v>166</v>
+        <v>456</v>
       </c>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="G43" s="6">
         <v>9072.65</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="J43" s="11" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="K43" s="11" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="Q43" s="6" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="R43" s="6" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="S43" s="6" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="T43" s="11" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="X43" s="6" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="Y43" s="6" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="Z43" s="6" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="AA43" s="6" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="AB43" s="12" t="s">
-        <v>177</v>
+        <v>444</v>
       </c>
       <c r="AC43" s="12" t="s">
-        <v>178</v>
+        <v>445</v>
       </c>
       <c r="AD43" s="12" t="s">
-        <v>179</v>
+        <v>446</v>
       </c>
       <c r="AE43" s="11" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="AF43" s="11" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="AG43" s="11" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="AB44" s="12" t="s">
-        <v>164</v>
+        <v>498</v>
       </c>
       <c r="AC44" s="12" t="s">
-        <v>165</v>
+        <v>499</v>
       </c>
       <c r="AD44" s="12" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
       <c r="Q45" s="6" t="s">
-        <v>385</v>
+        <v>500</v>
       </c>
       <c r="S45" s="10" t="s">
-        <v>386</v>
+        <v>501</v>
       </c>
       <c r="T45" s="10"/>
       <c r="U45" s="6" t="s">
-        <v>387</v>
+        <v>502</v>
       </c>
       <c r="V45" s="6" t="s">
-        <v>388</v>
+        <v>503</v>
       </c>
       <c r="AB45" s="12" t="s">
-        <v>328</v>
+        <v>454</v>
       </c>
       <c r="AC45" s="12" t="s">
-        <v>329</v>
+        <v>455</v>
       </c>
       <c r="AD45" s="12" t="s">
-        <v>166</v>
+        <v>456</v>
       </c>
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
       <c r="AB46" s="12" t="s">
-        <v>177</v>
+        <v>444</v>
       </c>
       <c r="AC46" s="12" t="s">
-        <v>178</v>
+        <v>445</v>
       </c>
       <c r="AD46" s="12" t="s">
-        <v>179</v>
+        <v>446</v>
       </c>
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="G47" s="6">
         <v>100000</v>
       </c>
       <c r="AB47" s="12" t="s">
-        <v>164</v>
+        <v>498</v>
       </c>
       <c r="AC47" s="12" t="s">
-        <v>165</v>
+        <v>499</v>
       </c>
       <c r="AD47" s="12" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="AE47" s="11" t="s">
-        <v>395</v>
+        <v>504</v>
       </c>
       <c r="AF47" s="11" t="s">
-        <v>396</v>
+        <v>375</v>
       </c>
     </row>
     <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>397</v>
+        <v>376</v>
       </c>
       <c r="G48" s="6">
         <v>2000</v>
       </c>
       <c r="X48" s="6" t="s">
-        <v>398</v>
+        <v>377</v>
       </c>
       <c r="Y48" s="6" t="s">
-        <v>399</v>
+        <v>378</v>
       </c>
       <c r="Z48" s="6" t="s">
-        <v>400</v>
+        <v>379</v>
       </c>
       <c r="AA48" s="6" t="s">
-        <v>401</v>
+        <v>380</v>
       </c>
       <c r="AB48" s="12" t="s">
-        <v>328</v>
+        <v>454</v>
       </c>
       <c r="AC48" s="12" t="s">
-        <v>329</v>
+        <v>455</v>
       </c>
       <c r="AD48" s="12" t="s">
-        <v>166</v>
+        <v>456</v>
       </c>
       <c r="AE48" s="11" t="s">
-        <v>404</v>
+        <v>383</v>
       </c>
       <c r="AF48" s="11" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="AG48" s="11" t="s">
-        <v>402</v>
+        <v>381</v>
       </c>
       <c r="AH48" s="12" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
       <c r="AB49" s="12" t="s">
-        <v>177</v>
+        <v>444</v>
       </c>
       <c r="AC49" s="12" t="s">
-        <v>178</v>
+        <v>445</v>
       </c>
       <c r="AD49" s="12" t="s">
-        <v>179</v>
+        <v>446</v>
       </c>
     </row>
     <row r="50" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>406</v>
+      <c r="A50" s="13" t="s">
+        <v>385</v>
       </c>
       <c r="AB50" s="12" t="s">
-        <v>164</v>
+        <v>454</v>
       </c>
       <c r="AC50" s="12" t="s">
-        <v>165</v>
+        <v>455</v>
       </c>
       <c r="AD50" s="12" t="s">
-        <v>166</v>
+        <v>456</v>
       </c>
     </row>
     <row r="51" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>407</v>
+      <c r="A51" s="13" t="s">
+        <v>386</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G51" s="6">
         <v>10000</v>
@@ -5458,59 +5441,59 @@
         <v>18</v>
       </c>
       <c r="R51" s="11" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="S51" s="11" t="s">
-        <v>412</v>
+        <v>391</v>
       </c>
       <c r="T51" s="11" t="s">
-        <v>408</v>
+        <v>387</v>
       </c>
       <c r="U51" s="11" t="s">
-        <v>409</v>
+        <v>388</v>
       </c>
       <c r="V51" s="11" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="W51" s="11" t="s">
-        <v>410</v>
+        <v>389</v>
       </c>
       <c r="X51" s="11" t="s">
-        <v>411</v>
+        <v>390</v>
       </c>
       <c r="Y51" s="11" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="Z51" s="11"/>
       <c r="AA51" s="11"/>
       <c r="AB51" s="12" t="s">
-        <v>328</v>
+        <v>498</v>
       </c>
       <c r="AC51" s="12" t="s">
-        <v>329</v>
+        <v>499</v>
       </c>
       <c r="AD51" s="12" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G52" s="6">
         <v>36541</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
       <c r="I52" s="6">
         <v>4000</v>
@@ -5519,139 +5502,139 @@
         <v>18</v>
       </c>
       <c r="R52" s="11" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="S52" s="11" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
       <c r="T52" s="11" t="s">
-        <v>415</v>
+        <v>394</v>
       </c>
       <c r="U52" s="11" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
       <c r="V52" s="11" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="W52" s="11" t="s">
-        <v>417</v>
+        <v>396</v>
       </c>
       <c r="X52" s="11" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
       <c r="Y52" s="11" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="AB52" s="12" t="s">
-        <v>177</v>
+        <v>444</v>
       </c>
       <c r="AC52" s="12" t="s">
-        <v>178</v>
+        <v>445</v>
       </c>
       <c r="AD52" s="12" t="s">
-        <v>179</v>
+        <v>446</v>
       </c>
       <c r="AE52" s="11" t="s">
-        <v>420</v>
+        <v>505</v>
       </c>
       <c r="AF52" s="11" t="s">
-        <v>421</v>
+        <v>507</v>
       </c>
       <c r="AG52" s="11" t="s">
-        <v>422</v>
+        <v>399</v>
       </c>
       <c r="AH52" s="11" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="AI52" s="11" t="s">
-        <v>424</v>
+        <v>401</v>
       </c>
       <c r="AJ52" s="11" t="s">
-        <v>425</v>
+        <v>402</v>
       </c>
     </row>
     <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>426</v>
+        <v>403</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="AB53" s="12" t="s">
-        <v>177</v>
+        <v>454</v>
       </c>
       <c r="AC53" s="12" t="s">
-        <v>178</v>
+        <v>455</v>
       </c>
       <c r="AD53" s="12" t="s">
-        <v>179</v>
+        <v>456</v>
       </c>
       <c r="AE53" s="11" t="s">
-        <v>420</v>
+        <v>506</v>
       </c>
       <c r="AF53" s="11" t="s">
-        <v>421</v>
+        <v>508</v>
       </c>
     </row>
     <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>427</v>
+        <v>404</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>428</v>
+        <v>405</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>430</v>
+        <v>407</v>
       </c>
       <c r="AB54" s="12" t="s">
-        <v>164</v>
+        <v>498</v>
       </c>
       <c r="AC54" s="12" t="s">
-        <v>165</v>
+        <v>499</v>
       </c>
       <c r="AD54" s="12" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="AE54" s="11" t="s">
-        <v>395</v>
+        <v>504</v>
       </c>
       <c r="AF54" s="11" t="s">
-        <v>396</v>
+        <v>375</v>
       </c>
     </row>
     <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G55" s="6">
         <v>8000</v>
@@ -5660,99 +5643,99 @@
         <v>16000</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>432</v>
+        <v>409</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>441</v>
+        <v>418</v>
       </c>
       <c r="L55" s="6" t="s">
-        <v>443</v>
+        <v>420</v>
       </c>
       <c r="M55" s="6" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
       <c r="N55" s="6" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
       <c r="O55" s="6" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
       <c r="P55" s="6" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="Q55" s="6" t="s">
         <v>18</v>
       </c>
       <c r="R55" s="11" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
       <c r="S55" s="11" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
       <c r="T55" s="11" t="s">
-        <v>435</v>
+        <v>412</v>
       </c>
       <c r="U55" s="11" t="s">
-        <v>436</v>
+        <v>413</v>
       </c>
       <c r="V55" s="11" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="W55" s="11" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="X55" s="11" t="s">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="Y55" s="11" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
       <c r="Z55" s="11" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
       <c r="AA55" s="11" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="AB55" s="12" t="s">
-        <v>328</v>
+        <v>444</v>
       </c>
       <c r="AC55" s="12" t="s">
-        <v>329</v>
+        <v>445</v>
       </c>
       <c r="AD55" s="12" t="s">
-        <v>166</v>
+        <v>446</v>
       </c>
       <c r="AE55" s="11" t="s">
-        <v>442</v>
+        <v>419</v>
       </c>
       <c r="AF55" s="11" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
       <c r="AG55" s="11" t="s">
-        <v>449</v>
+        <v>426</v>
       </c>
       <c r="AH55" s="11" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
       <c r="AI55" s="11" t="s">
-        <v>451</v>
+        <v>428</v>
       </c>
       <c r="AJ55" s="11" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="AK55" s="11" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
     </row>
     <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>454</v>
+        <v>431</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G56" s="6">
         <v>9874.06</v>
@@ -5761,51 +5744,51 @@
         <v>18</v>
       </c>
       <c r="R56" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="S56" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="T56" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="U56" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="V56" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="W56" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="S56" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="T56" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="U56" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="V56" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="W56" s="11" t="s">
-        <v>180</v>
-      </c>
       <c r="X56" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="Y56" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="Z56" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA56" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB56" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="AC56" s="12" t="s">
         <v>455</v>
       </c>
-      <c r="Y56" s="11" t="s">
+      <c r="AD56" s="12" t="s">
         <v>456</v>
-      </c>
-      <c r="Z56" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA56" s="11" t="s">
-        <v>338</v>
-      </c>
-      <c r="AB56" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="AC56" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="AD56" s="12" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>457</v>
+        <v>434</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G57" s="6">
         <v>111111</v>
@@ -5814,249 +5797,249 @@
         <v>222222</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
       <c r="Q57" s="6" t="s">
         <v>18</v>
       </c>
       <c r="R57" s="11" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="S57" s="11" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="T57" s="11" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="U57" s="11" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="V57" s="11" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="W57" s="11" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="X57" s="11" t="s">
-        <v>459</v>
+        <v>436</v>
       </c>
       <c r="Y57" s="11" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
       <c r="Z57" s="11" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="AA57" s="11"/>
       <c r="AB57" s="12" t="s">
-        <v>164</v>
+        <v>498</v>
       </c>
       <c r="AC57" s="12" t="s">
-        <v>165</v>
+        <v>499</v>
       </c>
       <c r="AD57" s="12" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>461</v>
+        <v>438</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>462</v>
+        <v>439</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>464</v>
+        <v>441</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>465</v>
+        <v>442</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>466</v>
+        <v>443</v>
       </c>
       <c r="AB58" s="12" t="s">
-        <v>467</v>
+        <v>444</v>
       </c>
       <c r="AC58" s="12" t="s">
-        <v>468</v>
+        <v>445</v>
       </c>
       <c r="AD58" s="12" t="s">
-        <v>469</v>
+        <v>446</v>
       </c>
     </row>
     <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>470</v>
+        <v>447</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>474</v>
+        <v>451</v>
       </c>
       <c r="G59" s="6">
         <v>2500</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>475</v>
+        <v>452</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>476</v>
+        <v>453</v>
       </c>
       <c r="Q59" s="6" t="s">
         <v>18</v>
       </c>
       <c r="R59" s="11" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="S59" s="11" t="s">
-        <v>471</v>
+        <v>448</v>
       </c>
       <c r="T59" s="11" t="s">
-        <v>472</v>
+        <v>449</v>
       </c>
       <c r="U59" s="11" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
       <c r="V59" s="11" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="W59" s="11" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="X59" s="11" t="s">
-        <v>473</v>
+        <v>450</v>
       </c>
       <c r="Y59" s="11" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="Z59" s="11" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="AA59" s="11" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="AB59" s="12" t="s">
-        <v>477</v>
+        <v>454</v>
       </c>
       <c r="AC59" s="12" t="s">
-        <v>478</v>
+        <v>455</v>
       </c>
       <c r="AD59" s="12" t="s">
-        <v>479</v>
+        <v>456</v>
       </c>
     </row>
     <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>482</v>
+        <v>459</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>480</v>
+        <v>177</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>483</v>
+        <v>460</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>484</v>
+        <v>461</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>475</v>
+        <v>452</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>487</v>
+        <v>464</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>488</v>
+        <v>465</v>
       </c>
       <c r="L60" s="6" t="s">
-        <v>489</v>
+        <v>466</v>
       </c>
       <c r="M60" s="6" t="s">
-        <v>490</v>
+        <v>467</v>
       </c>
       <c r="N60" s="6" t="s">
-        <v>491</v>
+        <v>468</v>
       </c>
       <c r="O60" s="6" t="s">
-        <v>492</v>
+        <v>469</v>
       </c>
       <c r="P60" s="6" t="s">
-        <v>493</v>
+        <v>470</v>
       </c>
       <c r="Q60" s="6" t="s">
-        <v>485</v>
+        <v>462</v>
       </c>
       <c r="R60" s="11" t="s">
-        <v>486</v>
+        <v>463</v>
       </c>
       <c r="S60" s="11" t="s">
-        <v>494</v>
+        <v>471</v>
       </c>
       <c r="AB60" s="12" t="s">
-        <v>467</v>
+        <v>498</v>
       </c>
       <c r="AC60" s="12" t="s">
-        <v>468</v>
+        <v>499</v>
       </c>
       <c r="AD60" s="12" t="s">
-        <v>469</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>495</v>
+        <v>472</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>496</v>
+        <v>473</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>497</v>
+        <v>474</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>498</v>
+        <v>475</v>
       </c>
       <c r="G61" s="6">
         <v>1000</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="Q61" s="6" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="AB61" s="12" t="s">
-        <v>477</v>
+        <v>444</v>
       </c>
       <c r="AC61" s="12" t="s">
-        <v>478</v>
+        <v>445</v>
       </c>
       <c r="AD61" s="12" t="s">
-        <v>479</v>
+        <v>446</v>
       </c>
     </row>
     <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>499</v>
+        <v>476</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>481</v>
+        <v>458</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>500</v>
+        <v>477</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>501</v>
+        <v>478</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="L62" s="6">
         <v>999.99</v>
@@ -6068,30 +6051,30 @@
         <v>50000</v>
       </c>
       <c r="AB62" s="12" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="AC62" s="12" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="AD62" s="12" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
     </row>
     <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>502</v>
+        <v>479</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>503</v>
+        <v>480</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="L63" s="6">
         <v>2501</v>
@@ -6103,50 +6086,50 @@
         <v>1000</v>
       </c>
       <c r="AB63" s="12" t="s">
-        <v>477</v>
+        <v>498</v>
       </c>
       <c r="AC63" s="12" t="s">
-        <v>478</v>
+        <v>499</v>
       </c>
       <c r="AD63" s="12" t="s">
-        <v>479</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>504</v>
+        <v>481</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="AB64" s="12" t="s">
-        <v>467</v>
+        <v>444</v>
       </c>
       <c r="AC64" s="12" t="s">
-        <v>468</v>
+        <v>445</v>
       </c>
       <c r="AD64" s="12" t="s">
-        <v>469</v>
+        <v>446</v>
       </c>
     </row>
     <row r="65" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>505</v>
+        <v>482</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>506</v>
+        <v>483</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>503</v>
+        <v>480</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="L65" s="6">
         <v>3000</v>
@@ -6158,65 +6141,65 @@
         <v>2500</v>
       </c>
       <c r="AB65" s="12" t="s">
-        <v>477</v>
+        <v>454</v>
       </c>
       <c r="AC65" s="12" t="s">
-        <v>478</v>
+        <v>455</v>
       </c>
       <c r="AD65" s="12" t="s">
-        <v>479</v>
+        <v>456</v>
       </c>
     </row>
     <row r="66" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>507</v>
+        <v>484</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>508</v>
+        <v>485</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="L66" s="6">
         <v>10</v>
       </c>
       <c r="AB66" s="12" t="s">
-        <v>467</v>
+        <v>498</v>
       </c>
       <c r="AC66" s="12" t="s">
-        <v>468</v>
+        <v>499</v>
       </c>
       <c r="AD66" s="12" t="s">
-        <v>469</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>511</v>
+        <v>487</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>512</v>
+        <v>488</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>514</v>
+        <v>486</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>513</v>
+        <v>489</v>
       </c>
       <c r="L67" s="6">
         <v>99999</v>
@@ -6225,42 +6208,42 @@
         <v>2000</v>
       </c>
       <c r="AB67" s="12" t="s">
-        <v>477</v>
+        <v>444</v>
       </c>
       <c r="AC67" s="12" t="s">
-        <v>478</v>
+        <v>445</v>
       </c>
       <c r="AD67" s="12" t="s">
-        <v>479</v>
+        <v>446</v>
       </c>
     </row>
     <row r="68" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>515</v>
+        <v>490</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>316</v>
+        <v>178</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>517</v>
+        <v>406</v>
       </c>
       <c r="G68" s="6">
         <v>1500</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="AB68" s="12" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="AC68" s="12" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="AD68" s="12" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -6302,16 +6285,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>19</v>
@@ -6332,13 +6315,13 @@
         <v>11</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>15</v>
@@ -6350,49 +6333,49 @@
         <v>17</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New Existing Member Joint Owner/Beneficiary scripts
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="625">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1243,9 +1243,6 @@
     <t>C24027_VerifyModifyAccountSelection</t>
   </si>
   <si>
-    <t>6 Month Share Certificate</t>
-  </si>
-  <si>
     <t>60 Month Share Certificate</t>
   </si>
   <si>
@@ -1345,9 +1342,6 @@
     <t>C24029_VerifyIdentityQuestions</t>
   </si>
   <si>
-    <t>36 Month Share Certificate</t>
-  </si>
-  <si>
     <t>Please select an answer for question 1.</t>
   </si>
   <si>
@@ -1399,9 +1393,6 @@
     <t>12251987</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
@@ -1562,6 +1553,354 @@
   </si>
   <si>
     <t>8244893 SAV - 718 Main Share</t>
+  </si>
+  <si>
+    <t>6 Month Share Certificate (Estimated Maturity Date:</t>
+  </si>
+  <si>
+    <t>36 Month Share Certificate (Estimated Maturity Date:</t>
+  </si>
+  <si>
+    <t>Mobile Check Deposit</t>
+  </si>
+  <si>
+    <t>Deposit checks using our mobile banking app and your smartphone’s camera.</t>
+  </si>
+  <si>
+    <t>C26852_VerifyMobileDepositLink</t>
+  </si>
+  <si>
+    <t>Please enter a value between $500 and $5,000</t>
+  </si>
+  <si>
+    <t>C24211_VerifyOneJointOwner</t>
+  </si>
+  <si>
+    <t>8244906</t>
+  </si>
+  <si>
+    <t>568634668</t>
+  </si>
+  <si>
+    <t>10101990</t>
+  </si>
+  <si>
+    <t>Adeline</t>
+  </si>
+  <si>
+    <t>Rose</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>2534 E Norris St</t>
+  </si>
+  <si>
+    <t>05231982</t>
+  </si>
+  <si>
+    <t>456121250</t>
+  </si>
+  <si>
+    <t>K34Ldk9</t>
+  </si>
+  <si>
+    <t>05232015</t>
+  </si>
+  <si>
+    <t>05232026</t>
+  </si>
+  <si>
+    <t>Peterson</t>
+  </si>
+  <si>
+    <t>Bartender</t>
+  </si>
+  <si>
+    <t>test@mail.edu</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>JR Brewery</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>OtherTxt10</t>
+  </si>
+  <si>
+    <t>OtherTxt11</t>
+  </si>
+  <si>
+    <t>OtherTxt12</t>
+  </si>
+  <si>
+    <t>OtherTxt13</t>
+  </si>
+  <si>
+    <t>OtherTxt14</t>
+  </si>
+  <si>
+    <t>1800</t>
+  </si>
+  <si>
+    <t>19125</t>
+  </si>
+  <si>
+    <t>8008391154</t>
+  </si>
+  <si>
+    <t>8244907</t>
+  </si>
+  <si>
+    <t>632557458</t>
+  </si>
+  <si>
+    <t>04271988</t>
+  </si>
+  <si>
+    <t>C24212_VerifyOneBeneficiary</t>
+  </si>
+  <si>
+    <t>Benny</t>
+  </si>
+  <si>
+    <t>Jacobs</t>
+  </si>
+  <si>
+    <t>Larson</t>
+  </si>
+  <si>
+    <t>3341 45th Ave S</t>
+  </si>
+  <si>
+    <t>55406</t>
+  </si>
+  <si>
+    <t>02221959</t>
+  </si>
+  <si>
+    <t>3352458870</t>
+  </si>
+  <si>
+    <t>MN83jfk9</t>
+  </si>
+  <si>
+    <t>02012018</t>
+  </si>
+  <si>
+    <t>02012028</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>test@mail.com</t>
+  </si>
+  <si>
+    <t>C24295_VerifyMultipleJointOwners</t>
+  </si>
+  <si>
+    <t>ref034857mOt204</t>
+  </si>
+  <si>
+    <t>lid0PQ3</t>
+  </si>
+  <si>
+    <t>11092015</t>
+  </si>
+  <si>
+    <t>03202029</t>
+  </si>
+  <si>
+    <t>2700</t>
+  </si>
+  <si>
+    <t>7200</t>
+  </si>
+  <si>
+    <t>JD Consulting</t>
+  </si>
+  <si>
+    <t>Camilla</t>
+  </si>
+  <si>
+    <t>Blackwell</t>
+  </si>
+  <si>
+    <t>02141981</t>
+  </si>
+  <si>
+    <t>410556879</t>
+  </si>
+  <si>
+    <t>pev893Bh</t>
+  </si>
+  <si>
+    <t>Consultant</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>jo1@gmail.com</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Gene</t>
+  </si>
+  <si>
+    <t>512036698</t>
+  </si>
+  <si>
+    <t>Li8Uyb80</t>
+  </si>
+  <si>
+    <t>jo2@gmail.com</t>
+  </si>
+  <si>
+    <t>4500</t>
+  </si>
+  <si>
+    <t>C24296_VerifyMultipleBeneficiaries</t>
+  </si>
+  <si>
+    <t>Libby</t>
+  </si>
+  <si>
+    <t>Jacobey</t>
+  </si>
+  <si>
+    <t>08141961</t>
+  </si>
+  <si>
+    <t>356997410</t>
+  </si>
+  <si>
+    <t>bene@gmail.com</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>09291972</t>
+  </si>
+  <si>
+    <t>402589874</t>
+  </si>
+  <si>
+    <t>Lef90sl</t>
+  </si>
+  <si>
+    <t>09292018</t>
+  </si>
+  <si>
+    <t>09292029</t>
+  </si>
+  <si>
+    <t>bene2@gmail.com</t>
+  </si>
+  <si>
+    <t>C24299_VerifyJointOwnerAndBeneficiary</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Bremmer</t>
+  </si>
+  <si>
+    <t>04111959</t>
+  </si>
+  <si>
+    <t>299568974</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>VT09329</t>
+  </si>
+  <si>
+    <t>04112010</t>
+  </si>
+  <si>
+    <t>04112025</t>
+  </si>
+  <si>
+    <t>Hart</t>
+  </si>
+  <si>
+    <t>Systems Admin</t>
+  </si>
+  <si>
+    <t>8004567890</t>
+  </si>
+  <si>
+    <t>joEmail@hotmail.com</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>08301989</t>
+  </si>
+  <si>
+    <t>560124578</t>
+  </si>
+  <si>
+    <t>beneEmail@hotmail.com</t>
+  </si>
+  <si>
+    <t>C24300_VerifyModifyJointOwner</t>
+  </si>
+  <si>
+    <t>Business Analyst</t>
+  </si>
+  <si>
+    <t>Gregory</t>
+  </si>
+  <si>
+    <t>o0hH452</t>
+  </si>
+  <si>
+    <t>test@mail.gov</t>
+  </si>
+  <si>
+    <t>8243 Hansen Rd NE</t>
+  </si>
+  <si>
+    <t>Bainbridge Island, WA 98110-1678</t>
+  </si>
+  <si>
+    <t>335245887</t>
+  </si>
+  <si>
+    <t>335-24-5887</t>
+  </si>
+  <si>
+    <t>01012029</t>
+  </si>
+  <si>
+    <t>02/22/1959</t>
+  </si>
+  <si>
+    <t>09/29/2018</t>
+  </si>
+  <si>
+    <t>09/29/2029</t>
+  </si>
+  <si>
+    <t>(800) 839-1154</t>
   </si>
 </sst>
 </file>
@@ -1614,7 +1953,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1631,6 +1970,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1949,7 +2289,7 @@
   <dimension ref="A1:F98"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:D68"/>
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2779,7 +3119,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>8</v>
@@ -2794,7 +3134,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>8</v>
@@ -2809,7 +3149,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>8</v>
@@ -2824,7 +3164,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>8</v>
@@ -2839,7 +3179,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>8</v>
@@ -2854,7 +3194,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>8</v>
@@ -2869,7 +3209,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>8</v>
@@ -2884,7 +3224,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>8</v>
@@ -2899,7 +3239,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>8</v>
@@ -2914,7 +3254,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>8</v>
@@ -2929,7 +3269,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>8</v>
@@ -2944,7 +3284,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>8</v>
@@ -2960,7 +3300,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>8</v>
@@ -2976,7 +3316,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>8</v>
@@ -2990,33 +3330,110 @@
       <c r="F68" s="1"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B69" s="4"/>
+      <c r="A69" t="s">
+        <v>513</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B70" s="4"/>
+      <c r="A70" t="s">
+        <v>515</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B71" s="4"/>
+      <c r="A71" t="s">
+        <v>545</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E71" s="2"/>
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B72" s="4"/>
+      <c r="A72" t="s">
+        <v>558</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E72" s="2"/>
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B73" s="4"/>
+      <c r="A73" t="s">
+        <v>580</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B74" s="4"/>
+      <c r="A74" t="s">
+        <v>594</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B75" s="4"/>
+      <c r="A75" t="s">
+        <v>611</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -3189,19 +3606,26 @@
     <hyperlink ref="B66" r:id="rId65"/>
     <hyperlink ref="B67" r:id="rId66"/>
     <hyperlink ref="B68" r:id="rId67"/>
+    <hyperlink ref="B69" r:id="rId68"/>
+    <hyperlink ref="B70" r:id="rId69"/>
+    <hyperlink ref="B71" r:id="rId70"/>
+    <hyperlink ref="B72" r:id="rId71"/>
+    <hyperlink ref="B73" r:id="rId72"/>
+    <hyperlink ref="B74" r:id="rId73"/>
+    <hyperlink ref="B75" r:id="rId74"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId68"/>
+  <pageSetup orientation="portrait" r:id="rId75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM68"/>
+  <dimension ref="A1:AR75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z75" sqref="Z75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3225,12 +3649,15 @@
     <col min="21" max="21" width="15.7109375" style="6" customWidth="1"/>
     <col min="22" max="22" width="18.42578125" style="6" customWidth="1"/>
     <col min="23" max="23" width="14.140625" style="6" customWidth="1"/>
-    <col min="24" max="30" width="9.140625" style="6"/>
+    <col min="24" max="24" width="10.85546875" style="6" customWidth="1"/>
+    <col min="25" max="25" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="9.140625" style="6"/>
     <col min="31" max="31" width="35.5703125" style="6" customWidth="1"/>
     <col min="32" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3348,8 +3775,23 @@
       <c r="AM1" s="3" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="2" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN1" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>29</v>
       </c>
@@ -3396,23 +3838,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>162</v>
@@ -3481,13 +3923,13 @@
         <v>157</v>
       </c>
       <c r="AB4" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC4" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD4" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="AC4" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD4" s="12" t="s">
-        <v>446</v>
       </c>
       <c r="AE4" s="11" t="s">
         <v>160</v>
@@ -3496,13 +3938,10 @@
         <v>161</v>
       </c>
       <c r="AG4" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="AH4" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>43</v>
       </c>
@@ -3582,13 +4021,13 @@
         <v>169</v>
       </c>
       <c r="AB5" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC5" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD5" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC5" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD5" s="12" t="s">
-        <v>456</v>
       </c>
       <c r="AE5" s="11" t="s">
         <v>151</v>
@@ -3600,7 +4039,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>58</v>
       </c>
@@ -3628,6 +4067,9 @@
       <c r="I6" s="6" t="s">
         <v>66</v>
       </c>
+      <c r="J6" s="6" t="s">
+        <v>449</v>
+      </c>
       <c r="K6" s="6" t="s">
         <v>172</v>
       </c>
@@ -3680,13 +4122,13 @@
         <v>146</v>
       </c>
       <c r="AB6" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC6" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD6" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="AC6" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD6" s="12" t="s">
-        <v>446</v>
       </c>
       <c r="AE6" s="11" t="s">
         <v>147</v>
@@ -3716,7 +4158,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>100</v>
       </c>
@@ -3742,13 +4184,13 @@
         <v>178</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>44</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="L7" s="6">
         <v>500</v>
@@ -3792,20 +4234,16 @@
       <c r="Y7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="Z7" s="11" t="s">
-        <v>302</v>
-      </c>
-      <c r="AA7" s="11" t="s">
-        <v>457</v>
-      </c>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
       <c r="AB7" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC7" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD7" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC7" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD7" s="12" t="s">
-        <v>456</v>
       </c>
       <c r="AE7" s="11" t="s">
         <v>167</v>
@@ -3826,10 +4264,10 @@
         <v>170</v>
       </c>
       <c r="AK7" s="11" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>101</v>
       </c>
@@ -3848,8 +4286,11 @@
       <c r="F8" s="6" t="s">
         <v>113</v>
       </c>
+      <c r="G8" s="6" t="s">
+        <v>511</v>
+      </c>
       <c r="P8" s="6" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>105</v>
@@ -3861,7 +4302,7 @@
         <v>107</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="U8" s="6" t="s">
         <v>108</v>
@@ -3872,8 +4313,11 @@
       <c r="Y8" s="6" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="Z8" s="6" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>180</v>
       </c>
@@ -3884,12 +4328,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>183</v>
       </c>
@@ -3900,7 +4344,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>186</v>
       </c>
@@ -3914,7 +4358,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>241</v>
       </c>
@@ -3922,7 +4366,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>187</v>
       </c>
@@ -3939,21 +4383,24 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>239</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>240</v>
       </c>
+      <c r="G15" s="6" t="s">
+        <v>511</v>
+      </c>
       <c r="H15" s="6" t="s">
         <v>111</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>188</v>
       </c>
@@ -4000,13 +4447,13 @@
         <v>161</v>
       </c>
       <c r="AB16" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC16" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD16" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="AC16" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD16" s="12" t="s">
-        <v>446</v>
       </c>
       <c r="AE16" s="11" t="s">
         <v>189</v>
@@ -4023,13 +4470,13 @@
         <v>104</v>
       </c>
       <c r="AB17" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC17" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD17" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC17" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD17" s="12" t="s">
-        <v>456</v>
       </c>
       <c r="AE17" s="6" t="s">
         <v>191</v>
@@ -4091,10 +4538,10 @@
         <v>161</v>
       </c>
       <c r="AB18" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="AC18" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="AD18" s="12" t="s">
         <v>159</v>
@@ -4108,13 +4555,13 @@
         <v>195</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>162</v>
@@ -4169,7 +4616,7 @@
         <v>205</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="G21" s="6">
         <v>99999</v>
@@ -4548,6 +4995,9 @@
       <c r="I28" s="6" t="s">
         <v>66</v>
       </c>
+      <c r="J28" s="6" t="s">
+        <v>449</v>
+      </c>
       <c r="L28" s="6">
         <v>5000</v>
       </c>
@@ -4592,24 +5042,27 @@
         <v>274</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="F30" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="G30" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="H30" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="I30" s="6" t="s">
         <v>66</v>
       </c>
       <c r="L30" s="6">
@@ -4644,6 +5097,9 @@
       </c>
       <c r="AH30" s="6" t="s">
         <v>282</v>
+      </c>
+      <c r="AI30" s="6" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
@@ -4692,13 +5148,13 @@
         <v>285</v>
       </c>
       <c r="AB32" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC32" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD32" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC32" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD32" s="12" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
@@ -4721,13 +5177,13 @@
         <v>294</v>
       </c>
       <c r="AB33" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC33" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD33" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="AC33" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD33" s="12" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
@@ -4765,13 +5221,13 @@
         <v>206</v>
       </c>
       <c r="AB34" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC34" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD34" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC34" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD34" s="12" t="s">
-        <v>456</v>
       </c>
       <c r="AE34" s="6" t="s">
         <v>18</v>
@@ -4818,13 +5274,13 @@
         <v>301</v>
       </c>
       <c r="AB35" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC35" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD35" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="AC35" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD35" s="12" t="s">
-        <v>446</v>
       </c>
       <c r="AF35" s="11"/>
       <c r="AG35" s="11"/>
@@ -4847,13 +5303,13 @@
         <v>311</v>
       </c>
       <c r="AB36" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC36" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD36" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC36" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD36" s="12" t="s">
-        <v>456</v>
       </c>
       <c r="AF36" s="11"/>
       <c r="AG36" s="11"/>
@@ -4906,13 +5362,13 @@
         <v>206</v>
       </c>
       <c r="AB37" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC37" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD37" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="AC37" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD37" s="12" t="s">
-        <v>446</v>
       </c>
       <c r="AE37" s="6" t="s">
         <v>18</v>
@@ -4959,10 +5415,10 @@
         <v>301</v>
       </c>
       <c r="AB38" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="AC38" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="AD38" s="12" t="s">
         <v>159</v>
@@ -4994,13 +5450,13 @@
         <v>206</v>
       </c>
       <c r="AB39" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC39" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD39" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC39" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD39" s="12" t="s">
-        <v>456</v>
       </c>
       <c r="AE39" s="6" t="s">
         <v>18</v>
@@ -5050,13 +5506,13 @@
         <v>335</v>
       </c>
       <c r="AB40" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC40" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD40" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="AC40" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD40" s="12" t="s">
-        <v>446</v>
       </c>
       <c r="AE40" s="6" t="s">
         <v>18</v>
@@ -5121,10 +5577,10 @@
         <v>206</v>
       </c>
       <c r="AB41" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="AC41" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="AD41" s="12" t="s">
         <v>159</v>
@@ -5174,13 +5630,13 @@
         <v>301</v>
       </c>
       <c r="AB42" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC42" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD42" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC42" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD42" s="12" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
@@ -5230,13 +5686,13 @@
         <v>358</v>
       </c>
       <c r="AB43" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC43" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD43" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="AC43" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD43" s="12" t="s">
-        <v>446</v>
       </c>
       <c r="AE43" s="11" t="s">
         <v>361</v>
@@ -5265,10 +5721,10 @@
         <v>219</v>
       </c>
       <c r="AB44" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="AC44" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="AD44" s="12" t="s">
         <v>159</v>
@@ -5281,26 +5737,26 @@
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
       <c r="Q45" s="6" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="S45" s="10" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="T45" s="10"/>
       <c r="U45" s="6" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="V45" s="6" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="AB45" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC45" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD45" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC45" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD45" s="12" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.25">
@@ -5320,13 +5776,13 @@
         <v>372</v>
       </c>
       <c r="AB46" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC46" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD46" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="AC46" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD46" s="12" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.25">
@@ -5337,16 +5793,16 @@
         <v>100000</v>
       </c>
       <c r="AB47" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="AC47" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="AD47" s="12" t="s">
         <v>159</v>
       </c>
       <c r="AE47" s="11" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="AF47" s="11" t="s">
         <v>375</v>
@@ -5372,13 +5828,13 @@
         <v>380</v>
       </c>
       <c r="AB48" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC48" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD48" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC48" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD48" s="12" t="s">
-        <v>456</v>
       </c>
       <c r="AE48" s="11" t="s">
         <v>383</v>
@@ -5398,13 +5854,13 @@
         <v>384</v>
       </c>
       <c r="AB49" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC49" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD49" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="AC49" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD49" s="12" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="50" spans="1:37" x14ac:dyDescent="0.25">
@@ -5412,13 +5868,13 @@
         <v>385</v>
       </c>
       <c r="AB50" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC50" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD50" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC50" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD50" s="12" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="51" spans="1:37" x14ac:dyDescent="0.25">
@@ -5467,10 +5923,10 @@
       <c r="Z51" s="11"/>
       <c r="AA51" s="11"/>
       <c r="AB51" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="AC51" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="AD51" s="12" t="s">
         <v>159</v>
@@ -5526,19 +5982,19 @@
         <v>173</v>
       </c>
       <c r="AB52" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC52" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD52" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="AC52" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD52" s="12" t="s">
-        <v>446</v>
-      </c>
       <c r="AE52" s="11" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="AF52" s="11" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="AG52" s="11" t="s">
         <v>399</v>
@@ -5567,19 +6023,19 @@
         <v>184</v>
       </c>
       <c r="AB53" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC53" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD53" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="AC53" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD53" s="12" t="s">
-        <v>456</v>
-      </c>
       <c r="AE53" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="AF53" s="11" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="54" spans="1:37" x14ac:dyDescent="0.25">
@@ -5593,7 +6049,7 @@
         <v>173</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>406</v>
+        <v>506</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>102</v>
@@ -5605,22 +6061,25 @@
         <v>111</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>405</v>
+        <v>509</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>511</v>
       </c>
       <c r="AB54" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="AC54" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="AD54" s="12" t="s">
         <v>159</v>
       </c>
       <c r="AE54" s="11" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="AF54" s="11" t="s">
         <v>375</v>
@@ -5628,7 +6087,7 @@
     </row>
     <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>49</v>
@@ -5643,43 +6102,43 @@
         <v>16000</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J55" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="K55" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="K55" s="6" t="s">
-        <v>418</v>
-      </c>
       <c r="L55" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="M55" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="M55" s="6" t="s">
+      <c r="N55" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="N55" s="6" t="s">
+      <c r="O55" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="O55" s="6" t="s">
+      <c r="P55" s="6" t="s">
         <v>423</v>
-      </c>
-      <c r="P55" s="6" t="s">
-        <v>424</v>
       </c>
       <c r="Q55" s="6" t="s">
         <v>18</v>
       </c>
       <c r="R55" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="S55" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="S55" s="11" t="s">
+      <c r="T55" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="T55" s="11" t="s">
+      <c r="U55" s="11" t="s">
         <v>412</v>
-      </c>
-      <c r="U55" s="11" t="s">
-        <v>413</v>
       </c>
       <c r="V55" s="11" t="s">
         <v>150</v>
@@ -5688,51 +6147,51 @@
         <v>303</v>
       </c>
       <c r="X55" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="Y55" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="Z55" s="11" t="s">
         <v>414</v>
-      </c>
-      <c r="Y55" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="Z55" s="11" t="s">
-        <v>415</v>
       </c>
       <c r="AA55" s="11" t="s">
         <v>167</v>
       </c>
       <c r="AB55" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC55" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD55" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="AC55" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD55" s="12" t="s">
-        <v>446</v>
-      </c>
       <c r="AE55" s="11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AF55" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="AG55" s="11" t="s">
         <v>425</v>
       </c>
-      <c r="AG55" s="11" t="s">
+      <c r="AH55" s="11" t="s">
         <v>426</v>
       </c>
-      <c r="AH55" s="11" t="s">
+      <c r="AI55" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="AI55" s="11" t="s">
+      <c r="AJ55" s="11" t="s">
         <v>428</v>
       </c>
-      <c r="AJ55" s="11" t="s">
+      <c r="AK55" s="11" t="s">
         <v>429</v>
-      </c>
-      <c r="AK55" s="11" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>62</v>
@@ -5762,10 +6221,10 @@
         <v>170</v>
       </c>
       <c r="X56" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="Y56" s="11" t="s">
         <v>432</v>
-      </c>
-      <c r="Y56" s="11" t="s">
-        <v>433</v>
       </c>
       <c r="Z56" s="11" t="s">
         <v>160</v>
@@ -5774,18 +6233,18 @@
         <v>322</v>
       </c>
       <c r="AB56" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC56" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD56" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC56" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD56" s="12" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>51</v>
@@ -5797,7 +6256,7 @@
         <v>222222</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Q57" s="6" t="s">
         <v>18</v>
@@ -5821,20 +6280,20 @@
         <v>308</v>
       </c>
       <c r="X57" s="11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="Y57" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Z57" s="11" t="s">
         <v>174</v>
       </c>
       <c r="AA57" s="11"/>
       <c r="AB57" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="AC57" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="AD57" s="12" t="s">
         <v>159</v>
@@ -5842,51 +6301,51 @@
     </row>
     <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>176</v>
       </c>
       <c r="C58" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="H58" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="G58" s="6" t="s">
+      <c r="I58" s="6" t="s">
         <v>440</v>
       </c>
-      <c r="H58" s="6" t="s">
+      <c r="J58" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="I58" s="6" t="s">
+      <c r="AB58" s="12" t="s">
         <v>442</v>
       </c>
-      <c r="J58" s="6" t="s">
+      <c r="AC58" s="12" t="s">
         <v>443</v>
       </c>
-      <c r="AB58" s="12" t="s">
+      <c r="AD58" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="AC58" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD58" s="12" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G59" s="6">
         <v>2500</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="Q59" s="6" t="s">
         <v>18</v>
@@ -5895,13 +6354,13 @@
         <v>146</v>
       </c>
       <c r="S59" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="T59" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U59" s="11" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="V59" s="11" t="s">
         <v>167</v>
@@ -5910,7 +6369,7 @@
         <v>151</v>
       </c>
       <c r="X59" s="11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="Y59" s="11" t="s">
         <v>169</v>
@@ -5922,66 +6381,66 @@
         <v>161</v>
       </c>
       <c r="AB59" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC59" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD59" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC59" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD59" s="12" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B60" s="11" t="s">
         <v>177</v>
       </c>
       <c r="G60" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="J60" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="L60" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="M60" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="N60" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="O60" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="P60" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="Q60" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="R60" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="H60" s="6" t="s">
-        <v>461</v>
-      </c>
-      <c r="I60" s="6" t="s">
-        <v>452</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>464</v>
-      </c>
-      <c r="K60" s="6" t="s">
-        <v>465</v>
-      </c>
-      <c r="L60" s="6" t="s">
-        <v>466</v>
-      </c>
-      <c r="M60" s="6" t="s">
-        <v>467</v>
-      </c>
-      <c r="N60" s="6" t="s">
+      <c r="S60" s="11" t="s">
         <v>468</v>
       </c>
-      <c r="O60" s="6" t="s">
-        <v>469</v>
-      </c>
-      <c r="P60" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="Q60" s="6" t="s">
-        <v>462</v>
-      </c>
-      <c r="R60" s="11" t="s">
-        <v>463</v>
-      </c>
-      <c r="S60" s="11" t="s">
-        <v>471</v>
-      </c>
       <c r="AB60" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="AC60" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="AD60" s="12" t="s">
         <v>159</v>
@@ -5989,19 +6448,19 @@
     </row>
     <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>102</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="G61" s="6">
         <v>1000</v>
@@ -6013,27 +6472,27 @@
         <v>189</v>
       </c>
       <c r="AB61" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC61" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD61" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="AC61" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD61" s="12" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>220</v>
@@ -6051,18 +6510,18 @@
         <v>50000</v>
       </c>
       <c r="AB62" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC62" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD62" s="12" t="s">
         <v>454</v>
-      </c>
-      <c r="AC62" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD62" s="12" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>102</v>
@@ -6071,7 +6530,7 @@
         <v>191</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I63" s="6" t="s">
         <v>189</v>
@@ -6086,10 +6545,10 @@
         <v>1000</v>
       </c>
       <c r="AB63" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="AC63" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="AD63" s="12" t="s">
         <v>159</v>
@@ -6097,7 +6556,7 @@
     </row>
     <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B64" s="11" t="s">
         <v>103</v>
@@ -6106,27 +6565,27 @@
         <v>228</v>
       </c>
       <c r="AB64" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC64" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD64" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="AC64" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD64" s="12" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>171</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I65" s="6" t="s">
         <v>189</v>
@@ -6141,30 +6600,30 @@
         <v>2500</v>
       </c>
       <c r="AB65" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC65" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD65" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="AC65" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD65" s="12" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>102</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H66" s="6" t="s">
         <v>245</v>
@@ -6173,33 +6632,33 @@
         <v>10</v>
       </c>
       <c r="AB66" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="AC66" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="AD66" s="12" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B67" s="11" t="s">
         <v>161</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>102</v>
       </c>
       <c r="E67" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="G67" s="6" t="s">
         <v>486</v>
-      </c>
-      <c r="G67" s="6" t="s">
-        <v>489</v>
       </c>
       <c r="L67" s="6">
         <v>99999</v>
@@ -6208,27 +6667,27 @@
         <v>2000</v>
       </c>
       <c r="AB67" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC67" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD67" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="AC67" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="AD67" s="12" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B68" s="11" t="s">
         <v>178</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G68" s="6">
         <v>1500</v>
@@ -6237,13 +6696,549 @@
         <v>196</v>
       </c>
       <c r="AB68" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC68" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD68" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="AC68" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="AD68" s="12" t="s">
-        <v>456</v>
+    </row>
+    <row r="69" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="AB69" s="12" t="s">
+        <v>495</v>
+      </c>
+      <c r="AC69" s="12" t="s">
+        <v>496</v>
+      </c>
+      <c r="AD69" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="70" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="B70" s="6">
+        <v>100000</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="H70" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I70" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="J70" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="K70" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="L70" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="M70" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="N70" s="11" t="s">
+        <v>519</v>
+      </c>
+      <c r="O70" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="P70" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="Q70" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="R70" s="11" t="s">
+        <v>540</v>
+      </c>
+      <c r="S70" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="T70" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="U70" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="V70" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="W70" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="X70" s="11" t="s">
+        <v>528</v>
+      </c>
+      <c r="Y70" s="11" t="s">
+        <v>529</v>
+      </c>
+      <c r="Z70" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="AA70" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="AB70" s="12" t="s">
+        <v>542</v>
+      </c>
+      <c r="AC70" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="AD70" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="AE70" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="AF70" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="AG70" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="AH70" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="AI70" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ70" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="AK70" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="AL70" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="AM70" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="AN70" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="AO70" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="AP70" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="AQ70" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="AR70" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="71" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="L71" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="M71" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="N71" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="O71" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="P71" s="11" t="s">
+        <v>550</v>
+      </c>
+      <c r="Q71" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="R71" s="11" t="s">
+        <v>552</v>
+      </c>
+      <c r="S71" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="T71" s="11" t="s">
+        <v>553</v>
+      </c>
+      <c r="U71" s="11" t="s">
+        <v>554</v>
+      </c>
+      <c r="V71" s="11" t="s">
+        <v>555</v>
+      </c>
+      <c r="W71" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="X71" s="11" t="s">
+        <v>556</v>
+      </c>
+      <c r="Y71" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="AB71" s="11" t="s">
+        <v>516</v>
+      </c>
+      <c r="AC71" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="AD71" s="11" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="72" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="B72" s="6">
+        <v>1234.56</v>
+      </c>
+      <c r="C72" s="14">
+        <v>2789</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G72" s="11" t="s">
+        <v>561</v>
+      </c>
+      <c r="H72" s="11" t="s">
+        <v>562</v>
+      </c>
+      <c r="I72" s="11" t="s">
+        <v>563</v>
+      </c>
+      <c r="J72" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K72" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="L72" s="11" t="s">
+        <v>564</v>
+      </c>
+      <c r="M72" s="11" t="s">
+        <v>566</v>
+      </c>
+      <c r="N72" s="11" t="s">
+        <v>567</v>
+      </c>
+      <c r="O72" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="P72" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="Q72" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="R72" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="S72" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="T72" s="11" t="s">
+        <v>572</v>
+      </c>
+      <c r="U72" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="V72" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="W72" s="11" t="s">
+        <v>574</v>
+      </c>
+      <c r="X72" s="11" t="s">
+        <v>575</v>
+      </c>
+      <c r="Y72" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="Z72" s="11" t="s">
+        <v>550</v>
+      </c>
+      <c r="AA72" s="11" t="s">
+        <v>576</v>
+      </c>
+      <c r="AB72" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC72" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD72" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="AE72" s="11" t="s">
+        <v>577</v>
+      </c>
+      <c r="AF72" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="AG72" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="AH72" s="11" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="73" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>581</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>582</v>
+      </c>
+      <c r="I73" s="11" t="s">
+        <v>583</v>
+      </c>
+      <c r="J73" s="11" t="s">
+        <v>584</v>
+      </c>
+      <c r="K73" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="L73" s="11" t="s">
+        <v>572</v>
+      </c>
+      <c r="M73" s="6" t="s">
+        <v>585</v>
+      </c>
+      <c r="N73" s="11" t="s">
+        <v>586</v>
+      </c>
+      <c r="O73" s="11" t="s">
+        <v>587</v>
+      </c>
+      <c r="P73" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="Q73" s="11" t="s">
+        <v>540</v>
+      </c>
+      <c r="R73" s="11" t="s">
+        <v>588</v>
+      </c>
+      <c r="S73" s="11" t="s">
+        <v>589</v>
+      </c>
+      <c r="T73" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="U73" s="11" t="s">
+        <v>590</v>
+      </c>
+      <c r="V73" s="11" t="s">
+        <v>591</v>
+      </c>
+      <c r="W73" s="11" t="s">
+        <v>592</v>
+      </c>
+      <c r="X73" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="AB73" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC73" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD73" s="12" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="74" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>594</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>595</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>596</v>
+      </c>
+      <c r="I74" s="11" t="s">
+        <v>597</v>
+      </c>
+      <c r="J74" s="11" t="s">
+        <v>598</v>
+      </c>
+      <c r="K74" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="L74" s="11" t="s">
+        <v>599</v>
+      </c>
+      <c r="M74" s="11" t="s">
+        <v>600</v>
+      </c>
+      <c r="N74" s="11" t="s">
+        <v>601</v>
+      </c>
+      <c r="O74" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="P74" s="11" t="s">
+        <v>603</v>
+      </c>
+      <c r="Q74" s="11" t="s">
+        <v>604</v>
+      </c>
+      <c r="R74" s="11" t="s">
+        <v>605</v>
+      </c>
+      <c r="S74" s="11" t="s">
+        <v>556</v>
+      </c>
+      <c r="T74" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="U74" s="11" t="s">
+        <v>607</v>
+      </c>
+      <c r="V74" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="W74" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="X74" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="AB74" s="12" t="s">
+        <v>542</v>
+      </c>
+      <c r="AC74" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="AD74" s="12" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="75" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="I75" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="J75" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="K75" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="L75" s="11" t="s">
+        <v>590</v>
+      </c>
+      <c r="M75" s="11" t="s">
+        <v>591</v>
+      </c>
+      <c r="N75" s="11" t="s">
+        <v>592</v>
+      </c>
+      <c r="O75" s="11" t="s">
+        <v>528</v>
+      </c>
+      <c r="P75" s="11" t="s">
+        <v>612</v>
+      </c>
+      <c r="Q75" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="R75" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="S75" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="T75" s="11" t="s">
+        <v>616</v>
+      </c>
+      <c r="U75" s="11" t="s">
+        <v>617</v>
+      </c>
+      <c r="V75" s="11" t="s">
+        <v>621</v>
+      </c>
+      <c r="W75" s="11" t="s">
+        <v>619</v>
+      </c>
+      <c r="X75" s="11" t="s">
+        <v>622</v>
+      </c>
+      <c r="Y75" s="11" t="s">
+        <v>623</v>
+      </c>
+      <c r="Z75" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="AB75" s="11" t="s">
+        <v>516</v>
+      </c>
+      <c r="AC75" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="AD75" s="11" t="s">
+        <v>518</v>
+      </c>
+      <c r="AE75" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="AF75" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG75" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="AH75" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="AI75" s="6" t="s">
+        <v>615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ädded new scripts for Progress bar validation as part of Existing member of InstantOpen
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrown\TDECUWorkspace\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474F77CF-BA0E-410B-8BB5-DDEB3E71DFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="682">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -2066,12 +2067,18 @@
   </si>
   <si>
     <t>If the Member#/SSN/DOB is changed, other test data will need to be updated for these test cases</t>
+  </si>
+  <si>
+    <t>C28336_VerifyInformationProgressBarHighlightedOnMemberVerificationPage</t>
+  </si>
+  <si>
+    <t>C28337_VerifyInformationProgressBarHighlightedOnExistingApplicantPage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2448,16 +2455,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88:D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="71.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -3786,12 +3793,34 @@
       <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B88" s="4"/>
+      <c r="A88" t="s">
+        <v>680</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="E88" s="2"/>
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B89" s="4"/>
+      <c r="A89" t="s">
+        <v>681</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="E89" s="2"/>
       <c r="F89" s="1"/>
     </row>
@@ -3834,105 +3863,107 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B14" r:id="rId12"/>
-    <hyperlink ref="B16" r:id="rId13"/>
-    <hyperlink ref="B17" r:id="rId14"/>
-    <hyperlink ref="B18" r:id="rId15"/>
-    <hyperlink ref="B19" r:id="rId16"/>
-    <hyperlink ref="B20" r:id="rId17"/>
-    <hyperlink ref="B21" r:id="rId18"/>
-    <hyperlink ref="B22" r:id="rId19"/>
-    <hyperlink ref="B23" r:id="rId20"/>
-    <hyperlink ref="B24" r:id="rId21"/>
-    <hyperlink ref="B15" r:id="rId22"/>
-    <hyperlink ref="B13" r:id="rId23"/>
-    <hyperlink ref="B25" r:id="rId24"/>
-    <hyperlink ref="B26" r:id="rId25"/>
-    <hyperlink ref="B27" r:id="rId26"/>
-    <hyperlink ref="B28" r:id="rId27"/>
-    <hyperlink ref="B29" r:id="rId28"/>
-    <hyperlink ref="B30" r:id="rId29"/>
-    <hyperlink ref="B31" r:id="rId30"/>
-    <hyperlink ref="B32" r:id="rId31"/>
-    <hyperlink ref="B33" r:id="rId32"/>
-    <hyperlink ref="B34" r:id="rId33"/>
-    <hyperlink ref="B35" r:id="rId34"/>
-    <hyperlink ref="B36" r:id="rId35"/>
-    <hyperlink ref="B37" r:id="rId36"/>
-    <hyperlink ref="B38" r:id="rId37"/>
-    <hyperlink ref="B39" r:id="rId38"/>
-    <hyperlink ref="B40" r:id="rId39"/>
-    <hyperlink ref="B41" r:id="rId40"/>
-    <hyperlink ref="B42" r:id="rId41"/>
-    <hyperlink ref="B43" r:id="rId42"/>
-    <hyperlink ref="B44" r:id="rId43"/>
-    <hyperlink ref="B45" r:id="rId44"/>
-    <hyperlink ref="B46" r:id="rId45"/>
-    <hyperlink ref="B47" r:id="rId46"/>
-    <hyperlink ref="B48" r:id="rId47"/>
-    <hyperlink ref="B49" r:id="rId48"/>
-    <hyperlink ref="B50" r:id="rId49"/>
-    <hyperlink ref="B51" r:id="rId50"/>
-    <hyperlink ref="B52" r:id="rId51"/>
-    <hyperlink ref="B53" r:id="rId52"/>
-    <hyperlink ref="B54" r:id="rId53"/>
-    <hyperlink ref="B55" r:id="rId54"/>
-    <hyperlink ref="B56" r:id="rId55"/>
-    <hyperlink ref="B57" r:id="rId56"/>
-    <hyperlink ref="B58" r:id="rId57"/>
-    <hyperlink ref="B59" r:id="rId58"/>
-    <hyperlink ref="B60" r:id="rId59"/>
-    <hyperlink ref="B61" r:id="rId60"/>
-    <hyperlink ref="B62" r:id="rId61"/>
-    <hyperlink ref="B63" r:id="rId62"/>
-    <hyperlink ref="B64" r:id="rId63"/>
-    <hyperlink ref="B65" r:id="rId64"/>
-    <hyperlink ref="B66" r:id="rId65"/>
-    <hyperlink ref="B67" r:id="rId66"/>
-    <hyperlink ref="B68" r:id="rId67"/>
-    <hyperlink ref="B69" r:id="rId68"/>
-    <hyperlink ref="B70" r:id="rId69"/>
-    <hyperlink ref="B71" r:id="rId70"/>
-    <hyperlink ref="B72" r:id="rId71"/>
-    <hyperlink ref="B73" r:id="rId72"/>
-    <hyperlink ref="B74" r:id="rId73"/>
-    <hyperlink ref="B75" r:id="rId74"/>
-    <hyperlink ref="B76" r:id="rId75"/>
-    <hyperlink ref="B77" r:id="rId76"/>
-    <hyperlink ref="B78" r:id="rId77"/>
-    <hyperlink ref="B79" r:id="rId78"/>
-    <hyperlink ref="B80" r:id="rId79"/>
-    <hyperlink ref="B81" r:id="rId80"/>
-    <hyperlink ref="B82" r:id="rId81"/>
-    <hyperlink ref="B83" r:id="rId82"/>
-    <hyperlink ref="B84" r:id="rId83"/>
-    <hyperlink ref="B85" r:id="rId84"/>
-    <hyperlink ref="B86" r:id="rId85"/>
-    <hyperlink ref="B87" r:id="rId86"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B15" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B13" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B88" r:id="rId87" xr:uid="{84D3A13C-89C8-4A21-B216-8750F5B20EB3}"/>
+    <hyperlink ref="B89" r:id="rId88" xr:uid="{464E9C1B-8CF7-4594-B0AB-B4C52BC5A953}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId87"/>
+  <pageSetup orientation="portrait" r:id="rId89"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AR87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E62" sqref="E62"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8251,7 +8282,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Modified existing scripts with PromoCode steps
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474F77CF-BA0E-410B-8BB5-DDEB3E71DFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA91D1E-B8B4-4AB0-B498-E2863BC7559C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="ProdData" sheetId="6" r:id="rId2"/>
-    <sheet name="Notes" sheetId="7" r:id="rId3"/>
+    <sheet name="MemberVerification" sheetId="8" r:id="rId3"/>
+    <sheet name="Notes" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="693">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -2073,6 +2074,39 @@
   </si>
   <si>
     <t>C28337_VerifyInformationProgressBarHighlightedOnExistingApplicantPage</t>
+  </si>
+  <si>
+    <t>C28347_VerifyProductsProgressBarHighlightedWhenOnSelectProductPage</t>
+  </si>
+  <si>
+    <t>C28346_VerifyInformationProgressBarHighLightedOnceInCreditCardInfoScreen</t>
+  </si>
+  <si>
+    <t>C238348_VerifyInformationProgressBarHighlightedUnderPersonalLoanSection</t>
+  </si>
+  <si>
+    <t>C28349_VerifyInformationprogressBarHighlightedOnVehicleInfoPage</t>
+  </si>
+  <si>
+    <t>C28338_UpdateTheDesignOfTheMemberVerificationScreen</t>
+  </si>
+  <si>
+    <t>C28370_ValidateSocialSecurityNoAndDOB</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>765437896</t>
+  </si>
+  <si>
+    <t>2/1/1960</t>
+  </si>
+  <si>
+    <t>C28371_ValidateDeliveryMethodForOneTimePassWord</t>
+  </si>
+  <si>
+    <t>02/01/1960</t>
   </si>
 </sst>
 </file>
@@ -2125,7 +2159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2141,6 +2175,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2458,8 +2493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88:D89"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95:D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3825,32 +3860,109 @@
       <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B90" s="4"/>
+      <c r="A90" t="s">
+        <v>682</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="E90" s="2"/>
       <c r="F90" s="1"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B91" s="4"/>
+      <c r="A91" t="s">
+        <v>683</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B92" s="4"/>
+      <c r="A92" t="s">
+        <v>684</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="F92" s="1"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B93" s="4"/>
+      <c r="A93" t="s">
+        <v>685</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B94" s="4"/>
+      <c r="A94" t="s">
+        <v>686</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B95" s="4"/>
+      <c r="A95" t="s">
+        <v>687</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B96" s="4"/>
+      <c r="A96" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="F96" s="1"/>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
@@ -3951,9 +4063,16 @@
     <hyperlink ref="B87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
     <hyperlink ref="B88" r:id="rId87" xr:uid="{84D3A13C-89C8-4A21-B216-8750F5B20EB3}"/>
     <hyperlink ref="B89" r:id="rId88" xr:uid="{464E9C1B-8CF7-4594-B0AB-B4C52BC5A953}"/>
+    <hyperlink ref="B90" r:id="rId89" xr:uid="{86B44990-3E55-42DE-9E90-332022DD739F}"/>
+    <hyperlink ref="B91" r:id="rId90" xr:uid="{DC3101AA-7029-4716-9408-5E3AB2E260D0}"/>
+    <hyperlink ref="B92" r:id="rId91" xr:uid="{433A11DB-A693-4326-9FC1-8EC0B8E9DE34}"/>
+    <hyperlink ref="B93" r:id="rId92" xr:uid="{9E97E79D-DBAD-4ACF-85A7-87C9ECC52E71}"/>
+    <hyperlink ref="B94" r:id="rId93" xr:uid="{D85BB755-7835-4701-8C59-33C0B6F9ED22}"/>
+    <hyperlink ref="B95" r:id="rId94" xr:uid="{0823C41D-A814-4C8B-AFB0-FCA64A53B4EB}"/>
+    <hyperlink ref="B96" r:id="rId95" xr:uid="{F6C44DA2-84C9-4B29-86CF-AD658211A5AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId89"/>
+  <pageSetup orientation="portrait" r:id="rId96"/>
 </worksheet>
 </file>
 
@@ -3961,9 +4080,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AR87"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE12" sqref="AE12"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8282,6 +8401,59 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7A3FC5-D09A-4697-BB1A-908D46717259}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>687</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>691</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>692</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Ädded new script with OTP fetching code from mail
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA91D1E-B8B4-4AB0-B498-E2863BC7559C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02F9E11-FA66-46A1-A74B-59A2CADD8C74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1733" uniqueCount="702">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -2107,6 +2107,33 @@
   </si>
   <si>
     <t>02/01/1960</t>
+  </si>
+  <si>
+    <t>C28329_ValidateUserCanAddPromotionalCodeToTheConfirmAccount</t>
+  </si>
+  <si>
+    <t>046202574</t>
+  </si>
+  <si>
+    <t>02141994</t>
+  </si>
+  <si>
+    <t>PromoCode</t>
+  </si>
+  <si>
+    <t>BankRate</t>
+  </si>
+  <si>
+    <t>C28338_VerifyThatInformationTabIsHighLightedWhenUserInJointOwnerPage</t>
+  </si>
+  <si>
+    <t>02011960</t>
+  </si>
+  <si>
+    <t>C28341_VerifyThatInformationTabIsHighLightedWhenUserInJointOwnerLookupPage</t>
+  </si>
+  <si>
+    <t>C28344_VerifyThatInformationTabIsHighLightedWhenUserInBeneficiariesPage</t>
   </si>
 </sst>
 </file>
@@ -2159,7 +2186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2176,6 +2203,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2491,10 +2521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95:D96"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99:D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3965,13 +3995,63 @@
       </c>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" s="4"/>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>693</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B98" s="4"/>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="F98" s="1"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>700</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>701</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4070,25 +4150,29 @@
     <hyperlink ref="B94" r:id="rId93" xr:uid="{D85BB755-7835-4701-8C59-33C0B6F9ED22}"/>
     <hyperlink ref="B95" r:id="rId94" xr:uid="{0823C41D-A814-4C8B-AFB0-FCA64A53B4EB}"/>
     <hyperlink ref="B96" r:id="rId95" xr:uid="{F6C44DA2-84C9-4B29-86CF-AD658211A5AA}"/>
+    <hyperlink ref="B97" r:id="rId96" xr:uid="{9D794C44-7EDC-4FFC-BFE8-BC12442D1CC8}"/>
+    <hyperlink ref="B98" r:id="rId97" xr:uid="{A549EE0A-D518-42A2-B9DB-3860040E4207}"/>
+    <hyperlink ref="B99" r:id="rId98" xr:uid="{59A1895D-EEF3-48A0-B800-5AE36A8695A8}"/>
+    <hyperlink ref="B100" r:id="rId99" xr:uid="{D2E5CDE2-6E6A-4C93-A4B8-A1A9668B27F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId96"/>
+  <pageSetup orientation="portrait" r:id="rId100"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AR87"/>
+  <dimension ref="A1:AS92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+    <sheetView topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="68.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="27" style="5" customWidth="1"/>
     <col min="5" max="5" width="24" style="5" customWidth="1"/>
@@ -4110,11 +4194,20 @@
     <col min="25" max="25" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="27" max="30" width="9.140625" style="5"/>
-    <col min="31" max="31" width="35.5703125" style="5" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="5"/>
+    <col min="31" max="31" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="9.140625" style="5"/>
+    <col min="36" max="36" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.140625" style="5"/>
+    <col min="38" max="38" width="101.140625" style="5" customWidth="1"/>
+    <col min="39" max="39" width="164.28515625" style="5" customWidth="1"/>
+    <col min="40" max="40" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="43" width="9.140625" style="5"/>
+    <col min="44" max="44" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.7109375" style="5" customWidth="1"/>
+    <col min="46" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4247,8 +4340,11 @@
       <c r="AR1" s="3" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="2" spans="1:44" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AS1" s="3" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
@@ -4295,12 +4391,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:44" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
@@ -4398,7 +4494,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
@@ -4496,7 +4592,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>48</v>
       </c>
@@ -4615,7 +4711,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>90</v>
       </c>
@@ -4724,7 +4820,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>91</v>
       </c>
@@ -4774,7 +4870,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>149</v>
       </c>
@@ -4785,12 +4881,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>152</v>
       </c>
@@ -4801,7 +4897,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>155</v>
       </c>
@@ -4815,7 +4911,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>210</v>
       </c>
@@ -4823,7 +4919,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>156</v>
       </c>
@@ -4840,7 +4936,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>208</v>
       </c>
@@ -4857,7 +4953,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>157</v>
       </c>
@@ -6306,7 +6402,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>353</v>
       </c>
@@ -6320,7 +6416,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>354</v>
       </c>
@@ -6334,7 +6430,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>355</v>
       </c>
@@ -6389,7 +6485,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>361</v>
       </c>
@@ -6466,7 +6562,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>372</v>
       </c>
@@ -6495,7 +6591,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>373</v>
       </c>
@@ -6542,7 +6638,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>376</v>
       </c>
@@ -6645,8 +6741,9 @@
       <c r="AK55" s="9" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL55" s="14"/>
+    </row>
+    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>399</v>
       </c>
@@ -6699,7 +6796,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>402</v>
       </c>
@@ -6756,7 +6853,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>406</v>
       </c>
@@ -6788,7 +6885,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>414</v>
       </c>
@@ -6847,7 +6944,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>425</v>
       </c>
@@ -6903,7 +7000,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>438</v>
       </c>
@@ -6938,7 +7035,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>442</v>
       </c>
@@ -6976,7 +7073,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>445</v>
       </c>
@@ -7011,7 +7108,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>447</v>
       </c>
@@ -8005,7 +8102,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>631</v>
       </c>
@@ -8097,7 +8194,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>646</v>
       </c>
@@ -8171,7 +8268,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>648</v>
       </c>
@@ -8260,7 +8357,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>655</v>
       </c>
@@ -8277,7 +8374,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>656</v>
       </c>
@@ -8297,7 +8394,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>657</v>
       </c>
@@ -8314,7 +8411,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>658</v>
       </c>
@@ -8392,6 +8489,257 @@
       </c>
       <c r="AF87" s="9" t="s">
         <v>663</v>
+      </c>
+    </row>
+    <row r="88" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G88" s="5">
+        <v>111111</v>
+      </c>
+      <c r="H88" s="5">
+        <v>222222</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q88" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R88" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="S88" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="T88" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="U88" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="V88" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="W88" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="X88" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y88" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="Z88" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA88" s="9"/>
+      <c r="AB88" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="AC88" s="10" t="s">
+        <v>694</v>
+      </c>
+      <c r="AD88" s="10" t="s">
+        <v>695</v>
+      </c>
+      <c r="AS88" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="89" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="AC89" s="10" t="s">
+        <v>694</v>
+      </c>
+      <c r="AD89" s="10" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="90" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G90" s="5">
+        <v>111111</v>
+      </c>
+      <c r="H90" s="5">
+        <v>222222</v>
+      </c>
+      <c r="I90" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q90" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R90" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="S90" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="T90" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="U90" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="V90" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="W90" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="X90" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y90" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="Z90" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA90" s="9"/>
+      <c r="AB90" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="AC90" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="AD90" s="10" t="s">
+        <v>699</v>
+      </c>
+      <c r="AS90" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="91" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G91" s="5">
+        <v>111111</v>
+      </c>
+      <c r="H91" s="5">
+        <v>222222</v>
+      </c>
+      <c r="I91" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q91" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R91" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="S91" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="T91" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="U91" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="V91" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="W91" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="X91" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y91" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="Z91" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA91" s="9"/>
+      <c r="AB91" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="AC91" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="AD91" s="10" t="s">
+        <v>699</v>
+      </c>
+      <c r="AS91" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="92" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G92" s="5">
+        <v>111111</v>
+      </c>
+      <c r="H92" s="5">
+        <v>222222</v>
+      </c>
+      <c r="I92" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q92" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R92" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="S92" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="T92" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="U92" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="V92" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="W92" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="X92" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y92" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="Z92" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA92" s="9"/>
+      <c r="AB92" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="AC92" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="AD92" s="10" t="s">
+        <v>699</v>
+      </c>
+      <c r="AS92" s="5" t="s">
+        <v>697</v>
       </c>
     </row>
   </sheetData>
@@ -8404,8 +8752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7A3FC5-D09A-4697-BB1A-908D46717259}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ädded new scripts as part of Existing Member
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02F9E11-FA66-46A1-A74B-59A2CADD8C74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73128261-DFAB-4496-B0B3-44646A7E454C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,25 @@
     <sheet name="MemberVerification" sheetId="8" r:id="rId3"/>
     <sheet name="Notes" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1733" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="707">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -2134,6 +2142,21 @@
   </si>
   <si>
     <t>C28344_VerifyThatInformationTabIsHighLightedWhenUserInBeneficiariesPage</t>
+  </si>
+  <si>
+    <t>046206978</t>
+  </si>
+  <si>
+    <t>02131986</t>
+  </si>
+  <si>
+    <t>C28351_VerifyThatInformationTabIsHighLightedWhenUserInConfirmAccountRolesPage</t>
+  </si>
+  <si>
+    <t>C28354_VerifyThatVerificationStepIsHighlightedWhenUserIsOnAccountSummaryPage</t>
+  </si>
+  <si>
+    <t>C28356_VerifyThatDisclouserStepIsHighlightedWhenUserOnIndentityVerificationPage</t>
   </si>
 </sst>
 </file>
@@ -2521,10 +2544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99:D100"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4050,6 +4073,48 @@
         <v>5</v>
       </c>
       <c r="D100" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>705</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>706</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4154,25 +4219,28 @@
     <hyperlink ref="B98" r:id="rId97" xr:uid="{A549EE0A-D518-42A2-B9DB-3860040E4207}"/>
     <hyperlink ref="B99" r:id="rId98" xr:uid="{59A1895D-EEF3-48A0-B800-5AE36A8695A8}"/>
     <hyperlink ref="B100" r:id="rId99" xr:uid="{D2E5CDE2-6E6A-4C93-A4B8-A1A9668B27F6}"/>
+    <hyperlink ref="B101" r:id="rId100" xr:uid="{F8187B01-7A56-4E6C-9D97-26E4FF46AF24}"/>
+    <hyperlink ref="B102" r:id="rId101" xr:uid="{6764C9E9-88E5-43C9-AFC0-627EF752E112}"/>
+    <hyperlink ref="B103" r:id="rId102" xr:uid="{3A7CC88D-6A43-499B-9DBC-72389851AE49}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId100"/>
+  <pageSetup orientation="portrait" r:id="rId103"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AS92"/>
+  <dimension ref="A1:AS96"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A92" sqref="A92"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="27" style="5" customWidth="1"/>
     <col min="5" max="5" width="24" style="5" customWidth="1"/>
@@ -4184,7 +4252,8 @@
     <col min="12" max="12" width="13.42578125" style="5" customWidth="1"/>
     <col min="13" max="13" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="9.140625" style="5"/>
-    <col min="17" max="18" width="22.7109375" style="5" customWidth="1"/>
+    <col min="17" max="17" width="30.85546875" style="5" customWidth="1"/>
+    <col min="18" max="18" width="22.7109375" style="5" customWidth="1"/>
     <col min="19" max="19" width="11.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.5703125" style="5" customWidth="1"/>
     <col min="21" max="21" width="15.7109375" style="5" customWidth="1"/>
@@ -4193,8 +4262,11 @@
     <col min="24" max="24" width="10.85546875" style="5" customWidth="1"/>
     <col min="25" max="25" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="30" width="9.140625" style="5"/>
-    <col min="31" max="31" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14" style="5" customWidth="1"/>
+    <col min="28" max="28" width="33.140625" style="5" customWidth="1"/>
+    <col min="29" max="29" width="21" style="5" customWidth="1"/>
+    <col min="30" max="30" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="53" style="5" customWidth="1"/>
     <col min="32" max="35" width="9.140625" style="5"/>
     <col min="36" max="36" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="9.140625" style="5"/>
@@ -8733,12 +8805,333 @@
         <v>464</v>
       </c>
       <c r="AC92" s="10" t="s">
-        <v>689</v>
+        <v>702</v>
       </c>
       <c r="AD92" s="10" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="AS92" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="93" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G93" s="5">
+        <v>111111</v>
+      </c>
+      <c r="H93" s="5">
+        <v>222222</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q93" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R93" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="S93" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="T93" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="U93" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="V93" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="W93" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="X93" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y93" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="Z93" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA93" s="9"/>
+      <c r="AB93" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="AC93" s="10" t="s">
+        <v>702</v>
+      </c>
+      <c r="AD93" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="AE93" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="AF93" s="9" t="s">
+        <v>536</v>
+      </c>
+      <c r="AG93" s="9" t="s">
+        <v>537</v>
+      </c>
+      <c r="AH93" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="AI93" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="AJ93" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="AK93" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="AL93" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="AM93" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="AN93" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="AO93" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="AS93" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="94" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G94" s="5">
+        <v>111111</v>
+      </c>
+      <c r="H94" s="5">
+        <v>222222</v>
+      </c>
+      <c r="I94" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q94" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R94" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="S94" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="T94" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="U94" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="V94" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="W94" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="X94" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y94" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="Z94" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA94" s="9"/>
+      <c r="AB94" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="AC94" s="10" t="s">
+        <v>702</v>
+      </c>
+      <c r="AD94" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="AS94" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="95" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>706</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G95" s="5">
+        <v>8000</v>
+      </c>
+      <c r="H95" s="5">
+        <v>16000</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="J95" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="K95" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="L95" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="M95" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="N95" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="O95" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="P95" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q95" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R95" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="S95" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="T95" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="U95" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="V95" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="W95" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="X95" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="Y95" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="Z95" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="AA95" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB95" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="AC95" s="10" t="s">
+        <v>702</v>
+      </c>
+      <c r="AD95" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="AE95" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="AF95" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="AG95" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="AH95" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="AI95" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="AJ95" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="AK95" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="AL95" s="14"/>
+      <c r="AS95" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="96" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G96" s="5">
+        <v>8000</v>
+      </c>
+      <c r="H96" s="5">
+        <v>16000</v>
+      </c>
+      <c r="I96" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q96" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R96" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="S96" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="T96" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="U96" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="V96" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="W96" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="X96" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y96" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="Z96" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA96" s="9"/>
+      <c r="AB96" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="AC96" s="10" t="s">
+        <v>702</v>
+      </c>
+      <c r="AD96" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="AS96" s="5" t="s">
         <v>697</v>
       </c>
     </row>
@@ -8753,7 +9146,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
New Feature scripts has been added
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B6476A-6085-45D1-B465-028EA499A780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DCA23E-9B91-4173-A0F9-36A44C9D0023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="720">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -2166,13 +2166,43 @@
   </si>
   <si>
     <t>C28360_VerifyThatDisclouserStepIsHighlightedWhenUserOnDeclineDisclouserPage</t>
+  </si>
+  <si>
+    <t>C28362_VerifyThatFundingStepIsHighlightedWhenUserOnFundAccountsPage</t>
+  </si>
+  <si>
+    <t>C28365_VerifyLanguageOnAconfirmAccountSelectionPage</t>
+  </si>
+  <si>
+    <t>C28367_VerifyThankYouPageProvidingClearInstructions</t>
+  </si>
+  <si>
+    <t>We’re already heads down, reviewing your application. We’re pretty quick so expect to hear from us within one business day — we’ll send a response to the email address we have on file.</t>
+  </si>
+  <si>
+    <t>SubHeaderText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For security purposes, we may need additional documentation to complete your application. You can even take pictures of the requested documents with your smartphone and upload them below. You can also upload the documents at a later time by visiting the </t>
+  </si>
+  <si>
+    <t>SubHeaderDocument</t>
+  </si>
+  <si>
+    <t>C28372_UserwouldLikeToRecieveOTPViaEmail</t>
+  </si>
+  <si>
+    <t>C28375_UserwouldLikeToEnterOTP</t>
+  </si>
+  <si>
+    <t>C28376_UserwouldLikeToReRequestOTP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2196,6 +2226,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2218,7 +2254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2238,6 +2274,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2553,10 +2590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105:D106"/>
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4166,6 +4203,90 @@
         <v>5</v>
       </c>
       <c r="D106" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>710</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>711</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>712</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>718</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>719</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D112" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4276,19 +4397,25 @@
     <hyperlink ref="B104" r:id="rId103" xr:uid="{A158A6E7-ACC4-4773-A6D5-610FA16CE692}"/>
     <hyperlink ref="B105" r:id="rId104" xr:uid="{E6149BEC-DA25-4B08-8C6A-564ACF89F763}"/>
     <hyperlink ref="B106" r:id="rId105" xr:uid="{91B47A1D-FB03-45A5-85AD-E6E1003CA367}"/>
+    <hyperlink ref="B107" r:id="rId106" xr:uid="{454C594D-9A11-4B29-802E-24294BB65339}"/>
+    <hyperlink ref="B108" r:id="rId107" xr:uid="{A52A6DB2-E949-45C7-A0D5-E041A0458DB3}"/>
+    <hyperlink ref="B109" r:id="rId108" xr:uid="{9667E24A-E6CE-4032-9FE8-C01FC994FB2C}"/>
+    <hyperlink ref="B110" r:id="rId109" xr:uid="{239E521A-02D7-4771-8C43-1713DD8FAC70}"/>
+    <hyperlink ref="B111" r:id="rId110" xr:uid="{EAAC0851-9B4B-4EAF-A3D0-833B8F8D3F6D}"/>
+    <hyperlink ref="B112" r:id="rId111" xr:uid="{4E177EAC-B594-4046-AB20-700489B8CAA7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId106"/>
+  <pageSetup orientation="portrait" r:id="rId112"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AS99"/>
+  <dimension ref="A1:AU105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A105" sqref="A105:XFD105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4330,10 +4457,12 @@
     <col min="41" max="43" width="9.140625" style="5"/>
     <col min="44" max="44" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="14.7109375" style="5" customWidth="1"/>
-    <col min="46" max="16384" width="9.140625" style="5"/>
+    <col min="46" max="46" width="58.28515625" style="5" customWidth="1"/>
+    <col min="47" max="47" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4469,8 +4598,14 @@
       <c r="AS1" s="3" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="2" spans="1:45" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AT1" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
@@ -4517,12 +4652,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:45" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:45" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
@@ -4620,7 +4755,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
@@ -4718,7 +4853,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>48</v>
       </c>
@@ -4837,7 +4972,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>90</v>
       </c>
@@ -4946,7 +5081,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>91</v>
       </c>
@@ -4996,7 +5131,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>149</v>
       </c>
@@ -5007,12 +5142,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>152</v>
       </c>
@@ -5023,7 +5158,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>155</v>
       </c>
@@ -5037,7 +5172,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>210</v>
       </c>
@@ -5045,7 +5180,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>156</v>
       </c>
@@ -5062,7 +5197,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>208</v>
       </c>
@@ -5079,7 +5214,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>157</v>
       </c>
@@ -9189,7 +9324,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="97" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>707</v>
       </c>
@@ -9249,7 +9384,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="98" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>708</v>
       </c>
@@ -9305,7 +9440,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="99" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>709</v>
       </c>
@@ -9361,9 +9496,511 @@
         <v>697</v>
       </c>
     </row>
+    <row r="100" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G100" s="5">
+        <v>9874.06</v>
+      </c>
+      <c r="Q100" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R100" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="S100" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="T100" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="U100" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="V100" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="W100" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="X100" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="Y100" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="Z100" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA100" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="AB100" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="AC100" s="10" t="s">
+        <v>702</v>
+      </c>
+      <c r="AD100" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="AS100" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="101" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G101" s="5">
+        <v>111111</v>
+      </c>
+      <c r="H101" s="5">
+        <v>222222</v>
+      </c>
+      <c r="I101" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q101" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R101" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="S101" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="T101" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="U101" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="V101" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="W101" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="X101" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y101" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="Z101" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA101" s="9"/>
+      <c r="AB101" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="AC101" s="10" t="s">
+        <v>702</v>
+      </c>
+      <c r="AD101" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="AS101" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="102" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G102" s="5">
+        <v>9874.06</v>
+      </c>
+      <c r="Q102" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R102" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="S102" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="T102" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="U102" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="V102" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="W102" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="X102" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="Y102" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="Z102" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA102" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="AB102" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="AC102" s="10" t="s">
+        <v>702</v>
+      </c>
+      <c r="AD102" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="AS102" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="AT102" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="AU102" s="15" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="103" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G103" s="5">
+        <v>8000</v>
+      </c>
+      <c r="H103" s="5">
+        <v>16000</v>
+      </c>
+      <c r="I103" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="J103" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="K103" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="L103" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="M103" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="N103" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="O103" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="P103" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q103" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R103" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="S103" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="T103" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="U103" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="V103" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="W103" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="X103" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="Y103" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="Z103" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="AA103" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB103" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="AC103" s="10" t="s">
+        <v>702</v>
+      </c>
+      <c r="AD103" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="AE103" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="AF103" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="AG103" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="AH103" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="AI103" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="AJ103" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="AK103" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="AL103" s="14"/>
+      <c r="AS103" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="104" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G104" s="5">
+        <v>8000</v>
+      </c>
+      <c r="H104" s="5">
+        <v>16000</v>
+      </c>
+      <c r="I104" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="J104" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="K104" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="L104" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="M104" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="N104" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="O104" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="P104" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q104" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R104" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="S104" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="T104" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="U104" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="V104" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="W104" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="X104" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="Y104" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="Z104" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="AA104" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB104" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="AC104" s="10" t="s">
+        <v>702</v>
+      </c>
+      <c r="AD104" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="AE104" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="AF104" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="AG104" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="AH104" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="AI104" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="AJ104" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="AK104" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="AL104" s="14"/>
+      <c r="AS104" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="105" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G105" s="5">
+        <v>8000</v>
+      </c>
+      <c r="H105" s="5">
+        <v>16000</v>
+      </c>
+      <c r="I105" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="J105" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="K105" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="L105" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="M105" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="N105" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="O105" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="P105" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q105" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R105" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="S105" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="T105" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="U105" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="V105" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="W105" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="X105" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="Y105" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="Z105" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="AA105" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB105" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="AC105" s="10" t="s">
+        <v>702</v>
+      </c>
+      <c r="AD105" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="AE105" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="AF105" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="AG105" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="AH105" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="AI105" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="AJ105" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="AK105" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="AL105" s="14"/>
+      <c r="AS105" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Modified steps for Account Funding
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DCA23E-9B91-4173-A0F9-36A44C9D0023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4129BA8-09D0-42F1-95B0-C5C5F479D1DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="722">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -2196,6 +2196,12 @@
   </si>
   <si>
     <t>C28376_UserwouldLikeToReRequestOTP</t>
+  </si>
+  <si>
+    <t>046205736</t>
+  </si>
+  <si>
+    <t>07041988</t>
   </si>
 </sst>
 </file>
@@ -2592,8 +2598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4413,9 +4419,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AU105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A105" sqref="A105:XFD105"/>
+    <sheetView topLeftCell="X1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC65" sqref="AC65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6663,7 +6669,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>353</v>
       </c>
@@ -6677,7 +6683,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>354</v>
       </c>
@@ -6691,7 +6697,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>355</v>
       </c>
@@ -6746,7 +6752,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>361</v>
       </c>
@@ -6823,7 +6829,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>372</v>
       </c>
@@ -6852,7 +6858,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>373</v>
       </c>
@@ -6899,7 +6905,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>376</v>
       </c>
@@ -7003,8 +7009,11 @@
         <v>398</v>
       </c>
       <c r="AL55" s="14"/>
-    </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AS55" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="56" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>399</v>
       </c>
@@ -7057,7 +7066,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>402</v>
       </c>
@@ -7114,7 +7123,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>406</v>
       </c>
@@ -7146,7 +7155,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>414</v>
       </c>
@@ -7205,7 +7214,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>425</v>
       </c>
@@ -7261,7 +7270,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>438</v>
       </c>
@@ -7284,19 +7293,52 @@
         <v>219</v>
       </c>
       <c r="Q61" s="5" t="s">
-        <v>158</v>
+        <v>11</v>
+      </c>
+      <c r="R61" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="S61" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="T61" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="U61" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="V61" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="W61" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="X61" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="Y61" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="Z61" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA61" s="9" t="s">
+        <v>291</v>
       </c>
       <c r="AB61" s="10" t="s">
         <v>411</v>
       </c>
       <c r="AC61" s="10" t="s">
-        <v>412</v>
+        <v>702</v>
       </c>
       <c r="AD61" s="10" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+        <v>703</v>
+      </c>
+      <c r="AS61" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="62" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>442</v>
       </c>
@@ -7328,13 +7370,16 @@
         <v>421</v>
       </c>
       <c r="AC62" s="10" t="s">
-        <v>422</v>
+        <v>702</v>
       </c>
       <c r="AD62" s="10" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+        <v>703</v>
+      </c>
+      <c r="AS62" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="63" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>445</v>
       </c>
@@ -7363,13 +7408,16 @@
         <v>464</v>
       </c>
       <c r="AC63" s="10" t="s">
-        <v>465</v>
+        <v>702</v>
       </c>
       <c r="AD63" s="10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+        <v>703</v>
+      </c>
+      <c r="AS63" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="64" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>447</v>
       </c>
@@ -7383,13 +7431,16 @@
         <v>411</v>
       </c>
       <c r="AC64" s="10" t="s">
-        <v>412</v>
+        <v>720</v>
       </c>
       <c r="AD64" s="10" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="65" spans="1:44" x14ac:dyDescent="0.25">
+        <v>721</v>
+      </c>
+      <c r="AS64" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="65" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>448</v>
       </c>
@@ -7418,13 +7469,16 @@
         <v>421</v>
       </c>
       <c r="AC65" s="10" t="s">
-        <v>422</v>
+        <v>720</v>
       </c>
       <c r="AD65" s="10" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="66" spans="1:44" x14ac:dyDescent="0.25">
+        <v>721</v>
+      </c>
+      <c r="AS65" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="66" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>450</v>
       </c>
@@ -7450,13 +7504,16 @@
         <v>464</v>
       </c>
       <c r="AC66" s="10" t="s">
-        <v>465</v>
+        <v>720</v>
       </c>
       <c r="AD66" s="10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="67" spans="1:44" x14ac:dyDescent="0.25">
+        <v>721</v>
+      </c>
+      <c r="AS66" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="67" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>453</v>
       </c>
@@ -7490,8 +7547,11 @@
       <c r="AD67" s="10" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS67" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="68" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>456</v>
       </c>
@@ -7519,8 +7579,11 @@
       <c r="AD68" s="10" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS68" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="69" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>482</v>
       </c>
@@ -7534,7 +7597,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="70" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>484</v>
       </c>
@@ -7668,7 +7731,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>514</v>
       </c>
@@ -7724,7 +7787,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>527</v>
       </c>
@@ -7828,7 +7891,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>549</v>
       </c>
@@ -7896,7 +7959,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="74" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>563</v>
       </c>
@@ -7964,7 +8027,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>678</v>
       </c>
@@ -8056,7 +8119,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="76" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>593</v>
       </c>
@@ -8172,7 +8235,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>607</v>
       </c>
@@ -8213,7 +8276,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>612</v>
       </c>
@@ -8272,7 +8335,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="79" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>620</v>
       </c>
@@ -8328,7 +8391,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="80" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>630</v>
       </c>
@@ -10009,7 +10072,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modification completed for AgreementDisclosures ConfirmAccounts ApplicantInfo WIP for JointOwnerBeneficiaries
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4129BA8-09D0-42F1-95B0-C5C5F479D1DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4295CD0-7913-4913-9779-63030C02BC92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2120" uniqueCount="722">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -2598,8 +2598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A56" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4419,9 +4419,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AU105"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC65" sqref="AC65"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AS73" sqref="AS73:AS74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5977,7 +5977,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>259</v>
       </c>
@@ -6006,7 +6006,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>264</v>
       </c>
@@ -6062,7 +6062,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>266</v>
       </c>
@@ -6106,7 +6106,7 @@
       <c r="AG35" s="9"/>
       <c r="AH35" s="9"/>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>276</v>
       </c>
@@ -6135,7 +6135,7 @@
       <c r="AG36" s="9"/>
       <c r="AH36" s="9"/>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>281</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>287</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>293</v>
       </c>
@@ -6291,7 +6291,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>299</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>305</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>313</v>
       </c>
@@ -6459,7 +6459,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>318</v>
       </c>
@@ -6524,7 +6524,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>334</v>
       </c>
@@ -6549,8 +6549,11 @@
       <c r="AD44" s="10" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AS44" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>337</v>
       </c>
@@ -6578,8 +6581,11 @@
       <c r="AD45" s="10" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AS45" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>342</v>
       </c>
@@ -6604,8 +6610,11 @@
       <c r="AD46" s="10" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AS46" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>343</v>
       </c>
@@ -6627,8 +6636,11 @@
       <c r="AF47" s="9" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AS47" s="5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>345</v>
       </c>
@@ -6667,6 +6679,9 @@
       </c>
       <c r="AH48" s="10" t="s">
         <v>127</v>
+      </c>
+      <c r="AS48" s="5" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="49" spans="1:45" x14ac:dyDescent="0.25">
@@ -6682,6 +6697,9 @@
       <c r="AD49" s="10" t="s">
         <v>413</v>
       </c>
+      <c r="AS49" s="5" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="50" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
@@ -6695,6 +6713,9 @@
       </c>
       <c r="AD50" s="10" t="s">
         <v>423</v>
+      </c>
+      <c r="AS50" s="5" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="51" spans="1:45" x14ac:dyDescent="0.25">
@@ -6751,6 +6772,9 @@
       <c r="AD51" s="10" t="s">
         <v>128</v>
       </c>
+      <c r="AS51" s="5" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
@@ -6828,6 +6852,9 @@
       <c r="AJ52" s="9" t="s">
         <v>371</v>
       </c>
+      <c r="AS52" s="5" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="53" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
@@ -6857,6 +6884,9 @@
       <c r="AF53" s="9" t="s">
         <v>474</v>
       </c>
+      <c r="AS53" s="5" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="54" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
@@ -6904,6 +6934,9 @@
       <c r="AF54" s="9" t="s">
         <v>344</v>
       </c>
+      <c r="AS54" s="5" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="55" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
@@ -7065,6 +7098,9 @@
       <c r="AD56" s="10" t="s">
         <v>423</v>
       </c>
+      <c r="AS56" s="5" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="57" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
@@ -7122,6 +7158,9 @@
       <c r="AD57" s="10" t="s">
         <v>128</v>
       </c>
+      <c r="AS57" s="5" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="58" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
@@ -7154,6 +7193,9 @@
       <c r="AD58" s="10" t="s">
         <v>413</v>
       </c>
+      <c r="AS58" s="5" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="59" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
@@ -7596,6 +7638,9 @@
       <c r="AD69" s="10" t="s">
         <v>128</v>
       </c>
+      <c r="AS69" s="5" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="70" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
@@ -7683,10 +7728,10 @@
         <v>511</v>
       </c>
       <c r="AC70" s="10" t="s">
-        <v>512</v>
+        <v>702</v>
       </c>
       <c r="AD70" s="10" t="s">
-        <v>513</v>
+        <v>703</v>
       </c>
       <c r="AE70" s="5" t="s">
         <v>499</v>
@@ -7729,6 +7774,9 @@
       </c>
       <c r="AR70" s="9" t="s">
         <v>136</v>
+      </c>
+      <c r="AS70" s="5" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="71" spans="1:45" x14ac:dyDescent="0.25">
@@ -7780,11 +7828,14 @@
       <c r="AB71" s="9" t="s">
         <v>485</v>
       </c>
-      <c r="AC71" s="9" t="s">
-        <v>486</v>
-      </c>
-      <c r="AD71" s="9" t="s">
-        <v>487</v>
+      <c r="AC71" s="10" t="s">
+        <v>702</v>
+      </c>
+      <c r="AD71" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="AS71" s="5" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="72" spans="1:45" x14ac:dyDescent="0.25">
@@ -7873,10 +7924,10 @@
         <v>411</v>
       </c>
       <c r="AC72" s="10" t="s">
-        <v>412</v>
+        <v>702</v>
       </c>
       <c r="AD72" s="10" t="s">
-        <v>413</v>
+        <v>703</v>
       </c>
       <c r="AE72" s="9" t="s">
         <v>546</v>
@@ -7889,6 +7940,9 @@
       </c>
       <c r="AH72" s="9" t="s">
         <v>548</v>
+      </c>
+      <c r="AS72" s="5" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="73" spans="1:45" x14ac:dyDescent="0.25">
@@ -7953,10 +8007,13 @@
         <v>421</v>
       </c>
       <c r="AC73" s="10" t="s">
-        <v>422</v>
+        <v>702</v>
       </c>
       <c r="AD73" s="10" t="s">
-        <v>423</v>
+        <v>703</v>
+      </c>
+      <c r="AS73" s="5" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="74" spans="1:45" x14ac:dyDescent="0.25">
@@ -8021,10 +8078,13 @@
         <v>511</v>
       </c>
       <c r="AC74" s="10" t="s">
-        <v>512</v>
+        <v>702</v>
       </c>
       <c r="AD74" s="10" t="s">
-        <v>513</v>
+        <v>703</v>
+      </c>
+      <c r="AS74" s="5" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="75" spans="1:45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ädded Modified scripts to the respective components
</commit_message>
<xml_diff>
--- a/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
+++ b/InstantOpen_ExistingMember/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\InstantOpen_ExistingMember\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4295CD0-7913-4913-9779-63030C02BC92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3BD640-CECF-4E4B-A13C-66280770C565}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2120" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2122" uniqueCount="720">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1572,12 +1572,6 @@
   </si>
   <si>
     <t>8244907</t>
-  </si>
-  <si>
-    <t>632557458</t>
-  </si>
-  <si>
-    <t>04271988</t>
   </si>
   <si>
     <t>C24212_VerifyOneBeneficiary</t>
@@ -3671,7 +3665,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>8</v>
@@ -3687,7 +3681,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>8</v>
@@ -3703,7 +3697,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>8</v>
@@ -3718,7 +3712,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>8</v>
@@ -3733,7 +3727,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>8</v>
@@ -3748,7 +3742,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>8</v>
@@ -3763,7 +3757,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>8</v>
@@ -3779,7 +3773,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>8</v>
@@ -3795,7 +3789,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>8</v>
@@ -3811,7 +3805,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>8</v>
@@ -3826,7 +3820,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>8</v>
@@ -3841,7 +3835,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>8</v>
@@ -3856,7 +3850,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>8</v>
@@ -3871,7 +3865,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>8</v>
@@ -3886,7 +3880,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>8</v>
@@ -3902,7 +3896,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>8</v>
@@ -3918,7 +3912,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>8</v>
@@ -3934,7 +3928,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>8</v>
@@ -3950,7 +3944,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>8</v>
@@ -3966,7 +3960,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>8</v>
@@ -3982,7 +3976,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>8</v>
@@ -3997,7 +3991,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>8</v>
@@ -4012,7 +4006,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>8</v>
@@ -4027,7 +4021,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>8</v>
@@ -4042,7 +4036,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>8</v>
@@ -4057,7 +4051,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>8</v>
@@ -4072,7 +4066,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>8</v>
@@ -4087,7 +4081,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>8</v>
@@ -4102,7 +4096,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>8</v>
@@ -4116,7 +4110,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>8</v>
@@ -4130,7 +4124,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>8</v>
@@ -4144,7 +4138,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>8</v>
@@ -4158,7 +4152,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>8</v>
@@ -4172,7 +4166,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>8</v>
@@ -4186,7 +4180,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>8</v>
@@ -4200,7 +4194,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>8</v>
@@ -4214,7 +4208,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>8</v>
@@ -4228,7 +4222,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>8</v>
@@ -4242,7 +4236,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>8</v>
@@ -4256,7 +4250,7 @@
     </row>
     <row r="110" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>8</v>
@@ -4270,7 +4264,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>8</v>
@@ -4284,7 +4278,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>8</v>
@@ -4419,9 +4413,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AU105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS73" sqref="AS73:AS74"/>
+    <sheetView topLeftCell="AN1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AT9" sqref="AT9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4602,13 +4596,13 @@
         <v>507</v>
       </c>
       <c r="AS1" s="3" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="AT1" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="AU1" s="3" t="s">
         <v>714</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="2" spans="1:47" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -5270,16 +5264,19 @@
         <v>411</v>
       </c>
       <c r="AC16" s="10" t="s">
-        <v>412</v>
+        <v>700</v>
       </c>
       <c r="AD16" s="10" t="s">
-        <v>413</v>
+        <v>701</v>
       </c>
       <c r="AE16" s="9" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AS16" s="5" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>159</v>
       </c>
@@ -5304,8 +5301,11 @@
       <c r="AF17" s="5" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AS17" s="5" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>162</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>164</v>
       </c>
@@ -5399,7 +5399,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>166</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>174</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>177</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>198</v>
       </c>
@@ -5590,7 +5590,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>201</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>212</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>217</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>218</v>
       </c>
@@ -5787,7 +5787,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>236</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>241</v>
       </c>
@@ -5857,7 +5857,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>243</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>253</v>
       </c>
@@ -5948,7 +5948,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>255</v>
       </c>
@@ -6550,7 +6550,7 @@
         <v>128</v>
       </c>
       <c r="AS44" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="45" spans="1:45" x14ac:dyDescent="0.25">
@@ -6582,7 +6582,7 @@
         <v>423</v>
       </c>
       <c r="AS45" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="46" spans="1:45" x14ac:dyDescent="0.25">
@@ -6611,7 +6611,7 @@
         <v>413</v>
       </c>
       <c r="AS46" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.25">
@@ -6637,7 +6637,7 @@
         <v>344</v>
       </c>
       <c r="AS47" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="48" spans="1:45" x14ac:dyDescent="0.25">
@@ -6681,7 +6681,7 @@
         <v>127</v>
       </c>
       <c r="AS48" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="49" spans="1:45" x14ac:dyDescent="0.25">
@@ -6698,7 +6698,7 @@
         <v>413</v>
       </c>
       <c r="AS49" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="50" spans="1:45" x14ac:dyDescent="0.25">
@@ -6715,7 +6715,7 @@
         <v>423</v>
       </c>
       <c r="AS50" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="51" spans="1:45" x14ac:dyDescent="0.25">
@@ -6773,7 +6773,7 @@
         <v>128</v>
       </c>
       <c r="AS51" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="52" spans="1:45" x14ac:dyDescent="0.25">
@@ -6853,7 +6853,7 @@
         <v>371</v>
       </c>
       <c r="AS52" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="53" spans="1:45" x14ac:dyDescent="0.25">
@@ -6885,7 +6885,7 @@
         <v>474</v>
       </c>
       <c r="AS53" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="54" spans="1:45" x14ac:dyDescent="0.25">
@@ -6935,7 +6935,7 @@
         <v>344</v>
       </c>
       <c r="AS54" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="55" spans="1:45" x14ac:dyDescent="0.25">
@@ -7043,7 +7043,7 @@
       </c>
       <c r="AL55" s="14"/>
       <c r="AS55" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="56" spans="1:45" x14ac:dyDescent="0.25">
@@ -7099,7 +7099,7 @@
         <v>423</v>
       </c>
       <c r="AS56" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="57" spans="1:45" x14ac:dyDescent="0.25">
@@ -7159,7 +7159,7 @@
         <v>128</v>
       </c>
       <c r="AS57" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="58" spans="1:45" x14ac:dyDescent="0.25">
@@ -7194,7 +7194,7 @@
         <v>413</v>
       </c>
       <c r="AS58" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="59" spans="1:45" x14ac:dyDescent="0.25">
@@ -7306,10 +7306,10 @@
         <v>464</v>
       </c>
       <c r="AC60" s="10" t="s">
-        <v>465</v>
+        <v>700</v>
       </c>
       <c r="AD60" s="10" t="s">
-        <v>128</v>
+        <v>701</v>
       </c>
     </row>
     <row r="61" spans="1:45" x14ac:dyDescent="0.25">
@@ -7371,13 +7371,13 @@
         <v>411</v>
       </c>
       <c r="AC61" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD61" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS61" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="62" spans="1:45" x14ac:dyDescent="0.25">
@@ -7412,13 +7412,13 @@
         <v>421</v>
       </c>
       <c r="AC62" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD62" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS62" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="63" spans="1:45" x14ac:dyDescent="0.25">
@@ -7450,13 +7450,13 @@
         <v>464</v>
       </c>
       <c r="AC63" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD63" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS63" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="64" spans="1:45" x14ac:dyDescent="0.25">
@@ -7473,13 +7473,13 @@
         <v>411</v>
       </c>
       <c r="AC64" s="10" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="AD64" s="10" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="AS64" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="65" spans="1:45" x14ac:dyDescent="0.25">
@@ -7511,13 +7511,13 @@
         <v>421</v>
       </c>
       <c r="AC65" s="10" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="AD65" s="10" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="AS65" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="66" spans="1:45" x14ac:dyDescent="0.25">
@@ -7546,13 +7546,13 @@
         <v>464</v>
       </c>
       <c r="AC66" s="10" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="AD66" s="10" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="AS66" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="67" spans="1:45" x14ac:dyDescent="0.25">
@@ -7590,7 +7590,7 @@
         <v>413</v>
       </c>
       <c r="AS67" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="68" spans="1:45" x14ac:dyDescent="0.25">
@@ -7622,7 +7622,7 @@
         <v>423</v>
       </c>
       <c r="AS68" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="69" spans="1:45" x14ac:dyDescent="0.25">
@@ -7639,7 +7639,7 @@
         <v>128</v>
       </c>
       <c r="AS69" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="70" spans="1:45" x14ac:dyDescent="0.25">
@@ -7728,10 +7728,10 @@
         <v>511</v>
       </c>
       <c r="AC70" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD70" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AE70" s="5" t="s">
         <v>499</v>
@@ -7776,71 +7776,71 @@
         <v>136</v>
       </c>
       <c r="AS70" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="71" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="L71" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="M71" s="5" t="s">
         <v>514</v>
       </c>
-      <c r="L71" s="5" t="s">
+      <c r="N71" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="M71" s="5" t="s">
+      <c r="O71" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="N71" s="5" t="s">
+      <c r="P71" s="9" t="s">
         <v>517</v>
       </c>
-      <c r="O71" s="5" t="s">
+      <c r="Q71" s="9" t="s">
         <v>518</v>
       </c>
-      <c r="P71" s="9" t="s">
+      <c r="R71" s="9" t="s">
         <v>519</v>
-      </c>
-      <c r="Q71" s="9" t="s">
-        <v>520</v>
-      </c>
-      <c r="R71" s="9" t="s">
-        <v>521</v>
       </c>
       <c r="S71" s="5" t="s">
         <v>11</v>
       </c>
       <c r="T71" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="U71" s="9" t="s">
+        <v>521</v>
+      </c>
+      <c r="V71" s="9" t="s">
         <v>522</v>
-      </c>
-      <c r="U71" s="9" t="s">
-        <v>523</v>
-      </c>
-      <c r="V71" s="9" t="s">
-        <v>524</v>
       </c>
       <c r="W71" s="9" t="s">
         <v>510</v>
       </c>
       <c r="X71" s="9" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="Y71" s="5" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="AB71" s="9" t="s">
         <v>485</v>
       </c>
       <c r="AC71" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD71" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS71" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="72" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B72" s="5">
         <v>1234.56</v>
@@ -7849,132 +7849,132 @@
         <v>2789</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F72" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="H72" s="9" t="s">
         <v>529</v>
       </c>
-      <c r="G72" s="9" t="s">
+      <c r="I72" s="9" t="s">
         <v>530</v>
-      </c>
-      <c r="H72" s="9" t="s">
-        <v>531</v>
-      </c>
-      <c r="I72" s="9" t="s">
-        <v>532</v>
       </c>
       <c r="J72" s="9" t="s">
         <v>120</v>
       </c>
       <c r="K72" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="L72" s="9" t="s">
+        <v>531</v>
+      </c>
+      <c r="M72" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="N72" s="9" t="s">
         <v>534</v>
       </c>
-      <c r="L72" s="9" t="s">
-        <v>533</v>
-      </c>
-      <c r="M72" s="9" t="s">
+      <c r="O72" s="9" t="s">
         <v>535</v>
       </c>
-      <c r="N72" s="9" t="s">
+      <c r="P72" s="9" t="s">
         <v>536</v>
       </c>
-      <c r="O72" s="9" t="s">
+      <c r="Q72" s="9" t="s">
         <v>537</v>
       </c>
-      <c r="P72" s="9" t="s">
+      <c r="R72" s="9" t="s">
         <v>538</v>
-      </c>
-      <c r="Q72" s="9" t="s">
-        <v>539</v>
-      </c>
-      <c r="R72" s="9" t="s">
-        <v>540</v>
       </c>
       <c r="S72" s="9" t="s">
         <v>510</v>
       </c>
       <c r="T72" s="9" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="U72" s="5" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="V72" s="9" t="s">
         <v>142</v>
       </c>
       <c r="W72" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="X72" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="Y72" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="Z72" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="AA72" s="9" t="s">
         <v>543</v>
-      </c>
-      <c r="X72" s="9" t="s">
-        <v>544</v>
-      </c>
-      <c r="Y72" s="5" t="s">
-        <v>518</v>
-      </c>
-      <c r="Z72" s="9" t="s">
-        <v>519</v>
-      </c>
-      <c r="AA72" s="9" t="s">
-        <v>545</v>
       </c>
       <c r="AB72" s="10" t="s">
         <v>411</v>
       </c>
       <c r="AC72" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD72" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AE72" s="9" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="AF72" s="5" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="AG72" s="9" t="s">
         <v>365</v>
       </c>
       <c r="AH72" s="9" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="AS72" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="73" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="H73" s="5" t="s">
         <v>549</v>
       </c>
-      <c r="G73" s="5" t="s">
+      <c r="I73" s="9" t="s">
         <v>550</v>
       </c>
-      <c r="H73" s="5" t="s">
+      <c r="J73" s="9" t="s">
         <v>551</v>
-      </c>
-      <c r="I73" s="9" t="s">
-        <v>552</v>
-      </c>
-      <c r="J73" s="9" t="s">
-        <v>553</v>
       </c>
       <c r="K73" s="9" t="s">
         <v>510</v>
       </c>
       <c r="L73" s="9" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="M73" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="N73" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="O73" s="9" t="s">
         <v>554</v>
-      </c>
-      <c r="N73" s="9" t="s">
-        <v>555</v>
-      </c>
-      <c r="O73" s="9" t="s">
-        <v>556</v>
       </c>
       <c r="P73" s="9" t="s">
         <v>491</v>
@@ -7983,146 +7983,146 @@
         <v>509</v>
       </c>
       <c r="R73" s="9" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="S73" s="9" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="T73" s="5" t="s">
         <v>11</v>
       </c>
       <c r="U73" s="9" t="s">
+        <v>557</v>
+      </c>
+      <c r="V73" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="W73" s="9" t="s">
         <v>559</v>
       </c>
-      <c r="V73" s="9" t="s">
+      <c r="X73" s="5" t="s">
         <v>560</v>
-      </c>
-      <c r="W73" s="9" t="s">
-        <v>561</v>
-      </c>
-      <c r="X73" s="5" t="s">
-        <v>562</v>
       </c>
       <c r="AB73" s="10" t="s">
         <v>421</v>
       </c>
       <c r="AC73" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD73" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS73" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="74" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="H74" s="9" t="s">
         <v>563</v>
       </c>
-      <c r="G74" s="9" t="s">
+      <c r="I74" s="9" t="s">
         <v>564</v>
       </c>
-      <c r="H74" s="9" t="s">
+      <c r="J74" s="9" t="s">
         <v>565</v>
-      </c>
-      <c r="I74" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="J74" s="9" t="s">
-        <v>567</v>
       </c>
       <c r="K74" s="5" t="s">
         <v>320</v>
       </c>
       <c r="L74" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="M74" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="N74" s="9" t="s">
         <v>568</v>
       </c>
-      <c r="M74" s="9" t="s">
+      <c r="O74" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="N74" s="9" t="s">
+      <c r="P74" s="9" t="s">
         <v>570</v>
       </c>
-      <c r="O74" s="9" t="s">
+      <c r="Q74" s="9" t="s">
         <v>571</v>
       </c>
-      <c r="P74" s="9" t="s">
+      <c r="R74" s="9" t="s">
         <v>572</v>
       </c>
-      <c r="Q74" s="9" t="s">
+      <c r="S74" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="T74" s="5" t="s">
         <v>573</v>
       </c>
-      <c r="R74" s="9" t="s">
+      <c r="U74" s="9" t="s">
         <v>574</v>
       </c>
-      <c r="S74" s="9" t="s">
-        <v>525</v>
-      </c>
-      <c r="T74" s="5" t="s">
+      <c r="V74" s="9" t="s">
         <v>575</v>
       </c>
-      <c r="U74" s="9" t="s">
+      <c r="W74" s="9" t="s">
         <v>576</v>
       </c>
-      <c r="V74" s="9" t="s">
+      <c r="X74" s="5" t="s">
         <v>577</v>
-      </c>
-      <c r="W74" s="9" t="s">
-        <v>578</v>
-      </c>
-      <c r="X74" s="5" t="s">
-        <v>579</v>
       </c>
       <c r="AB74" s="10" t="s">
         <v>511</v>
       </c>
       <c r="AC74" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD74" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS74" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="75" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B75" s="9" t="s">
         <v>145</v>
       </c>
       <c r="G75" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="H75" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="H75" s="5" t="s">
-        <v>517</v>
-      </c>
       <c r="I75" s="9" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J75" s="9" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="K75" s="9" t="s">
         <v>325</v>
       </c>
       <c r="L75" s="9" t="s">
+        <v>557</v>
+      </c>
+      <c r="M75" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="N75" s="9" t="s">
         <v>559</v>
-      </c>
-      <c r="M75" s="9" t="s">
-        <v>560</v>
-      </c>
-      <c r="N75" s="9" t="s">
-        <v>561</v>
       </c>
       <c r="O75" s="9" t="s">
         <v>497</v>
       </c>
       <c r="P75" s="9" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="Q75" s="9" t="s">
         <v>510</v>
@@ -8134,25 +8134,25 @@
         <v>499</v>
       </c>
       <c r="T75" s="9" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="U75" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="V75" s="9" t="s">
+        <v>587</v>
+      </c>
+      <c r="W75" s="9" t="s">
         <v>585</v>
       </c>
-      <c r="V75" s="9" t="s">
+      <c r="X75" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="Y75" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="W75" s="9" t="s">
-        <v>587</v>
-      </c>
-      <c r="X75" s="9" t="s">
+      <c r="Z75" s="5" t="s">
         <v>590</v>
-      </c>
-      <c r="Y75" s="9" t="s">
-        <v>591</v>
-      </c>
-      <c r="Z75" s="5" t="s">
-        <v>592</v>
       </c>
       <c r="AB75" s="9" t="s">
         <v>485</v>
@@ -8164,24 +8164,24 @@
         <v>487</v>
       </c>
       <c r="AE75" s="9" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="AF75" s="5" t="s">
         <v>11</v>
       </c>
       <c r="AG75" s="5" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="AH75" s="9" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="AI75" s="5" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="76" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B76" s="5">
         <v>7000</v>
@@ -8211,49 +8211,49 @@
         <v>359</v>
       </c>
       <c r="K76" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="L76" s="5" t="s">
+        <v>549</v>
+      </c>
+      <c r="M76" s="9" t="s">
         <v>550</v>
       </c>
-      <c r="L76" s="5" t="s">
+      <c r="N76" s="9" t="s">
         <v>551</v>
       </c>
-      <c r="M76" s="9" t="s">
-        <v>552</v>
-      </c>
-      <c r="N76" s="9" t="s">
-        <v>553</v>
-      </c>
       <c r="O76" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="P76" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="Q76" s="9" t="s">
         <v>594</v>
       </c>
-      <c r="P76" s="9" t="s">
+      <c r="R76" s="9" t="s">
         <v>595</v>
       </c>
-      <c r="Q76" s="9" t="s">
+      <c r="S76" s="9" t="s">
         <v>596</v>
-      </c>
-      <c r="R76" s="9" t="s">
-        <v>597</v>
-      </c>
-      <c r="S76" s="9" t="s">
-        <v>598</v>
       </c>
       <c r="T76" s="9" t="s">
         <v>510</v>
       </c>
       <c r="U76" s="9" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="V76" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="W76" s="9" t="s">
         <v>429</v>
       </c>
       <c r="X76" s="9" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="Y76" s="9" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="Z76" s="9" t="s">
         <v>319</v>
@@ -8265,10 +8265,10 @@
         <v>411</v>
       </c>
       <c r="AC76" s="10" t="s">
-        <v>412</v>
+        <v>700</v>
       </c>
       <c r="AD76" s="10" t="s">
-        <v>413</v>
+        <v>701</v>
       </c>
       <c r="AE76" s="9" t="s">
         <v>330</v>
@@ -8277,218 +8277,218 @@
         <v>332</v>
       </c>
       <c r="AG76" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="AH76" s="5" t="s">
+        <v>601</v>
+      </c>
+      <c r="AI76" s="5" t="s">
         <v>602</v>
-      </c>
-      <c r="AH76" s="5" t="s">
-        <v>603</v>
-      </c>
-      <c r="AI76" s="5" t="s">
-        <v>604</v>
       </c>
       <c r="AJ76" s="5" t="s">
         <v>175</v>
       </c>
       <c r="AK76" s="5" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="AL76" s="5" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="77" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="X77" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="Y77" s="5" t="s">
         <v>607</v>
       </c>
-      <c r="X77" s="9" t="s">
+      <c r="Z77" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="AA77" s="9" t="s">
         <v>608</v>
-      </c>
-      <c r="Y77" s="5" t="s">
-        <v>609</v>
-      </c>
-      <c r="Z77" s="9" t="s">
-        <v>611</v>
-      </c>
-      <c r="AA77" s="9" t="s">
-        <v>610</v>
       </c>
       <c r="AB77" s="10" t="s">
         <v>421</v>
       </c>
       <c r="AC77" s="10" t="s">
-        <v>422</v>
+        <v>700</v>
       </c>
       <c r="AD77" s="10" t="s">
-        <v>423</v>
+        <v>701</v>
       </c>
       <c r="AE77" s="9" t="s">
         <v>429</v>
       </c>
       <c r="AF77" s="9" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="AG77" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="AH77" s="5" t="s">
         <v>601</v>
       </c>
-      <c r="AH77" s="5" t="s">
-        <v>603</v>
-      </c>
       <c r="AI77" s="5" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="78" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B78" s="9" t="s">
         <v>142</v>
       </c>
       <c r="L78" s="9" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="M78" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="N78" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="O78" s="9" t="s">
         <v>565</v>
-      </c>
-      <c r="N78" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="O78" s="9" t="s">
-        <v>567</v>
       </c>
       <c r="P78" s="9" t="s">
         <v>510</v>
       </c>
       <c r="Q78" s="9" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="R78" s="5" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="S78" s="9" t="s">
+        <v>612</v>
+      </c>
+      <c r="T78" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="U78" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="V78" s="9" t="s">
         <v>614</v>
       </c>
-      <c r="T78" s="9" t="s">
+      <c r="W78" s="9" t="s">
+        <v>617</v>
+      </c>
+      <c r="X78" s="9" t="s">
+        <v>616</v>
+      </c>
+      <c r="Y78" s="9" t="s">
         <v>615</v>
-      </c>
-      <c r="U78" s="9" t="s">
-        <v>592</v>
-      </c>
-      <c r="V78" s="9" t="s">
-        <v>616</v>
-      </c>
-      <c r="W78" s="9" t="s">
-        <v>619</v>
-      </c>
-      <c r="X78" s="9" t="s">
-        <v>618</v>
-      </c>
-      <c r="Y78" s="9" t="s">
-        <v>617</v>
       </c>
       <c r="AB78" s="10" t="s">
         <v>511</v>
       </c>
       <c r="AC78" s="10" t="s">
-        <v>512</v>
+        <v>700</v>
       </c>
       <c r="AD78" s="10" t="s">
-        <v>513</v>
+        <v>701</v>
       </c>
     </row>
     <row r="79" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>144</v>
       </c>
       <c r="L79" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="M79" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="N79" s="9" t="s">
         <v>621</v>
       </c>
-      <c r="M79" s="9" t="s">
+      <c r="O79" s="9" t="s">
         <v>622</v>
-      </c>
-      <c r="N79" s="9" t="s">
-        <v>623</v>
-      </c>
-      <c r="O79" s="9" t="s">
-        <v>624</v>
       </c>
       <c r="P79" s="5" t="s">
         <v>11</v>
       </c>
       <c r="Q79" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="R79" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="S79" s="9" t="s">
+        <v>627</v>
+      </c>
+      <c r="T79" s="9" t="s">
+        <v>626</v>
+      </c>
+      <c r="U79" s="9" t="s">
         <v>625</v>
       </c>
-      <c r="R79" s="9" t="s">
-        <v>626</v>
-      </c>
-      <c r="S79" s="9" t="s">
-        <v>629</v>
-      </c>
-      <c r="T79" s="9" t="s">
-        <v>628</v>
-      </c>
-      <c r="U79" s="9" t="s">
-        <v>627</v>
-      </c>
       <c r="V79" s="9" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="W79" s="9" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="X79" s="5" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="AB79" s="9" t="s">
         <v>485</v>
       </c>
-      <c r="AC79" s="9" t="s">
-        <v>486</v>
-      </c>
-      <c r="AD79" s="9" t="s">
-        <v>487</v>
+      <c r="AC79" s="10" t="s">
+        <v>700</v>
+      </c>
+      <c r="AD79" s="10" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="80" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="L80" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="M80" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="N80" s="9" t="s">
         <v>535</v>
       </c>
-      <c r="M80" s="9" t="s">
+      <c r="O80" s="9" t="s">
         <v>536</v>
-      </c>
-      <c r="N80" s="9" t="s">
-        <v>537</v>
-      </c>
-      <c r="O80" s="9" t="s">
-        <v>538</v>
       </c>
       <c r="P80" s="9" t="s">
         <v>510</v>
       </c>
       <c r="Q80" s="9" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="R80" s="5" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="AB80" s="10" t="s">
         <v>411</v>
       </c>
       <c r="AC80" s="10" t="s">
-        <v>412</v>
+        <v>700</v>
       </c>
       <c r="AD80" s="10" t="s">
-        <v>413</v>
+        <v>701</v>
       </c>
     </row>
     <row r="81" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>459</v>
@@ -8515,13 +8515,13 @@
         <v>11</v>
       </c>
       <c r="J81" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="K81" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="L81" s="9" t="s">
         <v>632</v>
-      </c>
-      <c r="K81" s="9" t="s">
-        <v>633</v>
-      </c>
-      <c r="L81" s="9" t="s">
-        <v>634</v>
       </c>
       <c r="M81" s="5">
         <v>2356</v>
@@ -8530,63 +8530,63 @@
         <v>383</v>
       </c>
       <c r="O81" s="9" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="P81" s="5">
         <v>7000</v>
       </c>
       <c r="Q81" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="R81" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="S81" s="9" t="s">
         <v>636</v>
       </c>
-      <c r="R81" s="9" t="s">
+      <c r="T81" s="9" t="s">
         <v>637</v>
       </c>
-      <c r="S81" s="9" t="s">
+      <c r="U81" s="9" t="s">
         <v>638</v>
       </c>
-      <c r="T81" s="9" t="s">
+      <c r="V81" s="9" t="s">
         <v>639</v>
       </c>
-      <c r="U81" s="9" t="s">
+      <c r="W81" s="9" t="s">
         <v>640</v>
       </c>
-      <c r="V81" s="9" t="s">
-        <v>641</v>
-      </c>
-      <c r="W81" s="9" t="s">
+      <c r="X81" s="9" t="s">
         <v>642</v>
-      </c>
-      <c r="X81" s="9" t="s">
-        <v>644</v>
       </c>
       <c r="Y81" s="9" t="s">
         <v>500</v>
       </c>
       <c r="Z81" s="5" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="AB81" s="10" t="s">
         <v>421</v>
       </c>
       <c r="AC81" s="10" t="s">
-        <v>422</v>
+        <v>700</v>
       </c>
       <c r="AD81" s="10" t="s">
-        <v>423</v>
+        <v>701</v>
       </c>
       <c r="AE81" s="9" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="82" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B82" s="9" t="s">
         <v>143</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>462</v>
@@ -8601,69 +8601,69 @@
         <v>140</v>
       </c>
       <c r="L82" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="M82" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="N82" s="9" t="s">
         <v>636</v>
       </c>
-      <c r="M82" s="9" t="s">
+      <c r="O82" s="9" t="s">
         <v>637</v>
-      </c>
-      <c r="N82" s="9" t="s">
-        <v>638</v>
-      </c>
-      <c r="O82" s="9" t="s">
-        <v>639</v>
       </c>
       <c r="P82" s="5" t="s">
         <v>11</v>
       </c>
       <c r="Q82" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="R82" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="S82" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="T82" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="U82" s="9" t="s">
         <v>640</v>
       </c>
-      <c r="R82" s="9" t="s">
-        <v>633</v>
-      </c>
-      <c r="S82" s="9" t="s">
-        <v>634</v>
-      </c>
-      <c r="T82" s="9" t="s">
-        <v>641</v>
-      </c>
-      <c r="U82" s="9" t="s">
+      <c r="V82" s="9" t="s">
         <v>642</v>
-      </c>
-      <c r="V82" s="9" t="s">
-        <v>644</v>
       </c>
       <c r="W82" s="9" t="s">
         <v>500</v>
       </c>
       <c r="X82" s="5" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="AB82" s="10" t="s">
         <v>511</v>
       </c>
       <c r="AC82" s="10" t="s">
-        <v>512</v>
+        <v>700</v>
       </c>
       <c r="AD82" s="10" t="s">
-        <v>513</v>
+        <v>701</v>
       </c>
       <c r="AE82" s="9" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="83" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B83" s="9" t="s">
         <v>146</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>131</v>
@@ -8696,7 +8696,7 @@
         <v>116</v>
       </c>
       <c r="O83" s="9" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="P83" s="5">
         <v>2000</v>
@@ -8711,39 +8711,39 @@
         <v>6000</v>
       </c>
       <c r="T83" s="9" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="U83" s="9" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="V83" s="9" t="s">
         <v>128</v>
       </c>
       <c r="W83" s="9" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="X83" s="9" t="s">
         <v>510</v>
       </c>
       <c r="Y83" s="9" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="Z83" s="5" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="AB83" s="9" t="s">
         <v>485</v>
       </c>
-      <c r="AC83" s="9" t="s">
-        <v>486</v>
-      </c>
-      <c r="AD83" s="9" t="s">
-        <v>487</v>
+      <c r="AC83" s="10" t="s">
+        <v>700</v>
+      </c>
+      <c r="AD83" s="10" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="84" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="G84" s="5">
         <v>1000</v>
@@ -8752,15 +8752,15 @@
         <v>411</v>
       </c>
       <c r="AC84" s="10" t="s">
-        <v>412</v>
+        <v>700</v>
       </c>
       <c r="AD84" s="10" t="s">
-        <v>413</v>
+        <v>701</v>
       </c>
     </row>
     <row r="85" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="G85" s="5">
         <v>21000</v>
@@ -8772,15 +8772,15 @@
         <v>421</v>
       </c>
       <c r="AC85" s="10" t="s">
-        <v>422</v>
+        <v>700</v>
       </c>
       <c r="AD85" s="10" t="s">
-        <v>423</v>
+        <v>701</v>
       </c>
     </row>
     <row r="86" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="G86" s="5">
         <v>7000</v>
@@ -8789,15 +8789,15 @@
         <v>511</v>
       </c>
       <c r="AC86" s="10" t="s">
-        <v>512</v>
+        <v>700</v>
       </c>
       <c r="AD86" s="10" t="s">
-        <v>513</v>
+        <v>701</v>
       </c>
     </row>
     <row r="87" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="G87" s="5">
         <v>10</v>
@@ -8806,58 +8806,58 @@
         <v>225</v>
       </c>
       <c r="I87" s="9" t="s">
+        <v>658</v>
+      </c>
+      <c r="J87" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="K87" s="9" t="s">
         <v>660</v>
       </c>
-      <c r="J87" s="9" t="s">
-        <v>661</v>
-      </c>
-      <c r="K87" s="9" t="s">
+      <c r="L87" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="L87" s="9" t="s">
+      <c r="M87" s="9" t="s">
+        <v>663</v>
+      </c>
+      <c r="N87" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="M87" s="9" t="s">
+      <c r="O87" s="9" t="s">
         <v>665</v>
       </c>
-      <c r="N87" s="9" t="s">
+      <c r="P87" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="O87" s="9" t="s">
+      <c r="Q87" s="9" t="s">
         <v>667</v>
       </c>
-      <c r="P87" s="9" t="s">
+      <c r="R87" s="9" t="s">
         <v>668</v>
       </c>
-      <c r="Q87" s="9" t="s">
+      <c r="S87" s="9" t="s">
         <v>669</v>
       </c>
-      <c r="R87" s="9" t="s">
+      <c r="T87" s="9" t="s">
         <v>670</v>
       </c>
-      <c r="S87" s="9" t="s">
+      <c r="U87" s="9" t="s">
         <v>671</v>
       </c>
-      <c r="T87" s="9" t="s">
+      <c r="V87" s="9" t="s">
         <v>672</v>
       </c>
-      <c r="U87" s="9" t="s">
+      <c r="W87" s="9" t="s">
         <v>673</v>
       </c>
-      <c r="V87" s="9" t="s">
-        <v>674</v>
-      </c>
-      <c r="W87" s="9" t="s">
+      <c r="X87" s="9" t="s">
         <v>675</v>
-      </c>
-      <c r="X87" s="9" t="s">
-        <v>677</v>
       </c>
       <c r="Y87" s="9" t="s">
         <v>115</v>
       </c>
       <c r="Z87" s="9" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="AB87" s="9" t="s">
         <v>485</v>
@@ -8869,15 +8869,15 @@
         <v>487</v>
       </c>
       <c r="AE87" s="9" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="AF87" s="9" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="88" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>41</v>
@@ -8926,29 +8926,29 @@
         <v>464</v>
       </c>
       <c r="AC88" s="10" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="AD88" s="10" t="s">
+        <v>693</v>
+      </c>
+      <c r="AS88" s="5" t="s">
         <v>695</v>
-      </c>
-      <c r="AS88" s="5" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="89" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="AC89" s="10" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="AD89" s="10" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="90" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>41</v>
@@ -8997,18 +8997,18 @@
         <v>464</v>
       </c>
       <c r="AC90" s="10" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="AD90" s="10" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="AS90" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="91" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>41</v>
@@ -9057,18 +9057,18 @@
         <v>464</v>
       </c>
       <c r="AC91" s="10" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="AD91" s="10" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="AS91" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="92" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>41</v>
@@ -9117,18 +9117,18 @@
         <v>464</v>
       </c>
       <c r="AC92" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD92" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS92" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="93" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>41</v>
@@ -9177,37 +9177,37 @@
         <v>464</v>
       </c>
       <c r="AC93" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD93" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AE93" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="AF93" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="AG93" s="9" t="s">
         <v>535</v>
       </c>
-      <c r="AF93" s="9" t="s">
+      <c r="AH93" s="9" t="s">
         <v>536</v>
       </c>
-      <c r="AG93" s="9" t="s">
+      <c r="AI93" s="9" t="s">
         <v>537</v>
       </c>
-      <c r="AH93" s="9" t="s">
+      <c r="AJ93" s="9" t="s">
         <v>538</v>
-      </c>
-      <c r="AI93" s="9" t="s">
-        <v>539</v>
-      </c>
-      <c r="AJ93" s="9" t="s">
-        <v>540</v>
       </c>
       <c r="AK93" s="9" t="s">
         <v>510</v>
       </c>
       <c r="AL93" s="9" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="AM93" s="5" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="AN93" s="9" t="s">
         <v>142</v>
@@ -9216,12 +9216,12 @@
         <v>277</v>
       </c>
       <c r="AS93" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="94" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>41</v>
@@ -9270,18 +9270,18 @@
         <v>464</v>
       </c>
       <c r="AC94" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD94" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS94" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="95" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>39</v>
@@ -9356,10 +9356,10 @@
         <v>411</v>
       </c>
       <c r="AC95" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD95" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AE95" s="9" t="s">
         <v>387</v>
@@ -9384,12 +9384,12 @@
       </c>
       <c r="AL95" s="14"/>
       <c r="AS95" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="96" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>41</v>
@@ -9438,18 +9438,18 @@
         <v>464</v>
       </c>
       <c r="AC96" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD96" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS96" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="97" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>41</v>
@@ -9498,18 +9498,18 @@
         <v>464</v>
       </c>
       <c r="AC97" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD97" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS97" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="98" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>52</v>
@@ -9554,18 +9554,18 @@
         <v>421</v>
       </c>
       <c r="AC98" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD98" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS98" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="99" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>52</v>
@@ -9610,18 +9610,18 @@
         <v>421</v>
       </c>
       <c r="AC99" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD99" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS99" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="100" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>52</v>
@@ -9666,18 +9666,18 @@
         <v>421</v>
       </c>
       <c r="AC100" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD100" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS100" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="101" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>41</v>
@@ -9726,18 +9726,18 @@
         <v>464</v>
       </c>
       <c r="AC101" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD101" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS101" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="102" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>52</v>
@@ -9782,24 +9782,24 @@
         <v>421</v>
       </c>
       <c r="AC102" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD102" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AS102" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="AT102" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="AU102" s="15" t="s">
         <v>713</v>
-      </c>
-      <c r="AU102" s="15" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="103" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>39</v>
@@ -9874,10 +9874,10 @@
         <v>411</v>
       </c>
       <c r="AC103" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD103" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AE103" s="9" t="s">
         <v>387</v>
@@ -9902,12 +9902,12 @@
       </c>
       <c r="AL103" s="14"/>
       <c r="AS103" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="104" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>39</v>
@@ -9982,10 +9982,10 @@
         <v>411</v>
       </c>
       <c r="AC104" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD104" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AE104" s="9" t="s">
         <v>387</v>
@@ -10010,12 +10010,12 @@
       </c>
       <c r="AL104" s="14"/>
       <c r="AS104" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="105" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>39</v>
@@ -10090,10 +10090,10 @@
         <v>411</v>
       </c>
       <c r="AC105" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="AD105" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AE105" s="9" t="s">
         <v>387</v>
@@ -10118,7 +10118,7 @@
       </c>
       <c r="AL105" s="14"/>
       <c r="AS105" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -10131,8 +10131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7A3FC5-D09A-4697-BB1A-908D46717259}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10150,29 +10150,29 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>685</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>689</v>
-      </c>
       <c r="C2" s="13" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
   </sheetData>
@@ -10196,7 +10196,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>